<commit_message>
added new sheet for all libraries
</commit_message>
<xml_diff>
--- a/Library_architecture.xlsx
+++ b/Library_architecture.xlsx
@@ -5,18 +5,19 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ssipvtltd-my.sharepoint.com/personal/abhinay_singh_ssinnovations_org/Documents/Abhinay's Workspace/Libraries/Library/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ssipvtltd-my.sharepoint.com/personal/abhinay_singh_ssinnovations_org/Documents/Abhinay's Workspace/main x/GitHub Repo/Repository_architecture/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="198" documentId="11_F25DC773A252ABDACC104854799F7F145BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{41B719EB-F0E5-4BA4-A2DC-508FE3041CD7}"/>
+  <xr:revisionPtr revIDLastSave="337" documentId="11_F25DC773A252ABDACC104854799F7F145BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7821A3E0-929B-433A-8410-00C47BC414F2}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Control" sheetId="1" r:id="rId1"/>
-    <sheet name="Filter" sheetId="3" r:id="rId2"/>
-    <sheet name="Math" sheetId="2" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
+    <sheet name="Control system" sheetId="5" r:id="rId2"/>
+    <sheet name="Filter" sheetId="3" r:id="rId3"/>
+    <sheet name="Math" sheetId="2" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="92">
   <si>
     <t>Control_sys</t>
   </si>
@@ -196,13 +197,121 @@
   </si>
   <si>
     <t>Linear algebra</t>
+  </si>
+  <si>
+    <t>D + LPF_1</t>
+  </si>
+  <si>
+    <t>PD + LPF_1</t>
+  </si>
+  <si>
+    <t>PID + LPF_1</t>
+  </si>
+  <si>
+    <t>Sr. No.</t>
+  </si>
+  <si>
+    <t>Controller</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>C++</t>
+  </si>
+  <si>
+    <t>Python</t>
+  </si>
+  <si>
+    <t>Filter</t>
+  </si>
+  <si>
+    <t>LPF_1</t>
+  </si>
+  <si>
+    <t>LPF_2</t>
+  </si>
+  <si>
+    <t>HPF_1</t>
+  </si>
+  <si>
+    <t>HPF_2</t>
+  </si>
+  <si>
+    <t>BSF</t>
+  </si>
+  <si>
+    <t>BPF</t>
+  </si>
+  <si>
+    <t>HNF</t>
+  </si>
+  <si>
+    <t>SRF</t>
+  </si>
+  <si>
+    <t>QF_1</t>
+  </si>
+  <si>
+    <t>QF_2</t>
+  </si>
+  <si>
+    <t>Not Started</t>
+  </si>
+  <si>
+    <t>Complete</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>MA</t>
+  </si>
+  <si>
+    <t>Median</t>
+  </si>
+  <si>
+    <t>System Identification</t>
+  </si>
+  <si>
+    <t>First order</t>
+  </si>
+  <si>
+    <t>First order with dead time</t>
+  </si>
+  <si>
+    <t>Second order</t>
+  </si>
+  <si>
+    <t>Second order with dead time</t>
+  </si>
+  <si>
+    <t>Nth order</t>
+  </si>
+  <si>
+    <t>Nth order with dead time</t>
+  </si>
+  <si>
+    <t>System type</t>
+  </si>
+  <si>
+    <t>SISO</t>
+  </si>
+  <si>
+    <t>MISO</t>
+  </si>
+  <si>
+    <t>SIMO</t>
+  </si>
+  <si>
+    <t>MIMO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -225,8 +334,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -238,8 +369,30 @@
         <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -262,12 +415,368 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -275,18 +784,141 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -568,7 +1200,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -580,10 +1212,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="26" t="s">
         <v>8</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -592,16 +1224,16 @@
       <c r="D1" s="1"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
+      <c r="A2" s="26"/>
+      <c r="B2" s="26"/>
       <c r="C2" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3" t="s">
+      <c r="A3" s="26"/>
+      <c r="B3" s="26" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -610,19 +1242,19 @@
       <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
+      <c r="A4" s="26"/>
+      <c r="B4" s="26"/>
       <c r="C4" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3" t="s">
+      <c r="A5" s="26"/>
+      <c r="B5" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="26" t="s">
         <v>2</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -630,17 +1262,17 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
+      <c r="A6" s="26"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="26"/>
       <c r="D6" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3" t="s">
+      <c r="A7" s="26"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="26" t="s">
         <v>3</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -648,16 +1280,16 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
+      <c r="A8" s="26"/>
+      <c r="B8" s="26"/>
+      <c r="C8" s="26"/>
       <c r="D8" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3" t="s">
+      <c r="A9" s="26"/>
+      <c r="B9" s="26" t="s">
         <v>4</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -666,19 +1298,19 @@
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
+      <c r="A10" s="26"/>
+      <c r="B10" s="26"/>
       <c r="C10" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3" t="s">
+      <c r="A11" s="26"/>
+      <c r="B11" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="26" t="s">
         <v>5</v>
       </c>
       <c r="D11" s="1" t="s">
@@ -686,17 +1318,17 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
+      <c r="A12" s="26"/>
+      <c r="B12" s="26"/>
+      <c r="C12" s="26"/>
       <c r="D12" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3" t="s">
+      <c r="A13" s="26"/>
+      <c r="B13" s="26"/>
+      <c r="C13" s="26" t="s">
         <v>7</v>
       </c>
       <c r="D13" s="1" t="s">
@@ -704,19 +1336,19 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
+      <c r="A14" s="26"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="26"/>
       <c r="D14" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3" t="s">
+      <c r="A15" s="26"/>
+      <c r="B15" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="26" t="s">
         <v>6</v>
       </c>
       <c r="D15" s="1" t="s">
@@ -724,17 +1356,17 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
+      <c r="A16" s="26"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="26"/>
       <c r="D16" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3" t="s">
+      <c r="A17" s="26"/>
+      <c r="B17" s="26"/>
+      <c r="C17" s="26" t="s">
         <v>25</v>
       </c>
       <c r="D17" s="1" t="s">
@@ -742,9 +1374,9 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
+      <c r="A18" s="26"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="26"/>
       <c r="D18" s="1" t="s">
         <v>27</v>
       </c>
@@ -770,6 +1402,388 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FF893F8-BCFD-488B-AF9B-0D36D68641BC}">
+  <dimension ref="A1:R18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="27.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="I1" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="J1" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="K1" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="M1" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="N1" s="44" t="s">
+        <v>87</v>
+      </c>
+      <c r="O1" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="P1" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q1" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="R1" s="15" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" s="10">
+        <v>1</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="17"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="12"/>
+      <c r="G2" s="10">
+        <v>1</v>
+      </c>
+      <c r="H2" s="37" t="s">
+        <v>65</v>
+      </c>
+      <c r="I2" s="17"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="12"/>
+      <c r="M2" s="40">
+        <v>1</v>
+      </c>
+      <c r="N2" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="O2" s="43" t="s">
+        <v>81</v>
+      </c>
+      <c r="P2" s="42"/>
+      <c r="Q2" s="41"/>
+      <c r="R2" s="23"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>2</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="18"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="6"/>
+      <c r="G3" s="5">
+        <v>2</v>
+      </c>
+      <c r="H3" s="38" t="s">
+        <v>66</v>
+      </c>
+      <c r="I3" s="18"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="6"/>
+      <c r="M3" s="5">
+        <v>2</v>
+      </c>
+      <c r="N3" s="46"/>
+      <c r="O3" s="38" t="s">
+        <v>82</v>
+      </c>
+      <c r="P3" s="18"/>
+      <c r="Q3" s="4"/>
+      <c r="R3" s="6"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
+        <v>3</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="18"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="6"/>
+      <c r="G4" s="5">
+        <v>3</v>
+      </c>
+      <c r="H4" s="38" t="s">
+        <v>67</v>
+      </c>
+      <c r="I4" s="18"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="6"/>
+      <c r="M4" s="5">
+        <v>3</v>
+      </c>
+      <c r="N4" s="46"/>
+      <c r="O4" s="38" t="s">
+        <v>83</v>
+      </c>
+      <c r="P4" s="18"/>
+      <c r="Q4" s="4"/>
+      <c r="R4" s="6"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" s="18"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="6"/>
+      <c r="G5" s="5">
+        <v>4</v>
+      </c>
+      <c r="H5" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="I5" s="18"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="6"/>
+      <c r="M5" s="5">
+        <v>4</v>
+      </c>
+      <c r="N5" s="46"/>
+      <c r="O5" s="38" t="s">
+        <v>84</v>
+      </c>
+      <c r="P5" s="18"/>
+      <c r="Q5" s="4"/>
+      <c r="R5" s="6"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
+        <v>5</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="18"/>
+      <c r="D6" s="36"/>
+      <c r="E6" s="6"/>
+      <c r="G6" s="5">
+        <v>5</v>
+      </c>
+      <c r="H6" s="38" t="s">
+        <v>70</v>
+      </c>
+      <c r="I6" s="18"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="6"/>
+      <c r="M6" s="5">
+        <v>5</v>
+      </c>
+      <c r="N6" s="46"/>
+      <c r="O6" s="38" t="s">
+        <v>85</v>
+      </c>
+      <c r="P6" s="18"/>
+      <c r="Q6" s="4"/>
+      <c r="R6" s="6"/>
+    </row>
+    <row r="7" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="5">
+        <v>6</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="18"/>
+      <c r="D7" s="36"/>
+      <c r="E7" s="6"/>
+      <c r="G7" s="5">
+        <v>6</v>
+      </c>
+      <c r="H7" s="38" t="s">
+        <v>69</v>
+      </c>
+      <c r="I7" s="18"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="6"/>
+      <c r="M7" s="7">
+        <v>6</v>
+      </c>
+      <c r="N7" s="47"/>
+      <c r="O7" s="39" t="s">
+        <v>86</v>
+      </c>
+      <c r="P7" s="19"/>
+      <c r="Q7" s="8"/>
+      <c r="R7" s="9"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
+        <v>7</v>
+      </c>
+      <c r="B8" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8" s="18"/>
+      <c r="D8" s="36"/>
+      <c r="E8" s="6"/>
+      <c r="G8" s="5">
+        <v>7</v>
+      </c>
+      <c r="H8" s="38" t="s">
+        <v>71</v>
+      </c>
+      <c r="I8" s="18"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="6"/>
+      <c r="N8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <v>8</v>
+      </c>
+      <c r="B9" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="18"/>
+      <c r="D9" s="48"/>
+      <c r="E9" s="6"/>
+      <c r="G9" s="5">
+        <v>8</v>
+      </c>
+      <c r="H9" s="38" t="s">
+        <v>72</v>
+      </c>
+      <c r="I9" s="18"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="6"/>
+      <c r="N9" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="7">
+        <v>9</v>
+      </c>
+      <c r="B10" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" s="19"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="9"/>
+      <c r="G10" s="5">
+        <v>9</v>
+      </c>
+      <c r="H10" s="38" t="s">
+        <v>73</v>
+      </c>
+      <c r="I10" s="18"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="6"/>
+      <c r="N10" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="G11" s="5">
+        <v>10</v>
+      </c>
+      <c r="H11" s="38" t="s">
+        <v>74</v>
+      </c>
+      <c r="I11" s="18"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="6"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="G12" s="5">
+        <v>12</v>
+      </c>
+      <c r="H12" s="38" t="s">
+        <v>78</v>
+      </c>
+      <c r="I12" s="18"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="6"/>
+    </row>
+    <row r="13" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G13" s="7">
+        <v>13</v>
+      </c>
+      <c r="H13" s="39" t="s">
+        <v>79</v>
+      </c>
+      <c r="I13" s="19"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="9"/>
+    </row>
+    <row r="15" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B16" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="C16" s="28"/>
+      <c r="D16" s="23"/>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="C17" s="30"/>
+      <c r="D17" s="24"/>
+    </row>
+    <row r="18" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="C18" s="32"/>
+      <c r="D18" s="25"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="N2:N7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFD97391-339B-4313-8D6D-883D8A38F360}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -783,7 +1797,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FB061AE-55A5-4E7E-B1FB-948ACE22BB91}">
   <dimension ref="A1:L26"/>
   <sheetViews>
@@ -798,7 +1812,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="33" t="s">
         <v>55</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -807,7 +1821,7 @@
       <c r="C1" s="1"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
+      <c r="A2" s="33"/>
       <c r="B2" s="2" t="s">
         <v>34</v>
       </c>
@@ -835,113 +1849,113 @@
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="33" t="s">
         <v>29</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>38</v>
       </c>
       <c r="C6" s="1"/>
-      <c r="K6" s="5" t="s">
+      <c r="K6" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="L6" s="5"/>
+      <c r="L6" s="34"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
+      <c r="A7" s="33"/>
       <c r="B7" s="2" t="s">
         <v>39</v>
       </c>
       <c r="C7" s="1"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
+      <c r="K7" s="34"/>
+      <c r="L7" s="34"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
+      <c r="A8" s="33"/>
       <c r="B8" s="2" t="s">
         <v>41</v>
       </c>
       <c r="C8" s="1"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
+      <c r="A9" s="33"/>
       <c r="B9" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C9" s="1"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
+      <c r="A10" s="33"/>
       <c r="B10" s="2" t="s">
         <v>43</v>
       </c>
       <c r="C10" s="1"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
+      <c r="A11" s="33"/>
       <c r="B11" s="2" t="s">
         <v>40</v>
       </c>
       <c r="C11" s="1"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
+      <c r="A12" s="33"/>
       <c r="B12" s="2" t="s">
         <v>44</v>
       </c>
       <c r="C12" s="1"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
+      <c r="A13" s="33"/>
       <c r="B13" s="2" t="s">
         <v>45</v>
       </c>
       <c r="C13" s="1"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
+      <c r="A14" s="33"/>
       <c r="B14" s="2" t="s">
         <v>46</v>
       </c>
       <c r="C14" s="1"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
+      <c r="A15" s="33"/>
       <c r="B15" s="2" t="s">
         <v>47</v>
       </c>
       <c r="C15" s="1"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
+      <c r="A16" s="33"/>
       <c r="B16" s="2" t="s">
         <v>48</v>
       </c>
       <c r="C16" s="1"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
+      <c r="A17" s="33"/>
       <c r="B17" s="2" t="s">
         <v>49</v>
       </c>
       <c r="C17" s="1"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
+      <c r="A18" s="33"/>
       <c r="B18" s="2" t="s">
         <v>50</v>
       </c>
       <c r="C18" s="1"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
+      <c r="A19" s="33"/>
       <c r="B19" s="2" t="s">
         <v>51</v>
       </c>
       <c r="C19" s="1"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="4"/>
+      <c r="A20" s="33"/>
       <c r="B20" s="2" t="s">
         <v>52</v>
       </c>
@@ -955,7 +1969,7 @@
       <c r="C21" s="1"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="33" t="s">
         <v>31</v>
       </c>
       <c r="B22" s="2" t="s">
@@ -966,7 +1980,7 @@
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="4"/>
+      <c r="A23" s="33"/>
       <c r="B23" s="2" t="s">
         <v>36</v>
       </c>
@@ -999,11 +2013,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1683BD35-68D1-40C8-810D-7B22B62F74CE}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>

<commit_message>
added feed forward control
</commit_message>
<xml_diff>
--- a/Library_architecture.xlsx
+++ b/Library_architecture.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ssipvtltd-my.sharepoint.com/personal/abhinay_singh_ssinnovations_org/Documents/Abhinay's Workspace/main x/GitHub Repo/Repository_architecture/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="352" documentId="11_F25DC773A252ABDACC104854799F7F145BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{26432A7C-9C29-47B9-BD52-856B66A05976}"/>
+  <xr:revisionPtr revIDLastSave="366" documentId="11_F25DC773A252ABDACC104854799F7F145BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{50627FDA-DEDC-4DE7-83CC-81079429B3DA}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="98">
   <si>
     <t>Control_sys</t>
   </si>
@@ -320,6 +320,9 @@
   </si>
   <si>
     <t>Lag (cross correlation)</t>
+  </si>
+  <si>
+    <t>PID + LPF_1 + FF</t>
   </si>
 </sst>
 </file>
@@ -407,7 +410,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="28">
+  <borders count="31">
     <border>
       <left/>
       <right/>
@@ -782,6 +785,43 @@
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -791,7 +831,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -848,7 +888,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
@@ -860,9 +899,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -929,6 +965,22 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -1227,10 +1279,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="35" t="s">
         <v>8</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -1239,16 +1291,16 @@
       <c r="D1" s="1"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="37"/>
-      <c r="B2" s="37"/>
+      <c r="A2" s="35"/>
+      <c r="B2" s="35"/>
       <c r="C2" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="37"/>
-      <c r="B3" s="37" t="s">
+      <c r="A3" s="35"/>
+      <c r="B3" s="35" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -1257,19 +1309,19 @@
       <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="37"/>
-      <c r="B4" s="37"/>
+      <c r="A4" s="35"/>
+      <c r="B4" s="35"/>
       <c r="C4" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="37"/>
-      <c r="B5" s="37" t="s">
+      <c r="A5" s="35"/>
+      <c r="B5" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="37" t="s">
+      <c r="C5" s="35" t="s">
         <v>2</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -1277,17 +1329,17 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="37"/>
-      <c r="B6" s="37"/>
-      <c r="C6" s="37"/>
+      <c r="A6" s="35"/>
+      <c r="B6" s="35"/>
+      <c r="C6" s="35"/>
       <c r="D6" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="37"/>
-      <c r="B7" s="37"/>
-      <c r="C7" s="37" t="s">
+      <c r="A7" s="35"/>
+      <c r="B7" s="35"/>
+      <c r="C7" s="35" t="s">
         <v>3</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -1295,16 +1347,16 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="37"/>
-      <c r="B8" s="37"/>
-      <c r="C8" s="37"/>
+      <c r="A8" s="35"/>
+      <c r="B8" s="35"/>
+      <c r="C8" s="35"/>
       <c r="D8" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="37"/>
-      <c r="B9" s="37" t="s">
+      <c r="A9" s="35"/>
+      <c r="B9" s="35" t="s">
         <v>4</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -1313,19 +1365,19 @@
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="37"/>
-      <c r="B10" s="37"/>
+      <c r="A10" s="35"/>
+      <c r="B10" s="35"/>
       <c r="C10" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="37"/>
-      <c r="B11" s="37" t="s">
+      <c r="A11" s="35"/>
+      <c r="B11" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="37" t="s">
+      <c r="C11" s="35" t="s">
         <v>5</v>
       </c>
       <c r="D11" s="1" t="s">
@@ -1333,17 +1385,17 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="37"/>
-      <c r="B12" s="37"/>
-      <c r="C12" s="37"/>
+      <c r="A12" s="35"/>
+      <c r="B12" s="35"/>
+      <c r="C12" s="35"/>
       <c r="D12" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="37"/>
-      <c r="B13" s="37"/>
-      <c r="C13" s="37" t="s">
+      <c r="A13" s="35"/>
+      <c r="B13" s="35"/>
+      <c r="C13" s="35" t="s">
         <v>7</v>
       </c>
       <c r="D13" s="1" t="s">
@@ -1351,19 +1403,19 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="37"/>
-      <c r="B14" s="37"/>
-      <c r="C14" s="37"/>
+      <c r="A14" s="35"/>
+      <c r="B14" s="35"/>
+      <c r="C14" s="35"/>
       <c r="D14" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="37"/>
-      <c r="B15" s="37" t="s">
+      <c r="A15" s="35"/>
+      <c r="B15" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="37" t="s">
+      <c r="C15" s="35" t="s">
         <v>6</v>
       </c>
       <c r="D15" s="1" t="s">
@@ -1371,17 +1423,17 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="37"/>
-      <c r="B16" s="37"/>
-      <c r="C16" s="37"/>
+      <c r="A16" s="35"/>
+      <c r="B16" s="35"/>
+      <c r="C16" s="35"/>
       <c r="D16" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="37"/>
-      <c r="B17" s="37"/>
-      <c r="C17" s="37" t="s">
+      <c r="A17" s="35"/>
+      <c r="B17" s="35"/>
+      <c r="C17" s="35" t="s">
         <v>25</v>
       </c>
       <c r="D17" s="1" t="s">
@@ -1389,9 +1441,9 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="37"/>
-      <c r="B18" s="37"/>
-      <c r="C18" s="37"/>
+      <c r="A18" s="35"/>
+      <c r="B18" s="35"/>
+      <c r="C18" s="35"/>
       <c r="D18" s="1" t="s">
         <v>27</v>
       </c>
@@ -1422,31 +1474,31 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="V5" sqref="V5"/>
+      <selection pane="bottomLeft" activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="27.140625" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="20.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="47" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="49" t="s">
         <v>60</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="51" t="s">
         <v>61</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="48" t="s">
         <v>62</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="49" t="s">
         <v>63</v>
       </c>
       <c r="G1" s="13" t="s">
@@ -1467,7 +1519,7 @@
       <c r="M1" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="N1" s="35" t="s">
+      <c r="N1" s="33" t="s">
         <v>87</v>
       </c>
       <c r="O1" s="15" t="s">
@@ -1499,40 +1551,40 @@
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A2" s="10">
+      <c r="A2" s="29">
         <v>1</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="12"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="22"/>
       <c r="G2" s="10">
         <v>1</v>
       </c>
-      <c r="H2" s="28" t="s">
+      <c r="H2" s="26" t="s">
         <v>65</v>
       </c>
       <c r="I2" s="17"/>
       <c r="J2" s="11"/>
       <c r="K2" s="12"/>
-      <c r="M2" s="31">
+      <c r="M2" s="29">
         <v>1</v>
       </c>
-      <c r="N2" s="44" t="s">
+      <c r="N2" s="42" t="s">
         <v>88</v>
       </c>
-      <c r="O2" s="34" t="s">
+      <c r="O2" s="32" t="s">
         <v>81</v>
       </c>
-      <c r="P2" s="33"/>
-      <c r="Q2" s="32"/>
-      <c r="R2" s="23"/>
+      <c r="P2" s="31"/>
+      <c r="Q2" s="30"/>
+      <c r="R2" s="22"/>
       <c r="T2" s="10">
         <v>1</v>
       </c>
-      <c r="U2" s="28" t="s">
+      <c r="U2" s="26" t="s">
         <v>93</v>
       </c>
       <c r="V2" s="17"/>
@@ -1543,16 +1595,16 @@
       <c r="A3" s="5">
         <v>2</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="20" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="18"/>
-      <c r="D3" s="27"/>
+      <c r="D3" s="25"/>
       <c r="E3" s="6"/>
       <c r="G3" s="5">
         <v>2</v>
       </c>
-      <c r="H3" s="29" t="s">
+      <c r="H3" s="27" t="s">
         <v>66</v>
       </c>
       <c r="I3" s="18"/>
@@ -1561,8 +1613,8 @@
       <c r="M3" s="5">
         <v>2</v>
       </c>
-      <c r="N3" s="45"/>
-      <c r="O3" s="29" t="s">
+      <c r="N3" s="43"/>
+      <c r="O3" s="27" t="s">
         <v>82</v>
       </c>
       <c r="P3" s="18"/>
@@ -1571,7 +1623,7 @@
       <c r="T3" s="5">
         <v>2</v>
       </c>
-      <c r="U3" s="29" t="s">
+      <c r="U3" s="27" t="s">
         <v>94</v>
       </c>
       <c r="V3" s="18"/>
@@ -1582,16 +1634,16 @@
       <c r="A4" s="5">
         <v>3</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="20" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="18"/>
-      <c r="D4" s="27"/>
+      <c r="D4" s="25"/>
       <c r="E4" s="6"/>
       <c r="G4" s="5">
         <v>3</v>
       </c>
-      <c r="H4" s="29" t="s">
+      <c r="H4" s="27" t="s">
         <v>67</v>
       </c>
       <c r="I4" s="18"/>
@@ -1600,8 +1652,8 @@
       <c r="M4" s="5">
         <v>3</v>
       </c>
-      <c r="N4" s="45"/>
-      <c r="O4" s="29" t="s">
+      <c r="N4" s="43"/>
+      <c r="O4" s="27" t="s">
         <v>83</v>
       </c>
       <c r="P4" s="18"/>
@@ -1610,7 +1662,7 @@
       <c r="T4" s="5">
         <v>3</v>
       </c>
-      <c r="U4" s="29" t="s">
+      <c r="U4" s="27" t="s">
         <v>95</v>
       </c>
       <c r="V4" s="18"/>
@@ -1621,16 +1673,16 @@
       <c r="A5" s="5">
         <v>4</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="20" t="s">
         <v>56</v>
       </c>
       <c r="C5" s="18"/>
-      <c r="D5" s="27"/>
+      <c r="D5" s="25"/>
       <c r="E5" s="6"/>
       <c r="G5" s="5">
         <v>4</v>
       </c>
-      <c r="H5" s="29" t="s">
+      <c r="H5" s="27" t="s">
         <v>68</v>
       </c>
       <c r="I5" s="18"/>
@@ -1639,8 +1691,8 @@
       <c r="M5" s="5">
         <v>4</v>
       </c>
-      <c r="N5" s="45"/>
-      <c r="O5" s="29" t="s">
+      <c r="N5" s="43"/>
+      <c r="O5" s="27" t="s">
         <v>84</v>
       </c>
       <c r="P5" s="18"/>
@@ -1649,7 +1701,7 @@
       <c r="T5" s="5">
         <v>4</v>
       </c>
-      <c r="U5" s="29" t="s">
+      <c r="U5" s="27" t="s">
         <v>96</v>
       </c>
       <c r="V5" s="18"/>
@@ -1660,16 +1712,16 @@
       <c r="A6" s="5">
         <v>5</v>
       </c>
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="20" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="18"/>
-      <c r="D6" s="27"/>
+      <c r="D6" s="25"/>
       <c r="E6" s="6"/>
       <c r="G6" s="5">
         <v>5</v>
       </c>
-      <c r="H6" s="29" t="s">
+      <c r="H6" s="27" t="s">
         <v>70</v>
       </c>
       <c r="I6" s="18"/>
@@ -1678,8 +1730,8 @@
       <c r="M6" s="5">
         <v>5</v>
       </c>
-      <c r="N6" s="45"/>
-      <c r="O6" s="29" t="s">
+      <c r="N6" s="43"/>
+      <c r="O6" s="27" t="s">
         <v>85</v>
       </c>
       <c r="P6" s="18"/>
@@ -1690,16 +1742,16 @@
       <c r="A7" s="5">
         <v>6</v>
       </c>
-      <c r="B7" s="21" t="s">
+      <c r="B7" s="20" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="18"/>
-      <c r="D7" s="27"/>
+      <c r="D7" s="25"/>
       <c r="E7" s="6"/>
       <c r="G7" s="5">
         <v>6</v>
       </c>
-      <c r="H7" s="29" t="s">
+      <c r="H7" s="27" t="s">
         <v>69</v>
       </c>
       <c r="I7" s="18"/>
@@ -1708,8 +1760,8 @@
       <c r="M7" s="7">
         <v>6</v>
       </c>
-      <c r="N7" s="46"/>
-      <c r="O7" s="30" t="s">
+      <c r="N7" s="44"/>
+      <c r="O7" s="28" t="s">
         <v>86</v>
       </c>
       <c r="P7" s="19"/>
@@ -1720,16 +1772,16 @@
       <c r="A8" s="5">
         <v>7</v>
       </c>
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="20" t="s">
         <v>57</v>
       </c>
       <c r="C8" s="18"/>
-      <c r="D8" s="27"/>
+      <c r="D8" s="25"/>
       <c r="E8" s="6"/>
       <c r="G8" s="5">
         <v>7</v>
       </c>
-      <c r="H8" s="29" t="s">
+      <c r="H8" s="27" t="s">
         <v>71</v>
       </c>
       <c r="I8" s="18"/>
@@ -1743,16 +1795,16 @@
       <c r="A9" s="5">
         <v>8</v>
       </c>
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="20" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="18"/>
-      <c r="D9" s="27"/>
+      <c r="D9" s="25"/>
       <c r="E9" s="6"/>
       <c r="G9" s="5">
         <v>8</v>
       </c>
-      <c r="H9" s="29" t="s">
+      <c r="H9" s="27" t="s">
         <v>72</v>
       </c>
       <c r="I9" s="18"/>
@@ -1762,20 +1814,20 @@
         <v>90</v>
       </c>
     </row>
-    <row r="10" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="7">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
         <v>9</v>
       </c>
-      <c r="B10" s="22" t="s">
+      <c r="B10" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="C10" s="19"/>
-      <c r="D10" s="36"/>
-      <c r="E10" s="9"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="6"/>
       <c r="G10" s="5">
         <v>9</v>
       </c>
-      <c r="H10" s="29" t="s">
+      <c r="H10" s="27" t="s">
         <v>73</v>
       </c>
       <c r="I10" s="18"/>
@@ -1785,11 +1837,20 @@
         <v>91</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="7">
+        <v>10</v>
+      </c>
+      <c r="B11" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="C11" s="19"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="9"/>
       <c r="G11" s="5">
         <v>10</v>
       </c>
-      <c r="H11" s="29" t="s">
+      <c r="H11" s="27" t="s">
         <v>74</v>
       </c>
       <c r="I11" s="18"/>
@@ -1800,7 +1861,7 @@
       <c r="G12" s="5">
         <v>12</v>
       </c>
-      <c r="H12" s="29" t="s">
+      <c r="H12" s="27" t="s">
         <v>78</v>
       </c>
       <c r="I12" s="18"/>
@@ -1811,7 +1872,7 @@
       <c r="G13" s="7">
         <v>13</v>
       </c>
-      <c r="H13" s="30" t="s">
+      <c r="H13" s="28" t="s">
         <v>79</v>
       </c>
       <c r="I13" s="19"/>
@@ -1820,25 +1881,25 @@
     </row>
     <row r="15" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="B16" s="38" t="s">
+      <c r="B16" s="36" t="s">
         <v>75</v>
       </c>
-      <c r="C16" s="39"/>
-      <c r="D16" s="23"/>
+      <c r="C16" s="37"/>
+      <c r="D16" s="22"/>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="40" t="s">
+      <c r="B17" s="38" t="s">
         <v>77</v>
       </c>
-      <c r="C17" s="41"/>
-      <c r="D17" s="24"/>
+      <c r="C17" s="39"/>
+      <c r="D17" s="23"/>
     </row>
     <row r="18" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="42" t="s">
+      <c r="B18" s="40" t="s">
         <v>76</v>
       </c>
-      <c r="C18" s="43"/>
-      <c r="D18" s="25"/>
+      <c r="C18" s="41"/>
+      <c r="D18" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1880,7 +1941,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="45" t="s">
         <v>55</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -1889,7 +1950,7 @@
       <c r="C1" s="1"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="47"/>
+      <c r="A2" s="45"/>
       <c r="B2" s="2" t="s">
         <v>34</v>
       </c>
@@ -1917,113 +1978,113 @@
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="47" t="s">
+      <c r="A6" s="45" t="s">
         <v>29</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>38</v>
       </c>
       <c r="C6" s="1"/>
-      <c r="K6" s="48" t="s">
+      <c r="K6" s="46" t="s">
         <v>54</v>
       </c>
-      <c r="L6" s="48"/>
+      <c r="L6" s="46"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="47"/>
+      <c r="A7" s="45"/>
       <c r="B7" s="2" t="s">
         <v>39</v>
       </c>
       <c r="C7" s="1"/>
-      <c r="K7" s="48"/>
-      <c r="L7" s="48"/>
+      <c r="K7" s="46"/>
+      <c r="L7" s="46"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="47"/>
+      <c r="A8" s="45"/>
       <c r="B8" s="2" t="s">
         <v>41</v>
       </c>
       <c r="C8" s="1"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="47"/>
+      <c r="A9" s="45"/>
       <c r="B9" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C9" s="1"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="47"/>
+      <c r="A10" s="45"/>
       <c r="B10" s="2" t="s">
         <v>43</v>
       </c>
       <c r="C10" s="1"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="47"/>
+      <c r="A11" s="45"/>
       <c r="B11" s="2" t="s">
         <v>40</v>
       </c>
       <c r="C11" s="1"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="47"/>
+      <c r="A12" s="45"/>
       <c r="B12" s="2" t="s">
         <v>44</v>
       </c>
       <c r="C12" s="1"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="47"/>
+      <c r="A13" s="45"/>
       <c r="B13" s="2" t="s">
         <v>45</v>
       </c>
       <c r="C13" s="1"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="47"/>
+      <c r="A14" s="45"/>
       <c r="B14" s="2" t="s">
         <v>46</v>
       </c>
       <c r="C14" s="1"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="47"/>
+      <c r="A15" s="45"/>
       <c r="B15" s="2" t="s">
         <v>47</v>
       </c>
       <c r="C15" s="1"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="47"/>
+      <c r="A16" s="45"/>
       <c r="B16" s="2" t="s">
         <v>48</v>
       </c>
       <c r="C16" s="1"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="47"/>
+      <c r="A17" s="45"/>
       <c r="B17" s="2" t="s">
         <v>49</v>
       </c>
       <c r="C17" s="1"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="47"/>
+      <c r="A18" s="45"/>
       <c r="B18" s="2" t="s">
         <v>50</v>
       </c>
       <c r="C18" s="1"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="47"/>
+      <c r="A19" s="45"/>
       <c r="B19" s="2" t="s">
         <v>51</v>
       </c>
       <c r="C19" s="1"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="47"/>
+      <c r="A20" s="45"/>
       <c r="B20" s="2" t="s">
         <v>52</v>
       </c>
@@ -2037,7 +2098,7 @@
       <c r="C21" s="1"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="47" t="s">
+      <c r="A22" s="45" t="s">
         <v>31</v>
       </c>
       <c r="B22" s="2" t="s">
@@ -2048,7 +2109,7 @@
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="47"/>
+      <c r="A23" s="45"/>
       <c r="B23" s="2" t="s">
         <v>36</v>
       </c>

</xml_diff>

<commit_message>
PID standard and parallel form added
</commit_message>
<xml_diff>
--- a/Library_architecture.xlsx
+++ b/Library_architecture.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ssipvtltd-my.sharepoint.com/personal/abhinay_singh_ssinnovations_org/Documents/Abhinay's Workspace/main x/GitHub Repo/Repository_architecture/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="366" documentId="11_F25DC773A252ABDACC104854799F7F145BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{50627FDA-DEDC-4DE7-83CC-81079429B3DA}"/>
+  <xr:revisionPtr revIDLastSave="398" documentId="11_F25DC773A252ABDACC104854799F7F145BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BCF06686-47B7-4D21-AC01-4BD7C4BE2BEF}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="103">
   <si>
     <t>Control_sys</t>
   </si>
@@ -323,13 +323,28 @@
   </si>
   <si>
     <t>PID + LPF_1 + FF</t>
+  </si>
+  <si>
+    <t>PID_S</t>
+  </si>
+  <si>
+    <t>PID_P</t>
+  </si>
+  <si>
+    <t>Parallel</t>
+  </si>
+  <si>
+    <t>Standard</t>
+  </si>
+  <si>
+    <t>Equation Type</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -374,6 +389,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -410,7 +431,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="31">
+  <borders count="34">
     <border>
       <left/>
       <right/>
@@ -822,6 +843,45 @@
         <color indexed="64"/>
       </top>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -831,7 +891,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -926,9 +986,22 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -965,22 +1038,15 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="32" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -1279,10 +1345,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="40" t="s">
         <v>8</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -1291,16 +1357,16 @@
       <c r="D1" s="1"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="35"/>
-      <c r="B2" s="35"/>
+      <c r="A2" s="40"/>
+      <c r="B2" s="40"/>
       <c r="C2" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="35"/>
-      <c r="B3" s="35" t="s">
+      <c r="A3" s="40"/>
+      <c r="B3" s="40" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -1309,19 +1375,19 @@
       <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="35"/>
-      <c r="B4" s="35"/>
+      <c r="A4" s="40"/>
+      <c r="B4" s="40"/>
       <c r="C4" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="35"/>
-      <c r="B5" s="35" t="s">
+      <c r="A5" s="40"/>
+      <c r="B5" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="35" t="s">
+      <c r="C5" s="40" t="s">
         <v>2</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -1329,17 +1395,17 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="35"/>
-      <c r="B6" s="35"/>
-      <c r="C6" s="35"/>
+      <c r="A6" s="40"/>
+      <c r="B6" s="40"/>
+      <c r="C6" s="40"/>
       <c r="D6" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="35"/>
-      <c r="B7" s="35"/>
-      <c r="C7" s="35" t="s">
+      <c r="A7" s="40"/>
+      <c r="B7" s="40"/>
+      <c r="C7" s="40" t="s">
         <v>3</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -1347,16 +1413,16 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="35"/>
-      <c r="B8" s="35"/>
-      <c r="C8" s="35"/>
+      <c r="A8" s="40"/>
+      <c r="B8" s="40"/>
+      <c r="C8" s="40"/>
       <c r="D8" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="35"/>
-      <c r="B9" s="35" t="s">
+      <c r="A9" s="40"/>
+      <c r="B9" s="40" t="s">
         <v>4</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -1365,19 +1431,19 @@
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="35"/>
-      <c r="B10" s="35"/>
+      <c r="A10" s="40"/>
+      <c r="B10" s="40"/>
       <c r="C10" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="35"/>
-      <c r="B11" s="35" t="s">
+      <c r="A11" s="40"/>
+      <c r="B11" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="35" t="s">
+      <c r="C11" s="40" t="s">
         <v>5</v>
       </c>
       <c r="D11" s="1" t="s">
@@ -1385,17 +1451,17 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="35"/>
-      <c r="B12" s="35"/>
-      <c r="C12" s="35"/>
+      <c r="A12" s="40"/>
+      <c r="B12" s="40"/>
+      <c r="C12" s="40"/>
       <c r="D12" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="35"/>
-      <c r="B13" s="35"/>
-      <c r="C13" s="35" t="s">
+      <c r="A13" s="40"/>
+      <c r="B13" s="40"/>
+      <c r="C13" s="40" t="s">
         <v>7</v>
       </c>
       <c r="D13" s="1" t="s">
@@ -1403,19 +1469,19 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="35"/>
-      <c r="B14" s="35"/>
-      <c r="C14" s="35"/>
+      <c r="A14" s="40"/>
+      <c r="B14" s="40"/>
+      <c r="C14" s="40"/>
       <c r="D14" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="35"/>
-      <c r="B15" s="35" t="s">
+      <c r="A15" s="40"/>
+      <c r="B15" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="35" t="s">
+      <c r="C15" s="40" t="s">
         <v>6</v>
       </c>
       <c r="D15" s="1" t="s">
@@ -1423,17 +1489,17 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="35"/>
-      <c r="B16" s="35"/>
-      <c r="C16" s="35"/>
+      <c r="A16" s="40"/>
+      <c r="B16" s="40"/>
+      <c r="C16" s="40"/>
       <c r="D16" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="35"/>
-      <c r="B17" s="35"/>
-      <c r="C17" s="35" t="s">
+      <c r="A17" s="40"/>
+      <c r="B17" s="40"/>
+      <c r="C17" s="40" t="s">
         <v>25</v>
       </c>
       <c r="D17" s="1" t="s">
@@ -1441,9 +1507,9 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="35"/>
-      <c r="B18" s="35"/>
-      <c r="C18" s="35"/>
+      <c r="A18" s="40"/>
+      <c r="B18" s="40"/>
+      <c r="C18" s="40"/>
       <c r="D18" s="1" t="s">
         <v>27</v>
       </c>
@@ -1470,128 +1536,135 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FF893F8-BCFD-488B-AF9B-0D36D68641BC}">
-  <dimension ref="A1:X18"/>
+  <dimension ref="A1:Y20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P20" sqref="P20"/>
+      <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="20.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="47" t="s">
+    <row r="1" spans="1:25" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="36" t="s">
         <v>60</v>
       </c>
-      <c r="C1" s="51" t="s">
+      <c r="C1" s="38" t="s">
         <v>61</v>
       </c>
-      <c r="D1" s="48" t="s">
+      <c r="D1" s="35" t="s">
         <v>62</v>
       </c>
-      <c r="E1" s="49" t="s">
+      <c r="E1" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="F1" s="54" t="s">
+        <v>102</v>
+      </c>
+      <c r="H1" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="I1" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="J1" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="K1" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="K1" s="15" t="s">
+      <c r="L1" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="M1" s="13" t="s">
+      <c r="N1" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="N1" s="33" t="s">
+      <c r="O1" s="33" t="s">
         <v>87</v>
       </c>
-      <c r="O1" s="15" t="s">
+      <c r="P1" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="P1" s="16" t="s">
+      <c r="Q1" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="Q1" s="14" t="s">
+      <c r="R1" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="R1" s="15" t="s">
+      <c r="S1" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="T1" s="13" t="s">
+      <c r="U1" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="U1" s="15" t="s">
+      <c r="V1" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="V1" s="16" t="s">
+      <c r="W1" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="W1" s="14" t="s">
+      <c r="X1" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="X1" s="15" t="s">
+      <c r="Y1" s="15" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="29">
         <v>1</v>
       </c>
-      <c r="B2" s="52" t="s">
+      <c r="B2" s="39" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="31"/>
-      <c r="D2" s="50"/>
+      <c r="D2" s="37"/>
       <c r="E2" s="22"/>
-      <c r="G2" s="10">
+      <c r="F2" s="52" t="s">
+        <v>100</v>
+      </c>
+      <c r="H2" s="10">
         <v>1</v>
       </c>
-      <c r="H2" s="26" t="s">
+      <c r="I2" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="I2" s="17"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="12"/>
-      <c r="M2" s="29">
+      <c r="J2" s="17"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="12"/>
+      <c r="N2" s="29">
         <v>1</v>
       </c>
-      <c r="N2" s="42" t="s">
+      <c r="O2" s="47" t="s">
         <v>88</v>
       </c>
-      <c r="O2" s="32" t="s">
+      <c r="P2" s="32" t="s">
         <v>81</v>
       </c>
-      <c r="P2" s="31"/>
-      <c r="Q2" s="30"/>
-      <c r="R2" s="22"/>
-      <c r="T2" s="10">
+      <c r="Q2" s="31"/>
+      <c r="R2" s="30"/>
+      <c r="S2" s="22"/>
+      <c r="U2" s="10">
         <v>1</v>
       </c>
-      <c r="U2" s="26" t="s">
+      <c r="V2" s="26" t="s">
         <v>93</v>
       </c>
-      <c r="V2" s="17"/>
-      <c r="W2" s="11"/>
-      <c r="X2" s="12"/>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="W2" s="17"/>
+      <c r="X2" s="11"/>
+      <c r="Y2" s="12"/>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -1601,36 +1674,39 @@
       <c r="C3" s="18"/>
       <c r="D3" s="25"/>
       <c r="E3" s="6"/>
-      <c r="G3" s="5">
+      <c r="F3" s="52" t="s">
+        <v>100</v>
+      </c>
+      <c r="H3" s="5">
         <v>2</v>
       </c>
-      <c r="H3" s="27" t="s">
+      <c r="I3" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="I3" s="18"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="6"/>
-      <c r="M3" s="5">
+      <c r="J3" s="18"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="6"/>
+      <c r="N3" s="5">
         <v>2</v>
       </c>
-      <c r="N3" s="43"/>
-      <c r="O3" s="27" t="s">
+      <c r="O3" s="48"/>
+      <c r="P3" s="27" t="s">
         <v>82</v>
       </c>
-      <c r="P3" s="18"/>
-      <c r="Q3" s="4"/>
-      <c r="R3" s="6"/>
-      <c r="T3" s="5">
+      <c r="Q3" s="18"/>
+      <c r="R3" s="4"/>
+      <c r="S3" s="6"/>
+      <c r="U3" s="5">
         <v>2</v>
       </c>
-      <c r="U3" s="27" t="s">
+      <c r="V3" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="V3" s="18"/>
-      <c r="W3" s="4"/>
-      <c r="X3" s="6"/>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="W3" s="18"/>
+      <c r="X3" s="4"/>
+      <c r="Y3" s="6"/>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -1640,36 +1716,39 @@
       <c r="C4" s="18"/>
       <c r="D4" s="25"/>
       <c r="E4" s="6"/>
-      <c r="G4" s="5">
+      <c r="F4" s="52" t="s">
+        <v>100</v>
+      </c>
+      <c r="H4" s="5">
         <v>3</v>
       </c>
-      <c r="H4" s="27" t="s">
+      <c r="I4" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="I4" s="18"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="6"/>
-      <c r="M4" s="5">
+      <c r="J4" s="18"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="6"/>
+      <c r="N4" s="5">
         <v>3</v>
       </c>
-      <c r="N4" s="43"/>
-      <c r="O4" s="27" t="s">
+      <c r="O4" s="48"/>
+      <c r="P4" s="27" t="s">
         <v>83</v>
       </c>
-      <c r="P4" s="18"/>
-      <c r="Q4" s="4"/>
-      <c r="R4" s="6"/>
-      <c r="T4" s="5">
+      <c r="Q4" s="18"/>
+      <c r="R4" s="4"/>
+      <c r="S4" s="6"/>
+      <c r="U4" s="5">
         <v>3</v>
       </c>
-      <c r="U4" s="27" t="s">
+      <c r="V4" s="27" t="s">
         <v>95</v>
       </c>
-      <c r="V4" s="18"/>
-      <c r="W4" s="4"/>
-      <c r="X4" s="6"/>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="W4" s="18"/>
+      <c r="X4" s="4"/>
+      <c r="Y4" s="6"/>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -1679,36 +1758,39 @@
       <c r="C5" s="18"/>
       <c r="D5" s="25"/>
       <c r="E5" s="6"/>
-      <c r="G5" s="5">
+      <c r="F5" s="52" t="s">
+        <v>100</v>
+      </c>
+      <c r="H5" s="5">
         <v>4</v>
       </c>
-      <c r="H5" s="27" t="s">
+      <c r="I5" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="I5" s="18"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="6"/>
-      <c r="M5" s="5">
+      <c r="J5" s="18"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="6"/>
+      <c r="N5" s="5">
         <v>4</v>
       </c>
-      <c r="N5" s="43"/>
-      <c r="O5" s="27" t="s">
+      <c r="O5" s="48"/>
+      <c r="P5" s="27" t="s">
         <v>84</v>
       </c>
-      <c r="P5" s="18"/>
-      <c r="Q5" s="4"/>
-      <c r="R5" s="6"/>
-      <c r="T5" s="5">
+      <c r="Q5" s="18"/>
+      <c r="R5" s="4"/>
+      <c r="S5" s="6"/>
+      <c r="U5" s="5">
         <v>4</v>
       </c>
-      <c r="U5" s="27" t="s">
+      <c r="V5" s="27" t="s">
         <v>96</v>
       </c>
-      <c r="V5" s="18"/>
-      <c r="W5" s="4"/>
-      <c r="X5" s="6"/>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="W5" s="18"/>
+      <c r="X5" s="4"/>
+      <c r="Y5" s="6"/>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -1718,27 +1800,30 @@
       <c r="C6" s="18"/>
       <c r="D6" s="25"/>
       <c r="E6" s="6"/>
-      <c r="G6" s="5">
+      <c r="F6" s="52" t="s">
+        <v>100</v>
+      </c>
+      <c r="H6" s="5">
         <v>5</v>
       </c>
-      <c r="H6" s="27" t="s">
+      <c r="I6" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="I6" s="18"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="6"/>
-      <c r="M6" s="5">
+      <c r="J6" s="18"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="6"/>
+      <c r="N6" s="5">
         <v>5</v>
       </c>
-      <c r="N6" s="43"/>
-      <c r="O6" s="27" t="s">
+      <c r="O6" s="48"/>
+      <c r="P6" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="P6" s="18"/>
-      <c r="Q6" s="4"/>
-      <c r="R6" s="6"/>
-    </row>
-    <row r="7" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q6" s="18"/>
+      <c r="R6" s="4"/>
+      <c r="S6" s="6"/>
+    </row>
+    <row r="7" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -1748,27 +1833,30 @@
       <c r="C7" s="18"/>
       <c r="D7" s="25"/>
       <c r="E7" s="6"/>
-      <c r="G7" s="5">
+      <c r="F7" s="52" t="s">
+        <v>100</v>
+      </c>
+      <c r="H7" s="5">
         <v>6</v>
       </c>
-      <c r="H7" s="27" t="s">
+      <c r="I7" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="I7" s="18"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="6"/>
-      <c r="M7" s="7">
+      <c r="J7" s="18"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="6"/>
+      <c r="N7" s="7">
         <v>6</v>
       </c>
-      <c r="N7" s="44"/>
-      <c r="O7" s="28" t="s">
+      <c r="O7" s="49"/>
+      <c r="P7" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="P7" s="19"/>
-      <c r="Q7" s="8"/>
-      <c r="R7" s="9"/>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Q7" s="19"/>
+      <c r="R7" s="8"/>
+      <c r="S7" s="9"/>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -1778,20 +1866,23 @@
       <c r="C8" s="18"/>
       <c r="D8" s="25"/>
       <c r="E8" s="6"/>
-      <c r="G8" s="5">
+      <c r="F8" s="52" t="s">
+        <v>100</v>
+      </c>
+      <c r="H8" s="5">
         <v>7</v>
       </c>
-      <c r="H8" s="27" t="s">
+      <c r="I8" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="I8" s="18"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="6"/>
-      <c r="N8" t="s">
+      <c r="J8" s="18"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="6"/>
+      <c r="O8" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -1801,20 +1892,23 @@
       <c r="C9" s="18"/>
       <c r="D9" s="25"/>
       <c r="E9" s="6"/>
-      <c r="G9" s="5">
+      <c r="F9" s="52" t="s">
+        <v>100</v>
+      </c>
+      <c r="H9" s="5">
         <v>8</v>
       </c>
-      <c r="H9" s="27" t="s">
+      <c r="I9" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="I9" s="18"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="6"/>
-      <c r="N9" t="s">
+      <c r="J9" s="18"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="6"/>
+      <c r="O9" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -1824,89 +1918,133 @@
       <c r="C10" s="18"/>
       <c r="D10" s="25"/>
       <c r="E10" s="6"/>
-      <c r="G10" s="5">
+      <c r="F10" s="52" t="s">
+        <v>100</v>
+      </c>
+      <c r="H10" s="5">
         <v>9</v>
       </c>
-      <c r="H10" s="27" t="s">
+      <c r="I10" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="I10" s="18"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="6"/>
-      <c r="N10" t="s">
+      <c r="J10" s="18"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="6"/>
+      <c r="O10" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="11" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="7">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
         <v>10</v>
       </c>
-      <c r="B11" s="21" t="s">
+      <c r="B11" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="C11" s="19"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="9"/>
-      <c r="G11" s="5">
+      <c r="C11" s="18"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="52" t="s">
+        <v>100</v>
+      </c>
+      <c r="H11" s="5"/>
+      <c r="I11" s="27"/>
+      <c r="J11" s="18"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="6"/>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
+        <v>11</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="52" t="s">
+        <v>100</v>
+      </c>
+      <c r="H12" s="5"/>
+      <c r="I12" s="27"/>
+      <c r="J12" s="18"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="6"/>
+    </row>
+    <row r="13" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="7">
+        <v>12</v>
+      </c>
+      <c r="B13" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="53" t="s">
+        <v>101</v>
+      </c>
+      <c r="H13" s="5">
         <v>10</v>
       </c>
-      <c r="H11" s="27" t="s">
+      <c r="I13" s="27" t="s">
         <v>74</v>
       </c>
-      <c r="I11" s="18"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="6"/>
-    </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="G12" s="5">
+      <c r="J13" s="18"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="6"/>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="H14" s="5">
         <v>12</v>
       </c>
-      <c r="H12" s="27" t="s">
+      <c r="I14" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="I12" s="18"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="6"/>
-    </row>
-    <row r="13" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G13" s="7">
+      <c r="J14" s="18"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="6"/>
+    </row>
+    <row r="15" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H15" s="7">
         <v>13</v>
       </c>
-      <c r="H13" s="28" t="s">
+      <c r="I15" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="I13" s="19"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="9"/>
-    </row>
-    <row r="15" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="B16" s="36" t="s">
+      <c r="J15" s="19"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="9"/>
+    </row>
+    <row r="17" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="41" t="s">
         <v>75</v>
       </c>
-      <c r="C16" s="37"/>
-      <c r="D16" s="22"/>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="38" t="s">
+      <c r="C18" s="42"/>
+      <c r="D18" s="22"/>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="43" t="s">
         <v>77</v>
       </c>
-      <c r="C17" s="39"/>
-      <c r="D17" s="23"/>
-    </row>
-    <row r="18" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="40" t="s">
+      <c r="C19" s="44"/>
+      <c r="D19" s="23"/>
+    </row>
+    <row r="20" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="45" t="s">
         <v>76</v>
       </c>
-      <c r="C18" s="41"/>
-      <c r="D18" s="24"/>
+      <c r="C20" s="46"/>
+      <c r="D20" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
     <mergeCell ref="B18:C18"/>
-    <mergeCell ref="N2:N7"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="O2:O7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1941,7 +2079,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="50" t="s">
         <v>55</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -1950,7 +2088,7 @@
       <c r="C1" s="1"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="45"/>
+      <c r="A2" s="50"/>
       <c r="B2" s="2" t="s">
         <v>34</v>
       </c>
@@ -1978,113 +2116,113 @@
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="45" t="s">
+      <c r="A6" s="50" t="s">
         <v>29</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>38</v>
       </c>
       <c r="C6" s="1"/>
-      <c r="K6" s="46" t="s">
+      <c r="K6" s="51" t="s">
         <v>54</v>
       </c>
-      <c r="L6" s="46"/>
+      <c r="L6" s="51"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="45"/>
+      <c r="A7" s="50"/>
       <c r="B7" s="2" t="s">
         <v>39</v>
       </c>
       <c r="C7" s="1"/>
-      <c r="K7" s="46"/>
-      <c r="L7" s="46"/>
+      <c r="K7" s="51"/>
+      <c r="L7" s="51"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="45"/>
+      <c r="A8" s="50"/>
       <c r="B8" s="2" t="s">
         <v>41</v>
       </c>
       <c r="C8" s="1"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="45"/>
+      <c r="A9" s="50"/>
       <c r="B9" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C9" s="1"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="45"/>
+      <c r="A10" s="50"/>
       <c r="B10" s="2" t="s">
         <v>43</v>
       </c>
       <c r="C10" s="1"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="45"/>
+      <c r="A11" s="50"/>
       <c r="B11" s="2" t="s">
         <v>40</v>
       </c>
       <c r="C11" s="1"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="45"/>
+      <c r="A12" s="50"/>
       <c r="B12" s="2" t="s">
         <v>44</v>
       </c>
       <c r="C12" s="1"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="45"/>
+      <c r="A13" s="50"/>
       <c r="B13" s="2" t="s">
         <v>45</v>
       </c>
       <c r="C13" s="1"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="45"/>
+      <c r="A14" s="50"/>
       <c r="B14" s="2" t="s">
         <v>46</v>
       </c>
       <c r="C14" s="1"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="45"/>
+      <c r="A15" s="50"/>
       <c r="B15" s="2" t="s">
         <v>47</v>
       </c>
       <c r="C15" s="1"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="45"/>
+      <c r="A16" s="50"/>
       <c r="B16" s="2" t="s">
         <v>48</v>
       </c>
       <c r="C16" s="1"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="45"/>
+      <c r="A17" s="50"/>
       <c r="B17" s="2" t="s">
         <v>49</v>
       </c>
       <c r="C17" s="1"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="45"/>
+      <c r="A18" s="50"/>
       <c r="B18" s="2" t="s">
         <v>50</v>
       </c>
       <c r="C18" s="1"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="45"/>
+      <c r="A19" s="50"/>
       <c r="B19" s="2" t="s">
         <v>51</v>
       </c>
       <c r="C19" s="1"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="45"/>
+      <c r="A20" s="50"/>
       <c r="B20" s="2" t="s">
         <v>52</v>
       </c>
@@ -2098,7 +2236,7 @@
       <c r="C21" s="1"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="45" t="s">
+      <c r="A22" s="50" t="s">
         <v>31</v>
       </c>
       <c r="B22" s="2" t="s">
@@ -2109,7 +2247,7 @@
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="45"/>
+      <c r="A23" s="50"/>
       <c r="B23" s="2" t="s">
         <v>36</v>
       </c>

</xml_diff>

<commit_message>
PID_P parallel pid complete
</commit_message>
<xml_diff>
--- a/Library_architecture.xlsx
+++ b/Library_architecture.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ssipvtltd-my.sharepoint.com/personal/abhinay_singh_ssinnovations_org/Documents/Abhinay's Workspace/main x/GitHub Repo/Repository_architecture/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="424" documentId="11_F25DC773A252ABDACC104854799F7F145BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{41A8F2D9-4417-42BA-B08D-51E4908E946A}"/>
+  <xr:revisionPtr revIDLastSave="426" documentId="11_F25DC773A252ABDACC104854799F7F145BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7A723073-8939-4829-ABF1-A738FE28E1DD}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -966,6 +966,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1001,18 +1013,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1312,10 +1312,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="44" t="s">
         <v>8</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -1324,16 +1324,16 @@
       <c r="D1" s="1"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="40"/>
-      <c r="B2" s="40"/>
+      <c r="A2" s="44"/>
+      <c r="B2" s="44"/>
       <c r="C2" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="40"/>
-      <c r="B3" s="40" t="s">
+      <c r="A3" s="44"/>
+      <c r="B3" s="44" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -1342,19 +1342,19 @@
       <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="40"/>
-      <c r="B4" s="40"/>
+      <c r="A4" s="44"/>
+      <c r="B4" s="44"/>
       <c r="C4" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="40"/>
-      <c r="B5" s="40" t="s">
+      <c r="A5" s="44"/>
+      <c r="B5" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="40" t="s">
+      <c r="C5" s="44" t="s">
         <v>2</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -1362,17 +1362,17 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="40"/>
-      <c r="B6" s="40"/>
-      <c r="C6" s="40"/>
+      <c r="A6" s="44"/>
+      <c r="B6" s="44"/>
+      <c r="C6" s="44"/>
       <c r="D6" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="40"/>
-      <c r="B7" s="40"/>
-      <c r="C7" s="40" t="s">
+      <c r="A7" s="44"/>
+      <c r="B7" s="44"/>
+      <c r="C7" s="44" t="s">
         <v>3</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -1380,16 +1380,16 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="40"/>
-      <c r="B8" s="40"/>
-      <c r="C8" s="40"/>
+      <c r="A8" s="44"/>
+      <c r="B8" s="44"/>
+      <c r="C8" s="44"/>
       <c r="D8" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="40"/>
-      <c r="B9" s="40" t="s">
+      <c r="A9" s="44"/>
+      <c r="B9" s="44" t="s">
         <v>4</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -1398,19 +1398,19 @@
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="40"/>
-      <c r="B10" s="40"/>
+      <c r="A10" s="44"/>
+      <c r="B10" s="44"/>
       <c r="C10" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="40"/>
-      <c r="B11" s="40" t="s">
+      <c r="A11" s="44"/>
+      <c r="B11" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="40" t="s">
+      <c r="C11" s="44" t="s">
         <v>5</v>
       </c>
       <c r="D11" s="1" t="s">
@@ -1418,17 +1418,17 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="40"/>
-      <c r="B12" s="40"/>
-      <c r="C12" s="40"/>
+      <c r="A12" s="44"/>
+      <c r="B12" s="44"/>
+      <c r="C12" s="44"/>
       <c r="D12" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="40"/>
-      <c r="B13" s="40"/>
-      <c r="C13" s="40" t="s">
+      <c r="A13" s="44"/>
+      <c r="B13" s="44"/>
+      <c r="C13" s="44" t="s">
         <v>7</v>
       </c>
       <c r="D13" s="1" t="s">
@@ -1436,19 +1436,19 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="40"/>
-      <c r="B14" s="40"/>
-      <c r="C14" s="40"/>
+      <c r="A14" s="44"/>
+      <c r="B14" s="44"/>
+      <c r="C14" s="44"/>
       <c r="D14" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="40"/>
-      <c r="B15" s="40" t="s">
+      <c r="A15" s="44"/>
+      <c r="B15" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="40" t="s">
+      <c r="C15" s="44" t="s">
         <v>6</v>
       </c>
       <c r="D15" s="1" t="s">
@@ -1456,17 +1456,17 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="40"/>
-      <c r="B16" s="40"/>
-      <c r="C16" s="40"/>
+      <c r="A16" s="44"/>
+      <c r="B16" s="44"/>
+      <c r="C16" s="44"/>
       <c r="D16" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="40"/>
-      <c r="B17" s="40"/>
-      <c r="C17" s="40" t="s">
+      <c r="A17" s="44"/>
+      <c r="B17" s="44"/>
+      <c r="C17" s="44" t="s">
         <v>25</v>
       </c>
       <c r="D17" s="1" t="s">
@@ -1474,9 +1474,9 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="40"/>
-      <c r="B18" s="40"/>
-      <c r="C18" s="40"/>
+      <c r="A18" s="44"/>
+      <c r="B18" s="44"/>
+      <c r="C18" s="44"/>
       <c r="D18" s="1" t="s">
         <v>27</v>
       </c>
@@ -1507,7 +1507,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P26" sqref="P26"/>
+      <selection pane="bottomLeft" activeCell="N28" sqref="N28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1597,7 +1597,7 @@
       <c r="C2" s="31"/>
       <c r="D2" s="37"/>
       <c r="E2" s="30"/>
-      <c r="F2" s="54" t="s">
+      <c r="F2" s="42" t="s">
         <v>100</v>
       </c>
       <c r="H2" s="10">
@@ -1612,7 +1612,7 @@
       <c r="N2" s="29">
         <v>1</v>
       </c>
-      <c r="O2" s="47" t="s">
+      <c r="O2" s="51" t="s">
         <v>88</v>
       </c>
       <c r="P2" s="32" t="s">
@@ -1641,7 +1641,7 @@
       <c r="C3" s="18"/>
       <c r="D3" s="25"/>
       <c r="E3" s="4"/>
-      <c r="F3" s="52" t="s">
+      <c r="F3" s="40" t="s">
         <v>100</v>
       </c>
       <c r="H3" s="5">
@@ -1656,7 +1656,7 @@
       <c r="N3" s="5">
         <v>2</v>
       </c>
-      <c r="O3" s="48"/>
+      <c r="O3" s="52"/>
       <c r="P3" s="27" t="s">
         <v>82</v>
       </c>
@@ -1683,7 +1683,7 @@
       <c r="C4" s="18"/>
       <c r="D4" s="25"/>
       <c r="E4" s="4"/>
-      <c r="F4" s="52" t="s">
+      <c r="F4" s="40" t="s">
         <v>100</v>
       </c>
       <c r="H4" s="5">
@@ -1698,7 +1698,7 @@
       <c r="N4" s="5">
         <v>3</v>
       </c>
-      <c r="O4" s="48"/>
+      <c r="O4" s="52"/>
       <c r="P4" s="27" t="s">
         <v>83</v>
       </c>
@@ -1725,7 +1725,7 @@
       <c r="C5" s="18"/>
       <c r="D5" s="25"/>
       <c r="E5" s="4"/>
-      <c r="F5" s="52" t="s">
+      <c r="F5" s="40" t="s">
         <v>100</v>
       </c>
       <c r="H5" s="5">
@@ -1740,7 +1740,7 @@
       <c r="N5" s="5">
         <v>4</v>
       </c>
-      <c r="O5" s="48"/>
+      <c r="O5" s="52"/>
       <c r="P5" s="27" t="s">
         <v>84</v>
       </c>
@@ -1767,7 +1767,7 @@
       <c r="C6" s="18"/>
       <c r="D6" s="25"/>
       <c r="E6" s="4"/>
-      <c r="F6" s="52" t="s">
+      <c r="F6" s="40" t="s">
         <v>100</v>
       </c>
       <c r="H6" s="5">
@@ -1782,7 +1782,7 @@
       <c r="N6" s="5">
         <v>5</v>
       </c>
-      <c r="O6" s="48"/>
+      <c r="O6" s="52"/>
       <c r="P6" s="27" t="s">
         <v>85</v>
       </c>
@@ -1800,7 +1800,7 @@
       <c r="C7" s="18"/>
       <c r="D7" s="25"/>
       <c r="E7" s="4"/>
-      <c r="F7" s="52" t="s">
+      <c r="F7" s="40" t="s">
         <v>100</v>
       </c>
       <c r="H7" s="5">
@@ -1815,7 +1815,7 @@
       <c r="N7" s="7">
         <v>6</v>
       </c>
-      <c r="O7" s="49"/>
+      <c r="O7" s="53"/>
       <c r="P7" s="28" t="s">
         <v>86</v>
       </c>
@@ -1833,7 +1833,7 @@
       <c r="C8" s="18"/>
       <c r="D8" s="25"/>
       <c r="E8" s="4"/>
-      <c r="F8" s="52" t="s">
+      <c r="F8" s="40" t="s">
         <v>100</v>
       </c>
       <c r="H8" s="5">
@@ -1859,7 +1859,7 @@
       <c r="C9" s="18"/>
       <c r="D9" s="25"/>
       <c r="E9" s="4"/>
-      <c r="F9" s="52" t="s">
+      <c r="F9" s="40" t="s">
         <v>100</v>
       </c>
       <c r="H9" s="5">
@@ -1885,7 +1885,7 @@
       <c r="C10" s="18"/>
       <c r="D10" s="25"/>
       <c r="E10" s="4"/>
-      <c r="F10" s="52" t="s">
+      <c r="F10" s="40" t="s">
         <v>100</v>
       </c>
       <c r="H10" s="5">
@@ -1911,7 +1911,7 @@
       <c r="C11" s="18"/>
       <c r="D11" s="25"/>
       <c r="E11" s="4"/>
-      <c r="F11" s="52" t="s">
+      <c r="F11" s="40" t="s">
         <v>100</v>
       </c>
       <c r="H11" s="5"/>
@@ -1928,9 +1928,9 @@
         <v>98</v>
       </c>
       <c r="C12" s="18"/>
-      <c r="D12" s="4"/>
+      <c r="D12" s="43"/>
       <c r="E12" s="4"/>
-      <c r="F12" s="52" t="s">
+      <c r="F12" s="40" t="s">
         <v>101</v>
       </c>
       <c r="H12" s="5"/>
@@ -1947,9 +1947,9 @@
         <v>99</v>
       </c>
       <c r="C13" s="18"/>
-      <c r="D13" s="55"/>
+      <c r="D13" s="25"/>
       <c r="E13" s="4"/>
-      <c r="F13" s="52" t="s">
+      <c r="F13" s="40" t="s">
         <v>100</v>
       </c>
       <c r="H13" s="5">
@@ -1972,7 +1972,7 @@
       <c r="C14" s="19"/>
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
-      <c r="F14" s="53" t="s">
+      <c r="F14" s="41" t="s">
         <v>100</v>
       </c>
       <c r="H14" s="5">
@@ -1998,24 +1998,24 @@
     </row>
     <row r="17" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="41" t="s">
+      <c r="B18" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="C18" s="42"/>
+      <c r="C18" s="46"/>
       <c r="D18" s="22"/>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="43" t="s">
+      <c r="B19" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="C19" s="44"/>
+      <c r="C19" s="48"/>
       <c r="D19" s="23"/>
     </row>
     <row r="20" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="45" t="s">
+      <c r="B20" s="49" t="s">
         <v>76</v>
       </c>
-      <c r="C20" s="46"/>
+      <c r="C20" s="50"/>
       <c r="D20" s="24"/>
     </row>
   </sheetData>
@@ -2058,7 +2058,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="54" t="s">
         <v>55</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -2067,7 +2067,7 @@
       <c r="C1" s="1"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="50"/>
+      <c r="A2" s="54"/>
       <c r="B2" s="2" t="s">
         <v>34</v>
       </c>
@@ -2095,113 +2095,113 @@
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="50" t="s">
+      <c r="A6" s="54" t="s">
         <v>29</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>38</v>
       </c>
       <c r="C6" s="1"/>
-      <c r="K6" s="51" t="s">
+      <c r="K6" s="55" t="s">
         <v>54</v>
       </c>
-      <c r="L6" s="51"/>
+      <c r="L6" s="55"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="50"/>
+      <c r="A7" s="54"/>
       <c r="B7" s="2" t="s">
         <v>39</v>
       </c>
       <c r="C7" s="1"/>
-      <c r="K7" s="51"/>
-      <c r="L7" s="51"/>
+      <c r="K7" s="55"/>
+      <c r="L7" s="55"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="50"/>
+      <c r="A8" s="54"/>
       <c r="B8" s="2" t="s">
         <v>41</v>
       </c>
       <c r="C8" s="1"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="50"/>
+      <c r="A9" s="54"/>
       <c r="B9" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C9" s="1"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="50"/>
+      <c r="A10" s="54"/>
       <c r="B10" s="2" t="s">
         <v>43</v>
       </c>
       <c r="C10" s="1"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="50"/>
+      <c r="A11" s="54"/>
       <c r="B11" s="2" t="s">
         <v>40</v>
       </c>
       <c r="C11" s="1"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="50"/>
+      <c r="A12" s="54"/>
       <c r="B12" s="2" t="s">
         <v>44</v>
       </c>
       <c r="C12" s="1"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="50"/>
+      <c r="A13" s="54"/>
       <c r="B13" s="2" t="s">
         <v>45</v>
       </c>
       <c r="C13" s="1"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="50"/>
+      <c r="A14" s="54"/>
       <c r="B14" s="2" t="s">
         <v>46</v>
       </c>
       <c r="C14" s="1"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="50"/>
+      <c r="A15" s="54"/>
       <c r="B15" s="2" t="s">
         <v>47</v>
       </c>
       <c r="C15" s="1"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="50"/>
+      <c r="A16" s="54"/>
       <c r="B16" s="2" t="s">
         <v>48</v>
       </c>
       <c r="C16" s="1"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="50"/>
+      <c r="A17" s="54"/>
       <c r="B17" s="2" t="s">
         <v>49</v>
       </c>
       <c r="C17" s="1"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="50"/>
+      <c r="A18" s="54"/>
       <c r="B18" s="2" t="s">
         <v>50</v>
       </c>
       <c r="C18" s="1"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="50"/>
+      <c r="A19" s="54"/>
       <c r="B19" s="2" t="s">
         <v>51</v>
       </c>
       <c r="C19" s="1"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="50"/>
+      <c r="A20" s="54"/>
       <c r="B20" s="2" t="s">
         <v>52</v>
       </c>
@@ -2215,7 +2215,7 @@
       <c r="C21" s="1"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="50" t="s">
+      <c r="A22" s="54" t="s">
         <v>31</v>
       </c>
       <c r="B22" s="2" t="s">
@@ -2226,7 +2226,7 @@
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="50"/>
+      <c r="A23" s="54"/>
       <c r="B23" s="2" t="s">
         <v>36</v>
       </c>

</xml_diff>

<commit_message>
completed gain scheduling PID
</commit_message>
<xml_diff>
--- a/Library_architecture.xlsx
+++ b/Library_architecture.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ssipvtltd-my.sharepoint.com/personal/abhinay_singh_ssinnovations_org/Documents/Abhinay's Workspace/main x/GitHub Repo/Repository_architecture/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="428" documentId="11_F25DC773A252ABDACC104854799F7F145BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F87DEF3B-2795-4FB8-90A0-8A77B8FC3BED}"/>
+  <xr:revisionPtr revIDLastSave="432" documentId="11_F25DC773A252ABDACC104854799F7F145BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{318EC673-4DBA-4A45-84C8-2DA5902EC627}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1011,7 +1011,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1507,7 +1507,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P15" sqref="P15"/>
+      <selection pane="bottomLeft" activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1914,8 +1914,12 @@
       <c r="F11" s="40" t="s">
         <v>100</v>
       </c>
-      <c r="H11" s="5"/>
-      <c r="I11" s="27"/>
+      <c r="H11" s="5">
+        <v>10</v>
+      </c>
+      <c r="I11" s="27" t="s">
+        <v>74</v>
+      </c>
       <c r="J11" s="18"/>
       <c r="K11" s="4"/>
       <c r="L11" s="6"/>
@@ -1933,13 +1937,17 @@
       <c r="F12" s="40" t="s">
         <v>101</v>
       </c>
-      <c r="H12" s="5"/>
-      <c r="I12" s="27"/>
+      <c r="H12" s="5">
+        <v>12</v>
+      </c>
+      <c r="I12" s="27" t="s">
+        <v>78</v>
+      </c>
       <c r="J12" s="18"/>
       <c r="K12" s="4"/>
       <c r="L12" s="6"/>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -1952,15 +1960,15 @@
       <c r="F13" s="40" t="s">
         <v>100</v>
       </c>
-      <c r="H13" s="5">
-        <v>10</v>
-      </c>
-      <c r="I13" s="27" t="s">
-        <v>74</v>
-      </c>
-      <c r="J13" s="18"/>
-      <c r="K13" s="4"/>
-      <c r="L13" s="6"/>
+      <c r="H13" s="7">
+        <v>13</v>
+      </c>
+      <c r="I13" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="J13" s="19"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="9"/>
     </row>
     <row r="14" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="7">
@@ -1975,26 +1983,6 @@
       <c r="F14" s="41" t="s">
         <v>100</v>
       </c>
-      <c r="H14" s="5">
-        <v>12</v>
-      </c>
-      <c r="I14" s="27" t="s">
-        <v>78</v>
-      </c>
-      <c r="J14" s="18"/>
-      <c r="K14" s="4"/>
-      <c r="L14" s="6"/>
-    </row>
-    <row r="15" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H15" s="7">
-        <v>13</v>
-      </c>
-      <c r="I15" s="28" t="s">
-        <v>79</v>
-      </c>
-      <c r="J15" s="19"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="9"/>
     </row>
     <row r="17" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added FLC, BMFLC, LPF_1, LPF_2, HPF_1 done
</commit_message>
<xml_diff>
--- a/Library_architecture.xlsx
+++ b/Library_architecture.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ssipvtltd-my.sharepoint.com/personal/abhinay_singh_ssinnovations_org/Documents/Abhinay's Workspace/main x/GitHub Repo/Repository_architecture/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="432" documentId="11_F25DC773A252ABDACC104854799F7F145BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{318EC673-4DBA-4A45-84C8-2DA5902EC627}"/>
+  <xr:revisionPtr revIDLastSave="481" documentId="11_F25DC773A252ABDACC104854799F7F145BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9D122E49-6D6C-439E-A48C-CA93719C2593}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="114">
   <si>
     <t>Control_sys</t>
   </si>
@@ -341,6 +341,36 @@
   </si>
   <si>
     <t>PID_GS</t>
+  </si>
+  <si>
+    <t>Periodic system</t>
+  </si>
+  <si>
+    <t>Estimation</t>
+  </si>
+  <si>
+    <t>KF</t>
+  </si>
+  <si>
+    <t>CF</t>
+  </si>
+  <si>
+    <t>EKF</t>
+  </si>
+  <si>
+    <t>UKF</t>
+  </si>
+  <si>
+    <t>SKF</t>
+  </si>
+  <si>
+    <t>FLC</t>
+  </si>
+  <si>
+    <t>WFLC</t>
+  </si>
+  <si>
+    <t>BMFLC</t>
   </si>
 </sst>
 </file>
@@ -434,7 +464,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="31">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -777,24 +807,15 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -802,50 +823,37 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -855,7 +863,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -944,25 +952,19 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -975,6 +977,32 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -996,14 +1024,11 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1011,8 +1036,11 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1312,10 +1340,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="51" t="s">
         <v>8</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -1324,16 +1352,16 @@
       <c r="D1" s="1"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="43"/>
-      <c r="B2" s="43"/>
+      <c r="A2" s="51"/>
+      <c r="B2" s="51"/>
       <c r="C2" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="43"/>
-      <c r="B3" s="43" t="s">
+      <c r="A3" s="51"/>
+      <c r="B3" s="51" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -1342,19 +1370,19 @@
       <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="43"/>
-      <c r="B4" s="43"/>
+      <c r="A4" s="51"/>
+      <c r="B4" s="51"/>
       <c r="C4" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="43"/>
-      <c r="B5" s="43" t="s">
+      <c r="A5" s="51"/>
+      <c r="B5" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="43" t="s">
+      <c r="C5" s="51" t="s">
         <v>2</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -1362,17 +1390,17 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="43"/>
-      <c r="B6" s="43"/>
-      <c r="C6" s="43"/>
+      <c r="A6" s="51"/>
+      <c r="B6" s="51"/>
+      <c r="C6" s="51"/>
       <c r="D6" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="43"/>
-      <c r="B7" s="43"/>
-      <c r="C7" s="43" t="s">
+      <c r="A7" s="51"/>
+      <c r="B7" s="51"/>
+      <c r="C7" s="51" t="s">
         <v>3</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -1380,16 +1408,16 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="43"/>
-      <c r="B8" s="43"/>
-      <c r="C8" s="43"/>
+      <c r="A8" s="51"/>
+      <c r="B8" s="51"/>
+      <c r="C8" s="51"/>
       <c r="D8" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="43"/>
-      <c r="B9" s="43" t="s">
+      <c r="A9" s="51"/>
+      <c r="B9" s="51" t="s">
         <v>4</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -1398,19 +1426,19 @@
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="43"/>
-      <c r="B10" s="43"/>
+      <c r="A10" s="51"/>
+      <c r="B10" s="51"/>
       <c r="C10" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="43"/>
-      <c r="B11" s="43" t="s">
+      <c r="A11" s="51"/>
+      <c r="B11" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="43" t="s">
+      <c r="C11" s="51" t="s">
         <v>5</v>
       </c>
       <c r="D11" s="1" t="s">
@@ -1418,17 +1446,17 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="43"/>
-      <c r="B12" s="43"/>
-      <c r="C12" s="43"/>
+      <c r="A12" s="51"/>
+      <c r="B12" s="51"/>
+      <c r="C12" s="51"/>
       <c r="D12" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="43"/>
-      <c r="B13" s="43"/>
-      <c r="C13" s="43" t="s">
+      <c r="A13" s="51"/>
+      <c r="B13" s="51"/>
+      <c r="C13" s="51" t="s">
         <v>7</v>
       </c>
       <c r="D13" s="1" t="s">
@@ -1436,19 +1464,19 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="43"/>
-      <c r="B14" s="43"/>
-      <c r="C14" s="43"/>
+      <c r="A14" s="51"/>
+      <c r="B14" s="51"/>
+      <c r="C14" s="51"/>
       <c r="D14" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="43"/>
-      <c r="B15" s="43" t="s">
+      <c r="A15" s="51"/>
+      <c r="B15" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="43" t="s">
+      <c r="C15" s="51" t="s">
         <v>6</v>
       </c>
       <c r="D15" s="1" t="s">
@@ -1456,17 +1484,17 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="43"/>
-      <c r="B16" s="43"/>
-      <c r="C16" s="43"/>
+      <c r="A16" s="51"/>
+      <c r="B16" s="51"/>
+      <c r="C16" s="51"/>
       <c r="D16" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="43"/>
-      <c r="B17" s="43"/>
-      <c r="C17" s="43" t="s">
+      <c r="A17" s="51"/>
+      <c r="B17" s="51"/>
+      <c r="C17" s="51" t="s">
         <v>25</v>
       </c>
       <c r="D17" s="1" t="s">
@@ -1474,9 +1502,9 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="43"/>
-      <c r="B18" s="43"/>
-      <c r="C18" s="43"/>
+      <c r="A18" s="51"/>
+      <c r="B18" s="51"/>
+      <c r="C18" s="51"/>
       <c r="D18" s="1" t="s">
         <v>27</v>
       </c>
@@ -1503,11 +1531,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FF893F8-BCFD-488B-AF9B-0D36D68641BC}">
-  <dimension ref="A1:Y20"/>
+  <dimension ref="A1:AE20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J23" sqref="J23"/>
+      <selection pane="bottomLeft" activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1517,25 +1545,26 @@
     <col min="15" max="15" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="27.140625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="34" t="s">
+    <row r="1" spans="1:31" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="C1" s="38" t="s">
+      <c r="C1" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="D1" s="35" t="s">
+      <c r="D1" s="33" t="s">
         <v>62</v>
       </c>
-      <c r="E1" s="35" t="s">
+      <c r="E1" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="F1" s="36" t="s">
+      <c r="F1" s="34" t="s">
         <v>102</v>
       </c>
       <c r="H1" s="13" t="s">
@@ -1556,13 +1585,13 @@
       <c r="N1" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="O1" s="33" t="s">
+      <c r="O1" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="P1" s="15" t="s">
+      <c r="P1" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="Q1" s="16" t="s">
+      <c r="Q1" s="14" t="s">
         <v>61</v>
       </c>
       <c r="R1" s="14" t="s">
@@ -1586,41 +1615,56 @@
       <c r="Y1" s="15" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="AA1" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB1" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="AC1" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD1" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE1" s="15" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" s="29">
         <v>1</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="37" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="31"/>
-      <c r="D2" s="37"/>
+      <c r="D2" s="35"/>
       <c r="E2" s="30"/>
-      <c r="F2" s="42" t="s">
+      <c r="F2" s="40" t="s">
         <v>100</v>
       </c>
-      <c r="H2" s="10">
+      <c r="H2" s="29">
         <v>1</v>
       </c>
-      <c r="I2" s="26" t="s">
+      <c r="I2" s="62" t="s">
         <v>65</v>
       </c>
-      <c r="J2" s="17"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="12"/>
-      <c r="N2" s="29">
+      <c r="J2" s="31"/>
+      <c r="K2" s="35"/>
+      <c r="L2" s="22"/>
+      <c r="N2" s="49">
         <v>1</v>
       </c>
-      <c r="O2" s="50" t="s">
+      <c r="O2" s="58" t="s">
         <v>88</v>
       </c>
-      <c r="P2" s="32" t="s">
+      <c r="P2" s="50" t="s">
         <v>81</v>
       </c>
-      <c r="Q2" s="31"/>
-      <c r="R2" s="30"/>
-      <c r="S2" s="22"/>
+      <c r="Q2" s="11"/>
+      <c r="R2" s="11"/>
+      <c r="S2" s="12"/>
       <c r="U2" s="10">
         <v>1</v>
       </c>
@@ -1630,8 +1674,17 @@
       <c r="W2" s="17"/>
       <c r="X2" s="11"/>
       <c r="Y2" s="12"/>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="AA2" s="10">
+        <v>1</v>
+      </c>
+      <c r="AB2" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="AC2" s="17"/>
+      <c r="AD2" s="11"/>
+      <c r="AE2" s="12"/>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -1641,7 +1694,7 @@
       <c r="C3" s="18"/>
       <c r="D3" s="25"/>
       <c r="E3" s="4"/>
-      <c r="F3" s="40" t="s">
+      <c r="F3" s="38" t="s">
         <v>100</v>
       </c>
       <c r="H3" s="5">
@@ -1651,16 +1704,16 @@
         <v>66</v>
       </c>
       <c r="J3" s="18"/>
-      <c r="K3" s="4"/>
+      <c r="K3" s="25"/>
       <c r="L3" s="6"/>
-      <c r="N3" s="5">
+      <c r="N3" s="42">
         <v>2</v>
       </c>
-      <c r="O3" s="51"/>
-      <c r="P3" s="27" t="s">
+      <c r="O3" s="59"/>
+      <c r="P3" s="44" t="s">
         <v>82</v>
       </c>
-      <c r="Q3" s="18"/>
+      <c r="Q3" s="4"/>
       <c r="R3" s="4"/>
       <c r="S3" s="6"/>
       <c r="U3" s="5">
@@ -1672,8 +1725,17 @@
       <c r="W3" s="18"/>
       <c r="X3" s="4"/>
       <c r="Y3" s="6"/>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="AA3" s="5">
+        <v>2</v>
+      </c>
+      <c r="AB3" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="AC3" s="18"/>
+      <c r="AD3" s="4"/>
+      <c r="AE3" s="6"/>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -1683,7 +1745,7 @@
       <c r="C4" s="18"/>
       <c r="D4" s="25"/>
       <c r="E4" s="4"/>
-      <c r="F4" s="40" t="s">
+      <c r="F4" s="38" t="s">
         <v>100</v>
       </c>
       <c r="H4" s="5">
@@ -1693,16 +1755,16 @@
         <v>67</v>
       </c>
       <c r="J4" s="18"/>
-      <c r="K4" s="4"/>
+      <c r="K4" s="25"/>
       <c r="L4" s="6"/>
-      <c r="N4" s="5">
+      <c r="N4" s="42">
         <v>3</v>
       </c>
-      <c r="O4" s="51"/>
-      <c r="P4" s="27" t="s">
+      <c r="O4" s="59"/>
+      <c r="P4" s="44" t="s">
         <v>83</v>
       </c>
-      <c r="Q4" s="18"/>
+      <c r="Q4" s="4"/>
       <c r="R4" s="4"/>
       <c r="S4" s="6"/>
       <c r="U4" s="5">
@@ -1714,8 +1776,17 @@
       <c r="W4" s="18"/>
       <c r="X4" s="4"/>
       <c r="Y4" s="6"/>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="AA4" s="5">
+        <v>3</v>
+      </c>
+      <c r="AB4" s="27" t="s">
+        <v>108</v>
+      </c>
+      <c r="AC4" s="18"/>
+      <c r="AD4" s="4"/>
+      <c r="AE4" s="6"/>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -1725,7 +1796,7 @@
       <c r="C5" s="18"/>
       <c r="D5" s="25"/>
       <c r="E5" s="4"/>
-      <c r="F5" s="40" t="s">
+      <c r="F5" s="38" t="s">
         <v>100</v>
       </c>
       <c r="H5" s="5">
@@ -1737,14 +1808,14 @@
       <c r="J5" s="18"/>
       <c r="K5" s="4"/>
       <c r="L5" s="6"/>
-      <c r="N5" s="5">
+      <c r="N5" s="42">
         <v>4</v>
       </c>
-      <c r="O5" s="51"/>
-      <c r="P5" s="27" t="s">
+      <c r="O5" s="59"/>
+      <c r="P5" s="44" t="s">
         <v>84</v>
       </c>
-      <c r="Q5" s="18"/>
+      <c r="Q5" s="4"/>
       <c r="R5" s="4"/>
       <c r="S5" s="6"/>
       <c r="U5" s="5">
@@ -1756,8 +1827,17 @@
       <c r="W5" s="18"/>
       <c r="X5" s="4"/>
       <c r="Y5" s="6"/>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="AA5" s="5">
+        <v>4</v>
+      </c>
+      <c r="AB5" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC5" s="18"/>
+      <c r="AD5" s="4"/>
+      <c r="AE5" s="6"/>
+    </row>
+    <row r="6" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -1767,7 +1847,7 @@
       <c r="C6" s="18"/>
       <c r="D6" s="25"/>
       <c r="E6" s="4"/>
-      <c r="F6" s="40" t="s">
+      <c r="F6" s="38" t="s">
         <v>100</v>
       </c>
       <c r="H6" s="5">
@@ -1779,18 +1859,27 @@
       <c r="J6" s="18"/>
       <c r="K6" s="4"/>
       <c r="L6" s="6"/>
-      <c r="N6" s="5">
+      <c r="N6" s="42">
         <v>5</v>
       </c>
-      <c r="O6" s="51"/>
-      <c r="P6" s="27" t="s">
+      <c r="O6" s="59"/>
+      <c r="P6" s="44" t="s">
         <v>85</v>
       </c>
-      <c r="Q6" s="18"/>
+      <c r="Q6" s="4"/>
       <c r="R6" s="4"/>
       <c r="S6" s="6"/>
-    </row>
-    <row r="7" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AA6" s="7">
+        <v>5</v>
+      </c>
+      <c r="AB6" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="AC6" s="19"/>
+      <c r="AD6" s="8"/>
+      <c r="AE6" s="9"/>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -1800,7 +1889,7 @@
       <c r="C7" s="18"/>
       <c r="D7" s="25"/>
       <c r="E7" s="4"/>
-      <c r="F7" s="40" t="s">
+      <c r="F7" s="38" t="s">
         <v>100</v>
       </c>
       <c r="H7" s="5">
@@ -1812,18 +1901,18 @@
       <c r="J7" s="18"/>
       <c r="K7" s="4"/>
       <c r="L7" s="6"/>
-      <c r="N7" s="7">
+      <c r="N7" s="42">
         <v>6</v>
       </c>
-      <c r="O7" s="52"/>
-      <c r="P7" s="28" t="s">
+      <c r="O7" s="59"/>
+      <c r="P7" s="44" t="s">
         <v>86</v>
       </c>
-      <c r="Q7" s="19"/>
-      <c r="R7" s="8"/>
-      <c r="S7" s="9"/>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Q7" s="4"/>
+      <c r="R7" s="4"/>
+      <c r="S7" s="6"/>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -1833,7 +1922,7 @@
       <c r="C8" s="18"/>
       <c r="D8" s="25"/>
       <c r="E8" s="4"/>
-      <c r="F8" s="40" t="s">
+      <c r="F8" s="38" t="s">
         <v>100</v>
       </c>
       <c r="H8" s="5">
@@ -1845,11 +1934,18 @@
       <c r="J8" s="18"/>
       <c r="K8" s="4"/>
       <c r="L8" s="6"/>
-      <c r="O8" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="N8" s="42">
+        <v>7</v>
+      </c>
+      <c r="O8" s="59"/>
+      <c r="P8" s="44" t="s">
+        <v>104</v>
+      </c>
+      <c r="Q8" s="4"/>
+      <c r="R8" s="4"/>
+      <c r="S8" s="6"/>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -1859,7 +1955,7 @@
       <c r="C9" s="18"/>
       <c r="D9" s="25"/>
       <c r="E9" s="4"/>
-      <c r="F9" s="40" t="s">
+      <c r="F9" s="38" t="s">
         <v>100</v>
       </c>
       <c r="H9" s="5">
@@ -1871,11 +1967,18 @@
       <c r="J9" s="18"/>
       <c r="K9" s="4"/>
       <c r="L9" s="6"/>
-      <c r="O9" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="N9" s="42">
+        <v>8</v>
+      </c>
+      <c r="O9" s="45" t="s">
+        <v>89</v>
+      </c>
+      <c r="P9" s="43"/>
+      <c r="Q9" s="4"/>
+      <c r="R9" s="4"/>
+      <c r="S9" s="6"/>
+    </row>
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -1885,7 +1988,7 @@
       <c r="C10" s="18"/>
       <c r="D10" s="25"/>
       <c r="E10" s="4"/>
-      <c r="F10" s="40" t="s">
+      <c r="F10" s="38" t="s">
         <v>100</v>
       </c>
       <c r="H10" s="5">
@@ -1897,11 +2000,18 @@
       <c r="J10" s="18"/>
       <c r="K10" s="4"/>
       <c r="L10" s="6"/>
-      <c r="O10" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="N10" s="42">
+        <v>9</v>
+      </c>
+      <c r="O10" s="45" t="s">
+        <v>90</v>
+      </c>
+      <c r="P10" s="43"/>
+      <c r="Q10" s="4"/>
+      <c r="R10" s="4"/>
+      <c r="S10" s="6"/>
+    </row>
+    <row r="11" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -1911,7 +2021,7 @@
       <c r="C11" s="18"/>
       <c r="D11" s="25"/>
       <c r="E11" s="4"/>
-      <c r="F11" s="40" t="s">
+      <c r="F11" s="38" t="s">
         <v>100</v>
       </c>
       <c r="H11" s="5">
@@ -1923,8 +2033,18 @@
       <c r="J11" s="18"/>
       <c r="K11" s="4"/>
       <c r="L11" s="6"/>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="N11" s="46">
+        <v>10</v>
+      </c>
+      <c r="O11" s="47" t="s">
+        <v>91</v>
+      </c>
+      <c r="P11" s="48"/>
+      <c r="Q11" s="8"/>
+      <c r="R11" s="8"/>
+      <c r="S11" s="9"/>
+    </row>
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -1934,11 +2054,11 @@
       <c r="C12" s="18"/>
       <c r="D12" s="25"/>
       <c r="E12" s="4"/>
-      <c r="F12" s="40" t="s">
+      <c r="F12" s="38" t="s">
         <v>101</v>
       </c>
       <c r="H12" s="5">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I12" s="27" t="s">
         <v>78</v>
@@ -1947,7 +2067,7 @@
       <c r="K12" s="4"/>
       <c r="L12" s="6"/>
     </row>
-    <row r="13" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -1957,20 +2077,20 @@
       <c r="C13" s="18"/>
       <c r="D13" s="25"/>
       <c r="E13" s="4"/>
-      <c r="F13" s="40" t="s">
+      <c r="F13" s="38" t="s">
         <v>100</v>
       </c>
-      <c r="H13" s="7">
-        <v>13</v>
-      </c>
-      <c r="I13" s="28" t="s">
+      <c r="H13" s="5">
+        <v>12</v>
+      </c>
+      <c r="I13" s="27" t="s">
         <v>79</v>
       </c>
-      <c r="J13" s="19"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="9"/>
-    </row>
-    <row r="14" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J13" s="18"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="6"/>
+    </row>
+    <row r="14" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="7">
         <v>13</v>
       </c>
@@ -1978,32 +2098,63 @@
         <v>103</v>
       </c>
       <c r="C14" s="19"/>
-      <c r="D14" s="55"/>
+      <c r="D14" s="41"/>
       <c r="E14" s="8"/>
-      <c r="F14" s="41" t="s">
+      <c r="F14" s="39" t="s">
         <v>100</v>
       </c>
+      <c r="H14" s="5">
+        <v>13</v>
+      </c>
+      <c r="I14" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="J14" s="18"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="6"/>
+    </row>
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="H15" s="5">
+        <v>14</v>
+      </c>
+      <c r="I15" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="J15" s="18"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="6"/>
+    </row>
+    <row r="16" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H16" s="7">
+        <v>15</v>
+      </c>
+      <c r="I16" s="63" t="s">
+        <v>113</v>
+      </c>
+      <c r="J16" s="19"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="9"/>
     </row>
     <row r="17" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="44" t="s">
+      <c r="B18" s="52" t="s">
         <v>75</v>
       </c>
-      <c r="C18" s="45"/>
+      <c r="C18" s="53"/>
       <c r="D18" s="22"/>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="46" t="s">
+      <c r="B19" s="54" t="s">
         <v>77</v>
       </c>
-      <c r="C19" s="47"/>
+      <c r="C19" s="55"/>
       <c r="D19" s="23"/>
     </row>
     <row r="20" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="48" t="s">
+      <c r="B20" s="56" t="s">
         <v>76</v>
       </c>
-      <c r="C20" s="49"/>
+      <c r="C20" s="57"/>
       <c r="D20" s="24"/>
     </row>
   </sheetData>
@@ -2011,7 +2162,7 @@
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="B19:C19"/>
     <mergeCell ref="B20:C20"/>
-    <mergeCell ref="O2:O7"/>
+    <mergeCell ref="O2:O8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2046,7 +2197,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="60" t="s">
         <v>55</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -2055,7 +2206,7 @@
       <c r="C1" s="1"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="53"/>
+      <c r="A2" s="60"/>
       <c r="B2" s="2" t="s">
         <v>34</v>
       </c>
@@ -2083,113 +2234,113 @@
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="53" t="s">
+      <c r="A6" s="60" t="s">
         <v>29</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>38</v>
       </c>
       <c r="C6" s="1"/>
-      <c r="K6" s="54" t="s">
+      <c r="K6" s="61" t="s">
         <v>54</v>
       </c>
-      <c r="L6" s="54"/>
+      <c r="L6" s="61"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="53"/>
+      <c r="A7" s="60"/>
       <c r="B7" s="2" t="s">
         <v>39</v>
       </c>
       <c r="C7" s="1"/>
-      <c r="K7" s="54"/>
-      <c r="L7" s="54"/>
+      <c r="K7" s="61"/>
+      <c r="L7" s="61"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="53"/>
+      <c r="A8" s="60"/>
       <c r="B8" s="2" t="s">
         <v>41</v>
       </c>
       <c r="C8" s="1"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="53"/>
+      <c r="A9" s="60"/>
       <c r="B9" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C9" s="1"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="53"/>
+      <c r="A10" s="60"/>
       <c r="B10" s="2" t="s">
         <v>43</v>
       </c>
       <c r="C10" s="1"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="53"/>
+      <c r="A11" s="60"/>
       <c r="B11" s="2" t="s">
         <v>40</v>
       </c>
       <c r="C11" s="1"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="53"/>
+      <c r="A12" s="60"/>
       <c r="B12" s="2" t="s">
         <v>44</v>
       </c>
       <c r="C12" s="1"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="53"/>
+      <c r="A13" s="60"/>
       <c r="B13" s="2" t="s">
         <v>45</v>
       </c>
       <c r="C13" s="1"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="53"/>
+      <c r="A14" s="60"/>
       <c r="B14" s="2" t="s">
         <v>46</v>
       </c>
       <c r="C14" s="1"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="53"/>
+      <c r="A15" s="60"/>
       <c r="B15" s="2" t="s">
         <v>47</v>
       </c>
       <c r="C15" s="1"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="53"/>
+      <c r="A16" s="60"/>
       <c r="B16" s="2" t="s">
         <v>48</v>
       </c>
       <c r="C16" s="1"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="53"/>
+      <c r="A17" s="60"/>
       <c r="B17" s="2" t="s">
         <v>49</v>
       </c>
       <c r="C17" s="1"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="53"/>
+      <c r="A18" s="60"/>
       <c r="B18" s="2" t="s">
         <v>50</v>
       </c>
       <c r="C18" s="1"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="53"/>
+      <c r="A19" s="60"/>
       <c r="B19" s="2" t="s">
         <v>51</v>
       </c>
       <c r="C19" s="1"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="53"/>
+      <c r="A20" s="60"/>
       <c r="B20" s="2" t="s">
         <v>52</v>
       </c>
@@ -2203,7 +2354,7 @@
       <c r="C21" s="1"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="53" t="s">
+      <c r="A22" s="60" t="s">
         <v>31</v>
       </c>
       <c r="B22" s="2" t="s">
@@ -2214,7 +2365,7 @@
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="53"/>
+      <c r="A23" s="60"/>
       <c r="B23" s="2" t="s">
         <v>36</v>
       </c>

</xml_diff>

<commit_message>
added ackarman and bicycle model
</commit_message>
<xml_diff>
--- a/Library_architecture.xlsx
+++ b/Library_architecture.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ssipvtltd-my.sharepoint.com/personal/abhinay_singh_ssinnovations_org/Documents/Abhinay's Workspace/main x/GitHub Repo/Repository_architecture/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="565" documentId="11_F25DC773A252ABDACC104854799F7F145BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1728C7DD-785B-4513-B269-DFFFA3997FCF}"/>
+  <xr:revisionPtr revIDLastSave="590" documentId="11_F25DC773A252ABDACC104854799F7F145BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9F49195D-4598-4E77-BBAC-D941C60ECF2A}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="131">
   <si>
     <t>Control_sys</t>
   </si>
@@ -401,6 +401,27 @@
   </si>
   <si>
     <t>SRL</t>
+  </si>
+  <si>
+    <t>Mobile Robot</t>
+  </si>
+  <si>
+    <t>D_drive_unicycle</t>
+  </si>
+  <si>
+    <t>Wheel_odom_d_drive</t>
+  </si>
+  <si>
+    <t>Ackarman_unicycle</t>
+  </si>
+  <si>
+    <t>Wheel_odom_ackarman</t>
+  </si>
+  <si>
+    <t>Wheel_odom_bicycle</t>
+  </si>
+  <si>
+    <t>Bicycle_unicycle</t>
   </si>
 </sst>
 </file>
@@ -899,7 +920,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1083,6 +1104,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1573,11 +1597,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FF893F8-BCFD-488B-AF9B-0D36D68641BC}">
-  <dimension ref="A1:AK20"/>
+  <dimension ref="A1:AQ20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U11" sqref="U11"/>
+      <selection pane="bottomLeft" activeCell="AR19" sqref="AR19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1589,9 +1613,10 @@
     <col min="22" max="22" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:43" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="32" t="s">
         <v>59</v>
       </c>
@@ -1689,8 +1714,23 @@
       <c r="AK1" s="15" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AM1" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="AN1" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="AO1" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="AP1" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="AQ1" s="15" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A2" s="29">
         <v>1</v>
       </c>
@@ -1751,8 +1791,17 @@
       <c r="AI2" s="17"/>
       <c r="AJ2" s="11"/>
       <c r="AK2" s="12"/>
-    </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AM2" s="10">
+        <v>1</v>
+      </c>
+      <c r="AN2" s="26" t="s">
+        <v>125</v>
+      </c>
+      <c r="AO2" s="17"/>
+      <c r="AP2" s="66"/>
+      <c r="AQ2" s="12"/>
+    </row>
+    <row r="3" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -1811,8 +1860,17 @@
       <c r="AI3" s="18"/>
       <c r="AJ3" s="4"/>
       <c r="AK3" s="6"/>
-    </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AM3" s="5">
+        <v>2</v>
+      </c>
+      <c r="AN3" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="AO3" s="18"/>
+      <c r="AP3" s="25"/>
+      <c r="AQ3" s="6"/>
+    </row>
+    <row r="4" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -1871,8 +1929,17 @@
       <c r="AI4" s="18"/>
       <c r="AJ4" s="4"/>
       <c r="AK4" s="6"/>
-    </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AM4" s="5">
+        <v>3</v>
+      </c>
+      <c r="AN4" s="27" t="s">
+        <v>127</v>
+      </c>
+      <c r="AO4" s="18"/>
+      <c r="AP4" s="4"/>
+      <c r="AQ4" s="6"/>
+    </row>
+    <row r="5" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -1931,8 +1998,17 @@
       <c r="AI5" s="18"/>
       <c r="AJ5" s="4"/>
       <c r="AK5" s="6"/>
-    </row>
-    <row r="6" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AM5" s="5">
+        <v>4</v>
+      </c>
+      <c r="AN5" s="27" t="s">
+        <v>128</v>
+      </c>
+      <c r="AO5" s="18"/>
+      <c r="AP5" s="4"/>
+      <c r="AQ5" s="6"/>
+    </row>
+    <row r="6" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -1982,8 +2058,17 @@
       <c r="AI6" s="19"/>
       <c r="AJ6" s="8"/>
       <c r="AK6" s="9"/>
-    </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AM6" s="5">
+        <v>5</v>
+      </c>
+      <c r="AN6" s="27" t="s">
+        <v>130</v>
+      </c>
+      <c r="AO6" s="18"/>
+      <c r="AP6" s="4"/>
+      <c r="AQ6" s="6"/>
+    </row>
+    <row r="7" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -2024,8 +2109,17 @@
       <c r="W7" s="18"/>
       <c r="X7" s="4"/>
       <c r="Y7" s="6"/>
-    </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AM7" s="7">
+        <v>6</v>
+      </c>
+      <c r="AN7" s="28" t="s">
+        <v>129</v>
+      </c>
+      <c r="AO7" s="19"/>
+      <c r="AP7" s="8"/>
+      <c r="AQ7" s="9"/>
+    </row>
+    <row r="8" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -2067,7 +2161,7 @@
       <c r="X8" s="4"/>
       <c r="Y8" s="6"/>
     </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -2109,7 +2203,7 @@
       <c r="X9" s="4"/>
       <c r="Y9" s="6"/>
     </row>
-    <row r="10" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -2151,7 +2245,7 @@
       <c r="X10" s="8"/>
       <c r="Y10" s="9"/>
     </row>
-    <row r="11" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -2184,7 +2278,7 @@
       <c r="R11" s="8"/>
       <c r="S11" s="9"/>
     </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -2207,7 +2301,7 @@
       <c r="K12" s="4"/>
       <c r="L12" s="6"/>
     </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -2230,7 +2324,7 @@
       <c r="K13" s="53"/>
       <c r="L13" s="6"/>
     </row>
-    <row r="14" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="7">
         <v>13</v>
       </c>
@@ -2253,7 +2347,7 @@
       <c r="K14" s="53"/>
       <c r="L14" s="6"/>
     </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:43" x14ac:dyDescent="0.25">
       <c r="H15" s="5">
         <v>14</v>
       </c>
@@ -2264,7 +2358,7 @@
       <c r="K15" s="53"/>
       <c r="L15" s="6"/>
     </row>
-    <row r="16" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H16" s="7">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
added BPF and BSF
</commit_message>
<xml_diff>
--- a/Library_architecture.xlsx
+++ b/Library_architecture.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ssipvtltd-my.sharepoint.com/personal/abhinay_singh_ssinnovations_org/Documents/Abhinay's Workspace/main x/GitHub Repo/Repository_architecture/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="633" documentId="11_F25DC773A252ABDACC104854799F7F145BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F9D0C2DE-BE49-47A5-B2F5-FBD2D2A4D1B5}"/>
+  <xr:revisionPtr revIDLastSave="634" documentId="11_F25DC773A252ABDACC104854799F7F145BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0060B599-215E-4535-B7B3-EE40ECD3B93B}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1634,7 +1634,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K26" sqref="K26"/>
+      <selection pane="bottomLeft" activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2113,7 +2113,7 @@
         <v>70</v>
       </c>
       <c r="J6" s="18"/>
-      <c r="K6" s="4"/>
+      <c r="K6" s="25"/>
       <c r="L6" s="6"/>
       <c r="N6" s="42">
         <v>5</v>

</xml_diff>

<commit_message>
added aerial vehicle input modes
</commit_message>
<xml_diff>
--- a/Library_architecture.xlsx
+++ b/Library_architecture.xlsx
@@ -8,20 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ssipvtltd-my.sharepoint.com/personal/abhinay_singh_ssinnovations_org/Documents/Abhinay's Workspace/main x/GitHub Repo/Repository_architecture/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="40" documentId="13_ncr:1_{D84D0752-E4BB-48DB-83F5-1B8FFA54D692}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E7E1F23E-8B16-404B-B7E4-0847F105A486}"/>
+  <xr:revisionPtr revIDLastSave="253" documentId="13_ncr:1_{D84D0752-E4BB-48DB-83F5-1B8FFA54D692}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FC136B26-C786-4EFA-BA53-316FA637DB7B}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Control system" sheetId="5" r:id="rId1"/>
-    <sheet name="Analysis" sheetId="10" r:id="rId2"/>
-    <sheet name="System identification" sheetId="9" r:id="rId3"/>
+    <sheet name="Filter" sheetId="3" r:id="rId2"/>
+    <sheet name="Analysis" sheetId="10" r:id="rId3"/>
     <sheet name="Signal Generator" sheetId="8" r:id="rId4"/>
     <sheet name="Estimation" sheetId="7" r:id="rId5"/>
-    <sheet name="Mobile robot" sheetId="6" r:id="rId6"/>
-    <sheet name="Constants" sheetId="4" r:id="rId7"/>
-    <sheet name="Filter" sheetId="3" r:id="rId8"/>
+    <sheet name="System identification" sheetId="9" r:id="rId6"/>
+    <sheet name="Mobile robot" sheetId="6" r:id="rId7"/>
+    <sheet name="Constants" sheetId="4" r:id="rId8"/>
     <sheet name="Math" sheetId="2" r:id="rId9"/>
+    <sheet name="Aerial vehicle" sheetId="11" r:id="rId10"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="141">
   <si>
     <t>I</t>
   </si>
@@ -392,7 +393,70 @@
     <t>Chirp</t>
   </si>
   <si>
-    <t>Inpulse</t>
+    <t>Input Combination</t>
+  </si>
+  <si>
+    <t>psi</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>z</t>
+  </si>
+  <si>
+    <t>wz</t>
+  </si>
+  <si>
+    <t>vz</t>
+  </si>
+  <si>
+    <t>phi</t>
+  </si>
+  <si>
+    <t>th</t>
+  </si>
+  <si>
+    <t>vx</t>
+  </si>
+  <si>
+    <t>vy</t>
+  </si>
+  <si>
+    <t>ax</t>
+  </si>
+  <si>
+    <t>ay</t>
+  </si>
+  <si>
+    <t>az</t>
+  </si>
+  <si>
+    <t>wx</t>
+  </si>
+  <si>
+    <t>wy</t>
+  </si>
+  <si>
+    <t>Mx</t>
+  </si>
+  <si>
+    <t>My</t>
+  </si>
+  <si>
+    <t>Mz</t>
+  </si>
+  <si>
+    <t>Fx</t>
+  </si>
+  <si>
+    <t>Fy</t>
+  </si>
+  <si>
+    <t>Fz</t>
   </si>
 </sst>
 </file>
@@ -451,7 +515,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -491,8 +555,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="29">
+  <borders count="48">
     <border>
       <left/>
       <right/>
@@ -884,6 +954,239 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -891,7 +1194,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="157">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1046,6 +1349,117 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="9" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="8" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="10" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="3" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="36" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="37" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="37" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="38" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="39" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="31" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="40" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="42" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="8" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="9" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="9" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="23" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="24" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="24" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="19" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="5" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="6" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="23" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="24" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="24" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="43" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="30" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="30" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="44" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="45" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="36" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="43" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="44" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="31" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="40" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="23" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="46" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="37" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="38" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="47" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="46" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="41" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="23" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1085,6 +1499,12 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF3300"/>
+      <color rgb="FFFF0000"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1363,7 +1783,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O23" sqref="O23"/>
+      <selection pane="bottomLeft" activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1405,10 +1825,10 @@
       <c r="F2" s="40" t="s">
         <v>77</v>
       </c>
-      <c r="H2" s="56" t="s">
+      <c r="H2" s="147" t="s">
         <v>52</v>
       </c>
-      <c r="I2" s="57"/>
+      <c r="I2" s="148"/>
       <c r="J2" s="22"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -1424,10 +1844,10 @@
       <c r="F3" s="38" t="s">
         <v>77</v>
       </c>
-      <c r="H3" s="58" t="s">
+      <c r="H3" s="149" t="s">
         <v>54</v>
       </c>
-      <c r="I3" s="59"/>
+      <c r="I3" s="150"/>
       <c r="J3" s="23"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1443,10 +1863,10 @@
       <c r="F4" s="38" t="s">
         <v>77</v>
       </c>
-      <c r="H4" s="60" t="s">
+      <c r="H4" s="151" t="s">
         <v>53</v>
       </c>
-      <c r="I4" s="61"/>
+      <c r="I4" s="152"/>
       <c r="J4" s="24"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -1600,26 +2020,1436 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0761546C-2124-4D87-9532-0ECA1AEF2C0F}">
-  <dimension ref="A1:I5"/>
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C19B9CAB-2F1B-47BE-BDE0-1AC6DEAAB058}">
+  <dimension ref="A1:V52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G2" sqref="G2:I4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="X35" sqref="X35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
   </cols>
+  <sheetData>
+    <row r="1" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="61" t="s">
+        <v>119</v>
+      </c>
+      <c r="B1" s="57" t="s">
+        <v>121</v>
+      </c>
+      <c r="C1" s="58" t="s">
+        <v>122</v>
+      </c>
+      <c r="D1" s="58" t="s">
+        <v>123</v>
+      </c>
+      <c r="E1" s="58" t="s">
+        <v>128</v>
+      </c>
+      <c r="F1" s="58" t="s">
+        <v>129</v>
+      </c>
+      <c r="G1" s="58" t="s">
+        <v>125</v>
+      </c>
+      <c r="H1" s="58" t="s">
+        <v>130</v>
+      </c>
+      <c r="I1" s="58" t="s">
+        <v>131</v>
+      </c>
+      <c r="J1" s="81" t="s">
+        <v>132</v>
+      </c>
+      <c r="K1" s="57" t="s">
+        <v>126</v>
+      </c>
+      <c r="L1" s="58" t="s">
+        <v>127</v>
+      </c>
+      <c r="M1" s="58" t="s">
+        <v>120</v>
+      </c>
+      <c r="N1" s="58" t="s">
+        <v>133</v>
+      </c>
+      <c r="O1" s="58" t="s">
+        <v>134</v>
+      </c>
+      <c r="P1" s="59" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q1" s="60" t="s">
+        <v>135</v>
+      </c>
+      <c r="R1" s="58" t="s">
+        <v>136</v>
+      </c>
+      <c r="S1" s="58" t="s">
+        <v>137</v>
+      </c>
+      <c r="T1" s="58" t="s">
+        <v>138</v>
+      </c>
+      <c r="U1" s="58" t="s">
+        <v>139</v>
+      </c>
+      <c r="V1" s="59" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="62">
+        <v>0</v>
+      </c>
+      <c r="B2" s="92"/>
+      <c r="C2" s="93"/>
+      <c r="D2" s="93"/>
+      <c r="E2" s="93"/>
+      <c r="F2" s="93"/>
+      <c r="G2" s="93"/>
+      <c r="H2" s="93"/>
+      <c r="I2" s="93"/>
+      <c r="J2" s="95"/>
+      <c r="K2" s="92"/>
+      <c r="L2" s="93"/>
+      <c r="M2" s="93"/>
+      <c r="N2" s="93"/>
+      <c r="O2" s="93"/>
+      <c r="P2" s="94"/>
+      <c r="Q2" s="140"/>
+      <c r="R2" s="128"/>
+      <c r="S2" s="128"/>
+      <c r="T2" s="128"/>
+      <c r="U2" s="128"/>
+      <c r="V2" s="129"/>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A3" s="63">
+        <v>1</v>
+      </c>
+      <c r="B3" s="99"/>
+      <c r="C3" s="100"/>
+      <c r="D3" s="100"/>
+      <c r="E3" s="101"/>
+      <c r="F3" s="101"/>
+      <c r="G3" s="101"/>
+      <c r="H3" s="101"/>
+      <c r="I3" s="101"/>
+      <c r="J3" s="135"/>
+      <c r="K3" s="130"/>
+      <c r="L3" s="101"/>
+      <c r="M3" s="100"/>
+      <c r="N3" s="101"/>
+      <c r="O3" s="101"/>
+      <c r="P3" s="102"/>
+      <c r="Q3" s="103"/>
+      <c r="R3" s="101"/>
+      <c r="S3" s="101"/>
+      <c r="T3" s="101"/>
+      <c r="U3" s="101"/>
+      <c r="V3" s="102"/>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A4" s="63">
+        <v>2</v>
+      </c>
+      <c r="B4" s="78"/>
+      <c r="C4" s="75"/>
+      <c r="D4" s="75"/>
+      <c r="E4" s="69"/>
+      <c r="F4" s="69"/>
+      <c r="G4" s="69"/>
+      <c r="H4" s="69"/>
+      <c r="I4" s="69"/>
+      <c r="J4" s="84"/>
+      <c r="K4" s="79"/>
+      <c r="L4" s="69"/>
+      <c r="M4" s="69"/>
+      <c r="N4" s="69"/>
+      <c r="O4" s="69"/>
+      <c r="P4" s="87"/>
+      <c r="Q4" s="68"/>
+      <c r="R4" s="69"/>
+      <c r="S4" s="69"/>
+      <c r="T4" s="69"/>
+      <c r="U4" s="69"/>
+      <c r="V4" s="70"/>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A5" s="63">
+        <v>3</v>
+      </c>
+      <c r="B5" s="78"/>
+      <c r="C5" s="75"/>
+      <c r="D5" s="66"/>
+      <c r="E5" s="66"/>
+      <c r="F5" s="66"/>
+      <c r="G5" s="75"/>
+      <c r="H5" s="66"/>
+      <c r="I5" s="66"/>
+      <c r="J5" s="83"/>
+      <c r="K5" s="86"/>
+      <c r="L5" s="66"/>
+      <c r="M5" s="75"/>
+      <c r="N5" s="66"/>
+      <c r="O5" s="66"/>
+      <c r="P5" s="67"/>
+      <c r="Q5" s="68"/>
+      <c r="R5" s="69"/>
+      <c r="S5" s="69"/>
+      <c r="T5" s="69"/>
+      <c r="U5" s="69"/>
+      <c r="V5" s="70"/>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A6" s="63">
+        <v>4</v>
+      </c>
+      <c r="B6" s="78"/>
+      <c r="C6" s="75"/>
+      <c r="D6" s="69"/>
+      <c r="E6" s="69"/>
+      <c r="F6" s="69"/>
+      <c r="G6" s="75"/>
+      <c r="H6" s="69"/>
+      <c r="I6" s="69"/>
+      <c r="J6" s="84"/>
+      <c r="K6" s="79"/>
+      <c r="L6" s="69"/>
+      <c r="M6" s="69"/>
+      <c r="N6" s="69"/>
+      <c r="O6" s="69"/>
+      <c r="P6" s="87"/>
+      <c r="Q6" s="68"/>
+      <c r="R6" s="69"/>
+      <c r="S6" s="69"/>
+      <c r="T6" s="69"/>
+      <c r="U6" s="69"/>
+      <c r="V6" s="70"/>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A7" s="63">
+        <v>5</v>
+      </c>
+      <c r="B7" s="78"/>
+      <c r="C7" s="75"/>
+      <c r="D7" s="66"/>
+      <c r="E7" s="66"/>
+      <c r="F7" s="66"/>
+      <c r="G7" s="66"/>
+      <c r="H7" s="66"/>
+      <c r="I7" s="66"/>
+      <c r="J7" s="136"/>
+      <c r="K7" s="86"/>
+      <c r="L7" s="66"/>
+      <c r="M7" s="75"/>
+      <c r="N7" s="66"/>
+      <c r="O7" s="66"/>
+      <c r="P7" s="67"/>
+      <c r="Q7" s="68"/>
+      <c r="R7" s="69"/>
+      <c r="S7" s="69"/>
+      <c r="T7" s="69"/>
+      <c r="U7" s="69"/>
+      <c r="V7" s="70"/>
+    </row>
+    <row r="8" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="63">
+        <v>6</v>
+      </c>
+      <c r="B8" s="104"/>
+      <c r="C8" s="105"/>
+      <c r="D8" s="72"/>
+      <c r="E8" s="72"/>
+      <c r="F8" s="72"/>
+      <c r="G8" s="106"/>
+      <c r="H8" s="72"/>
+      <c r="I8" s="72"/>
+      <c r="J8" s="137"/>
+      <c r="K8" s="80"/>
+      <c r="L8" s="72"/>
+      <c r="M8" s="72"/>
+      <c r="N8" s="72"/>
+      <c r="O8" s="72"/>
+      <c r="P8" s="107"/>
+      <c r="Q8" s="71"/>
+      <c r="R8" s="72"/>
+      <c r="S8" s="72"/>
+      <c r="T8" s="72"/>
+      <c r="U8" s="72"/>
+      <c r="V8" s="73"/>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A9" s="63">
+        <v>7</v>
+      </c>
+      <c r="B9" s="108"/>
+      <c r="C9" s="109"/>
+      <c r="D9" s="100"/>
+      <c r="E9" s="110"/>
+      <c r="F9" s="110"/>
+      <c r="G9" s="101"/>
+      <c r="H9" s="101"/>
+      <c r="I9" s="101"/>
+      <c r="J9" s="135"/>
+      <c r="K9" s="130"/>
+      <c r="L9" s="101"/>
+      <c r="M9" s="100"/>
+      <c r="N9" s="101"/>
+      <c r="O9" s="101"/>
+      <c r="P9" s="102"/>
+      <c r="Q9" s="141"/>
+      <c r="R9" s="131"/>
+      <c r="S9" s="131"/>
+      <c r="T9" s="131"/>
+      <c r="U9" s="131"/>
+      <c r="V9" s="132"/>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A10" s="63">
+        <v>8</v>
+      </c>
+      <c r="B10" s="88"/>
+      <c r="C10" s="89"/>
+      <c r="D10" s="75"/>
+      <c r="E10" s="91"/>
+      <c r="F10" s="91"/>
+      <c r="G10" s="69"/>
+      <c r="H10" s="69"/>
+      <c r="I10" s="69"/>
+      <c r="J10" s="84"/>
+      <c r="K10" s="79"/>
+      <c r="L10" s="69"/>
+      <c r="M10" s="69"/>
+      <c r="N10" s="69"/>
+      <c r="O10" s="69"/>
+      <c r="P10" s="87"/>
+      <c r="Q10" s="68"/>
+      <c r="R10" s="69"/>
+      <c r="S10" s="69"/>
+      <c r="T10" s="69"/>
+      <c r="U10" s="69"/>
+      <c r="V10" s="70"/>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A11" s="63">
+        <v>9</v>
+      </c>
+      <c r="B11" s="88"/>
+      <c r="C11" s="89"/>
+      <c r="D11" s="66"/>
+      <c r="E11" s="90"/>
+      <c r="F11" s="90"/>
+      <c r="G11" s="75"/>
+      <c r="H11" s="66"/>
+      <c r="I11" s="66"/>
+      <c r="J11" s="83"/>
+      <c r="K11" s="86"/>
+      <c r="L11" s="66"/>
+      <c r="M11" s="75"/>
+      <c r="N11" s="66"/>
+      <c r="O11" s="66"/>
+      <c r="P11" s="67"/>
+      <c r="Q11" s="68"/>
+      <c r="R11" s="69"/>
+      <c r="S11" s="69"/>
+      <c r="T11" s="69"/>
+      <c r="U11" s="69"/>
+      <c r="V11" s="70"/>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A12" s="63">
+        <v>10</v>
+      </c>
+      <c r="B12" s="88"/>
+      <c r="C12" s="89"/>
+      <c r="D12" s="69"/>
+      <c r="E12" s="91"/>
+      <c r="F12" s="91"/>
+      <c r="G12" s="75"/>
+      <c r="H12" s="69"/>
+      <c r="I12" s="69"/>
+      <c r="J12" s="84"/>
+      <c r="K12" s="79"/>
+      <c r="L12" s="69"/>
+      <c r="M12" s="69"/>
+      <c r="N12" s="69"/>
+      <c r="O12" s="69"/>
+      <c r="P12" s="87"/>
+      <c r="Q12" s="68"/>
+      <c r="R12" s="69"/>
+      <c r="S12" s="69"/>
+      <c r="T12" s="69"/>
+      <c r="U12" s="69"/>
+      <c r="V12" s="70"/>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A13" s="63">
+        <v>11</v>
+      </c>
+      <c r="B13" s="88"/>
+      <c r="C13" s="89"/>
+      <c r="D13" s="66"/>
+      <c r="E13" s="90"/>
+      <c r="F13" s="90"/>
+      <c r="G13" s="66"/>
+      <c r="H13" s="66"/>
+      <c r="I13" s="66"/>
+      <c r="J13" s="136"/>
+      <c r="K13" s="86"/>
+      <c r="L13" s="66"/>
+      <c r="M13" s="75"/>
+      <c r="N13" s="66"/>
+      <c r="O13" s="66"/>
+      <c r="P13" s="67"/>
+      <c r="Q13" s="68"/>
+      <c r="R13" s="69"/>
+      <c r="S13" s="69"/>
+      <c r="T13" s="69"/>
+      <c r="U13" s="69"/>
+      <c r="V13" s="70"/>
+    </row>
+    <row r="14" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="63">
+        <v>12</v>
+      </c>
+      <c r="B14" s="111"/>
+      <c r="C14" s="112"/>
+      <c r="D14" s="72"/>
+      <c r="E14" s="113"/>
+      <c r="F14" s="113"/>
+      <c r="G14" s="106"/>
+      <c r="H14" s="72"/>
+      <c r="I14" s="72"/>
+      <c r="J14" s="137"/>
+      <c r="K14" s="80"/>
+      <c r="L14" s="72"/>
+      <c r="M14" s="72"/>
+      <c r="N14" s="72"/>
+      <c r="O14" s="72"/>
+      <c r="P14" s="107"/>
+      <c r="Q14" s="71"/>
+      <c r="R14" s="72"/>
+      <c r="S14" s="72"/>
+      <c r="T14" s="72"/>
+      <c r="U14" s="72"/>
+      <c r="V14" s="73"/>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A15" s="56">
+        <v>13</v>
+      </c>
+      <c r="B15" s="96"/>
+      <c r="C15" s="97"/>
+      <c r="D15" s="74"/>
+      <c r="E15" s="97"/>
+      <c r="F15" s="97"/>
+      <c r="G15" s="65"/>
+      <c r="H15" s="98"/>
+      <c r="I15" s="98"/>
+      <c r="J15" s="82"/>
+      <c r="K15" s="76"/>
+      <c r="L15" s="65"/>
+      <c r="M15" s="74"/>
+      <c r="N15" s="65"/>
+      <c r="O15" s="65"/>
+      <c r="P15" s="77"/>
+      <c r="Q15" s="124"/>
+      <c r="R15" s="122"/>
+      <c r="S15" s="122"/>
+      <c r="T15" s="122"/>
+      <c r="U15" s="122"/>
+      <c r="V15" s="123"/>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A16" s="56">
+        <v>14</v>
+      </c>
+      <c r="B16" s="88"/>
+      <c r="C16" s="89"/>
+      <c r="D16" s="75"/>
+      <c r="E16" s="89"/>
+      <c r="F16" s="89"/>
+      <c r="G16" s="69"/>
+      <c r="H16" s="91"/>
+      <c r="I16" s="91"/>
+      <c r="J16" s="84"/>
+      <c r="K16" s="79"/>
+      <c r="L16" s="69"/>
+      <c r="M16" s="69"/>
+      <c r="N16" s="69"/>
+      <c r="O16" s="69"/>
+      <c r="P16" s="87"/>
+      <c r="Q16" s="68"/>
+      <c r="R16" s="69"/>
+      <c r="S16" s="69"/>
+      <c r="T16" s="69"/>
+      <c r="U16" s="69"/>
+      <c r="V16" s="70"/>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A17" s="56">
+        <v>15</v>
+      </c>
+      <c r="B17" s="88"/>
+      <c r="C17" s="89"/>
+      <c r="D17" s="66"/>
+      <c r="E17" s="89"/>
+      <c r="F17" s="89"/>
+      <c r="G17" s="75"/>
+      <c r="H17" s="90"/>
+      <c r="I17" s="90"/>
+      <c r="J17" s="83"/>
+      <c r="K17" s="86"/>
+      <c r="L17" s="66"/>
+      <c r="M17" s="75"/>
+      <c r="N17" s="66"/>
+      <c r="O17" s="66"/>
+      <c r="P17" s="67"/>
+      <c r="Q17" s="68"/>
+      <c r="R17" s="69"/>
+      <c r="S17" s="69"/>
+      <c r="T17" s="69"/>
+      <c r="U17" s="69"/>
+      <c r="V17" s="70"/>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A18" s="56">
+        <v>16</v>
+      </c>
+      <c r="B18" s="88"/>
+      <c r="C18" s="89"/>
+      <c r="D18" s="69"/>
+      <c r="E18" s="69"/>
+      <c r="F18" s="69"/>
+      <c r="G18" s="75"/>
+      <c r="H18" s="91"/>
+      <c r="I18" s="91"/>
+      <c r="J18" s="84"/>
+      <c r="K18" s="79"/>
+      <c r="L18" s="69"/>
+      <c r="M18" s="69"/>
+      <c r="N18" s="69"/>
+      <c r="O18" s="69"/>
+      <c r="P18" s="87"/>
+      <c r="Q18" s="68"/>
+      <c r="R18" s="69"/>
+      <c r="S18" s="69"/>
+      <c r="T18" s="69"/>
+      <c r="U18" s="69"/>
+      <c r="V18" s="70"/>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A19" s="56">
+        <v>17</v>
+      </c>
+      <c r="B19" s="88"/>
+      <c r="C19" s="89"/>
+      <c r="D19" s="66"/>
+      <c r="E19" s="69"/>
+      <c r="F19" s="69"/>
+      <c r="G19" s="66"/>
+      <c r="H19" s="90"/>
+      <c r="I19" s="90"/>
+      <c r="J19" s="136"/>
+      <c r="K19" s="86"/>
+      <c r="L19" s="66"/>
+      <c r="M19" s="75"/>
+      <c r="N19" s="66"/>
+      <c r="O19" s="66"/>
+      <c r="P19" s="67"/>
+      <c r="Q19" s="68"/>
+      <c r="R19" s="69"/>
+      <c r="S19" s="69"/>
+      <c r="T19" s="69"/>
+      <c r="U19" s="69"/>
+      <c r="V19" s="70"/>
+    </row>
+    <row r="20" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="56">
+        <v>18</v>
+      </c>
+      <c r="B20" s="114"/>
+      <c r="C20" s="115"/>
+      <c r="D20" s="116"/>
+      <c r="E20" s="116"/>
+      <c r="F20" s="116"/>
+      <c r="G20" s="118"/>
+      <c r="H20" s="117"/>
+      <c r="I20" s="117"/>
+      <c r="J20" s="138"/>
+      <c r="K20" s="126"/>
+      <c r="L20" s="116"/>
+      <c r="M20" s="116"/>
+      <c r="N20" s="116"/>
+      <c r="O20" s="116"/>
+      <c r="P20" s="119"/>
+      <c r="Q20" s="120"/>
+      <c r="R20" s="116"/>
+      <c r="S20" s="116"/>
+      <c r="T20" s="116"/>
+      <c r="U20" s="116"/>
+      <c r="V20" s="127"/>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A21" s="63">
+        <v>19</v>
+      </c>
+      <c r="B21" s="108"/>
+      <c r="C21" s="109"/>
+      <c r="D21" s="100"/>
+      <c r="E21" s="101"/>
+      <c r="F21" s="101"/>
+      <c r="G21" s="101"/>
+      <c r="H21" s="101"/>
+      <c r="I21" s="101"/>
+      <c r="J21" s="135"/>
+      <c r="K21" s="142"/>
+      <c r="L21" s="110"/>
+      <c r="M21" s="100"/>
+      <c r="N21" s="101"/>
+      <c r="O21" s="101"/>
+      <c r="P21" s="102"/>
+      <c r="Q21" s="141"/>
+      <c r="R21" s="131"/>
+      <c r="S21" s="131"/>
+      <c r="T21" s="131"/>
+      <c r="U21" s="131"/>
+      <c r="V21" s="132"/>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A22" s="63">
+        <v>20</v>
+      </c>
+      <c r="B22" s="88"/>
+      <c r="C22" s="89"/>
+      <c r="D22" s="75"/>
+      <c r="E22" s="69"/>
+      <c r="F22" s="69"/>
+      <c r="G22" s="69"/>
+      <c r="H22" s="69"/>
+      <c r="I22" s="69"/>
+      <c r="J22" s="84"/>
+      <c r="K22" s="143"/>
+      <c r="L22" s="91"/>
+      <c r="M22" s="69"/>
+      <c r="N22" s="69"/>
+      <c r="O22" s="69"/>
+      <c r="P22" s="87"/>
+      <c r="Q22" s="68"/>
+      <c r="R22" s="69"/>
+      <c r="S22" s="69"/>
+      <c r="T22" s="69"/>
+      <c r="U22" s="69"/>
+      <c r="V22" s="70"/>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A23" s="63">
+        <v>21</v>
+      </c>
+      <c r="B23" s="88"/>
+      <c r="C23" s="89"/>
+      <c r="D23" s="66"/>
+      <c r="E23" s="66"/>
+      <c r="F23" s="66"/>
+      <c r="G23" s="75"/>
+      <c r="H23" s="66"/>
+      <c r="I23" s="66"/>
+      <c r="J23" s="83"/>
+      <c r="K23" s="144"/>
+      <c r="L23" s="90"/>
+      <c r="M23" s="75"/>
+      <c r="N23" s="66"/>
+      <c r="O23" s="66"/>
+      <c r="P23" s="67"/>
+      <c r="Q23" s="68"/>
+      <c r="R23" s="69"/>
+      <c r="S23" s="69"/>
+      <c r="T23" s="69"/>
+      <c r="U23" s="69"/>
+      <c r="V23" s="70"/>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A24" s="63">
+        <v>22</v>
+      </c>
+      <c r="B24" s="88"/>
+      <c r="C24" s="89"/>
+      <c r="D24" s="69"/>
+      <c r="E24" s="69"/>
+      <c r="F24" s="69"/>
+      <c r="G24" s="75"/>
+      <c r="H24" s="69"/>
+      <c r="I24" s="69"/>
+      <c r="J24" s="84"/>
+      <c r="K24" s="143"/>
+      <c r="L24" s="91"/>
+      <c r="M24" s="69"/>
+      <c r="N24" s="69"/>
+      <c r="O24" s="69"/>
+      <c r="P24" s="87"/>
+      <c r="Q24" s="68"/>
+      <c r="R24" s="69"/>
+      <c r="S24" s="69"/>
+      <c r="T24" s="69"/>
+      <c r="U24" s="69"/>
+      <c r="V24" s="70"/>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A25" s="63">
+        <v>23</v>
+      </c>
+      <c r="B25" s="88"/>
+      <c r="C25" s="89"/>
+      <c r="D25" s="66"/>
+      <c r="E25" s="66"/>
+      <c r="F25" s="66"/>
+      <c r="G25" s="66"/>
+      <c r="H25" s="66"/>
+      <c r="I25" s="66"/>
+      <c r="J25" s="136"/>
+      <c r="K25" s="144"/>
+      <c r="L25" s="90"/>
+      <c r="M25" s="75"/>
+      <c r="N25" s="66"/>
+      <c r="O25" s="66"/>
+      <c r="P25" s="67"/>
+      <c r="Q25" s="68"/>
+      <c r="R25" s="69"/>
+      <c r="S25" s="69"/>
+      <c r="T25" s="69"/>
+      <c r="U25" s="69"/>
+      <c r="V25" s="70"/>
+    </row>
+    <row r="26" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="63">
+        <v>24</v>
+      </c>
+      <c r="B26" s="111"/>
+      <c r="C26" s="112"/>
+      <c r="D26" s="72"/>
+      <c r="E26" s="72"/>
+      <c r="F26" s="72"/>
+      <c r="G26" s="106"/>
+      <c r="H26" s="72"/>
+      <c r="I26" s="72"/>
+      <c r="J26" s="137"/>
+      <c r="K26" s="145"/>
+      <c r="L26" s="113"/>
+      <c r="M26" s="72"/>
+      <c r="N26" s="72"/>
+      <c r="O26" s="72"/>
+      <c r="P26" s="107"/>
+      <c r="Q26" s="71"/>
+      <c r="R26" s="72"/>
+      <c r="S26" s="72"/>
+      <c r="T26" s="72"/>
+      <c r="U26" s="72"/>
+      <c r="V26" s="73"/>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A27" s="63">
+        <v>25</v>
+      </c>
+      <c r="B27" s="96"/>
+      <c r="C27" s="97"/>
+      <c r="D27" s="74"/>
+      <c r="E27" s="65"/>
+      <c r="F27" s="65"/>
+      <c r="G27" s="65"/>
+      <c r="H27" s="65"/>
+      <c r="I27" s="65"/>
+      <c r="J27" s="82"/>
+      <c r="K27" s="76"/>
+      <c r="L27" s="65"/>
+      <c r="M27" s="74"/>
+      <c r="N27" s="98"/>
+      <c r="O27" s="98"/>
+      <c r="P27" s="77"/>
+      <c r="Q27" s="124"/>
+      <c r="R27" s="122"/>
+      <c r="S27" s="122"/>
+      <c r="T27" s="122"/>
+      <c r="U27" s="122"/>
+      <c r="V27" s="123"/>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A28" s="63">
+        <v>26</v>
+      </c>
+      <c r="B28" s="88"/>
+      <c r="C28" s="89"/>
+      <c r="D28" s="75"/>
+      <c r="E28" s="69"/>
+      <c r="F28" s="69"/>
+      <c r="G28" s="69"/>
+      <c r="H28" s="69"/>
+      <c r="I28" s="69"/>
+      <c r="J28" s="84"/>
+      <c r="K28" s="79"/>
+      <c r="L28" s="69"/>
+      <c r="M28" s="69"/>
+      <c r="N28" s="91"/>
+      <c r="O28" s="91"/>
+      <c r="P28" s="87"/>
+      <c r="Q28" s="68"/>
+      <c r="R28" s="69"/>
+      <c r="S28" s="69"/>
+      <c r="T28" s="69"/>
+      <c r="U28" s="69"/>
+      <c r="V28" s="70"/>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A29" s="63">
+        <v>27</v>
+      </c>
+      <c r="B29" s="88"/>
+      <c r="C29" s="89"/>
+      <c r="D29" s="66"/>
+      <c r="E29" s="66"/>
+      <c r="F29" s="66"/>
+      <c r="G29" s="75"/>
+      <c r="H29" s="66"/>
+      <c r="I29" s="66"/>
+      <c r="J29" s="83"/>
+      <c r="K29" s="86"/>
+      <c r="L29" s="66"/>
+      <c r="M29" s="75"/>
+      <c r="N29" s="90"/>
+      <c r="O29" s="90"/>
+      <c r="P29" s="67"/>
+      <c r="Q29" s="68"/>
+      <c r="R29" s="69"/>
+      <c r="S29" s="69"/>
+      <c r="T29" s="69"/>
+      <c r="U29" s="69"/>
+      <c r="V29" s="70"/>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A30" s="63">
+        <v>28</v>
+      </c>
+      <c r="B30" s="88"/>
+      <c r="C30" s="89"/>
+      <c r="D30" s="69"/>
+      <c r="E30" s="69"/>
+      <c r="F30" s="69"/>
+      <c r="G30" s="75"/>
+      <c r="H30" s="69"/>
+      <c r="I30" s="69"/>
+      <c r="J30" s="84"/>
+      <c r="K30" s="79"/>
+      <c r="L30" s="69"/>
+      <c r="M30" s="69"/>
+      <c r="N30" s="91"/>
+      <c r="O30" s="91"/>
+      <c r="P30" s="87"/>
+      <c r="Q30" s="68"/>
+      <c r="R30" s="69"/>
+      <c r="S30" s="69"/>
+      <c r="T30" s="69"/>
+      <c r="U30" s="69"/>
+      <c r="V30" s="70"/>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A31" s="63">
+        <v>29</v>
+      </c>
+      <c r="B31" s="88"/>
+      <c r="C31" s="89"/>
+      <c r="D31" s="66"/>
+      <c r="E31" s="66"/>
+      <c r="F31" s="66"/>
+      <c r="G31" s="66"/>
+      <c r="H31" s="66"/>
+      <c r="I31" s="66"/>
+      <c r="J31" s="136"/>
+      <c r="K31" s="86"/>
+      <c r="L31" s="66"/>
+      <c r="M31" s="75"/>
+      <c r="N31" s="90"/>
+      <c r="O31" s="90"/>
+      <c r="P31" s="67"/>
+      <c r="Q31" s="68"/>
+      <c r="R31" s="69"/>
+      <c r="S31" s="69"/>
+      <c r="T31" s="69"/>
+      <c r="U31" s="69"/>
+      <c r="V31" s="70"/>
+    </row>
+    <row r="32" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="63">
+        <v>30</v>
+      </c>
+      <c r="B32" s="114"/>
+      <c r="C32" s="115"/>
+      <c r="D32" s="116"/>
+      <c r="E32" s="116"/>
+      <c r="F32" s="116"/>
+      <c r="G32" s="118"/>
+      <c r="H32" s="116"/>
+      <c r="I32" s="116"/>
+      <c r="J32" s="138"/>
+      <c r="K32" s="126"/>
+      <c r="L32" s="116"/>
+      <c r="M32" s="116"/>
+      <c r="N32" s="117"/>
+      <c r="O32" s="117"/>
+      <c r="P32" s="119"/>
+      <c r="Q32" s="120"/>
+      <c r="R32" s="116"/>
+      <c r="S32" s="116"/>
+      <c r="T32" s="116"/>
+      <c r="U32" s="116"/>
+      <c r="V32" s="127"/>
+    </row>
+    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A33" s="56">
+        <v>31</v>
+      </c>
+      <c r="B33" s="108"/>
+      <c r="C33" s="109"/>
+      <c r="D33" s="131"/>
+      <c r="E33" s="131"/>
+      <c r="F33" s="131"/>
+      <c r="G33" s="101"/>
+      <c r="H33" s="131"/>
+      <c r="I33" s="131"/>
+      <c r="J33" s="139"/>
+      <c r="K33" s="146"/>
+      <c r="L33" s="133"/>
+      <c r="M33" s="133"/>
+      <c r="N33" s="131"/>
+      <c r="O33" s="131"/>
+      <c r="P33" s="132"/>
+      <c r="Q33" s="141"/>
+      <c r="R33" s="131"/>
+      <c r="S33" s="131"/>
+      <c r="T33" s="131"/>
+      <c r="U33" s="131"/>
+      <c r="V33" s="134"/>
+    </row>
+    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A34" s="56">
+        <v>32</v>
+      </c>
+      <c r="B34" s="88"/>
+      <c r="C34" s="89"/>
+      <c r="D34" s="69"/>
+      <c r="E34" s="69"/>
+      <c r="F34" s="69"/>
+      <c r="G34" s="66"/>
+      <c r="H34" s="69"/>
+      <c r="I34" s="69"/>
+      <c r="J34" s="84"/>
+      <c r="K34" s="143"/>
+      <c r="L34" s="91"/>
+      <c r="M34" s="69"/>
+      <c r="N34" s="69"/>
+      <c r="O34" s="69"/>
+      <c r="P34" s="87"/>
+      <c r="Q34" s="68"/>
+      <c r="R34" s="69"/>
+      <c r="S34" s="69"/>
+      <c r="T34" s="69"/>
+      <c r="U34" s="69"/>
+      <c r="V34" s="87"/>
+    </row>
+    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A35" s="56">
+        <v>33</v>
+      </c>
+      <c r="B35" s="79"/>
+      <c r="C35" s="69"/>
+      <c r="D35" s="69"/>
+      <c r="E35" s="69"/>
+      <c r="F35" s="69"/>
+      <c r="G35" s="69"/>
+      <c r="H35" s="69"/>
+      <c r="I35" s="69"/>
+      <c r="J35" s="84"/>
+      <c r="K35" s="79"/>
+      <c r="L35" s="69"/>
+      <c r="M35" s="91"/>
+      <c r="N35" s="91"/>
+      <c r="O35" s="91"/>
+      <c r="P35" s="70"/>
+      <c r="Q35" s="68"/>
+      <c r="R35" s="69"/>
+      <c r="S35" s="69"/>
+      <c r="T35" s="69"/>
+      <c r="U35" s="69"/>
+      <c r="V35" s="87"/>
+    </row>
+    <row r="36" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="56">
+        <v>34</v>
+      </c>
+      <c r="B36" s="80"/>
+      <c r="C36" s="72"/>
+      <c r="D36" s="72"/>
+      <c r="E36" s="72"/>
+      <c r="F36" s="72"/>
+      <c r="G36" s="72"/>
+      <c r="H36" s="72"/>
+      <c r="I36" s="72"/>
+      <c r="J36" s="85"/>
+      <c r="K36" s="80"/>
+      <c r="L36" s="72"/>
+      <c r="M36" s="72"/>
+      <c r="N36" s="113"/>
+      <c r="O36" s="113"/>
+      <c r="P36" s="107"/>
+      <c r="Q36" s="71"/>
+      <c r="R36" s="72"/>
+      <c r="S36" s="72"/>
+      <c r="T36" s="72"/>
+      <c r="U36" s="72"/>
+      <c r="V36" s="107"/>
+    </row>
+    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A37" s="63">
+        <v>35</v>
+      </c>
+      <c r="B37" s="121"/>
+      <c r="C37" s="122"/>
+      <c r="D37" s="122"/>
+      <c r="E37" s="122"/>
+      <c r="F37" s="122"/>
+      <c r="G37" s="122"/>
+      <c r="H37" s="122"/>
+      <c r="I37" s="122"/>
+      <c r="J37" s="125"/>
+      <c r="K37" s="121"/>
+      <c r="L37" s="122"/>
+      <c r="M37" s="122"/>
+      <c r="N37" s="122"/>
+      <c r="O37" s="122"/>
+      <c r="P37" s="123"/>
+      <c r="Q37" s="124"/>
+      <c r="R37" s="122"/>
+      <c r="S37" s="122"/>
+      <c r="T37" s="122"/>
+      <c r="U37" s="122"/>
+      <c r="V37" s="123"/>
+    </row>
+    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A38" s="63">
+        <v>36</v>
+      </c>
+      <c r="B38" s="79"/>
+      <c r="C38" s="69"/>
+      <c r="D38" s="69"/>
+      <c r="E38" s="69"/>
+      <c r="F38" s="69"/>
+      <c r="G38" s="69"/>
+      <c r="H38" s="69"/>
+      <c r="I38" s="69"/>
+      <c r="J38" s="84"/>
+      <c r="K38" s="79"/>
+      <c r="L38" s="69"/>
+      <c r="M38" s="69"/>
+      <c r="N38" s="69"/>
+      <c r="O38" s="69"/>
+      <c r="P38" s="70"/>
+      <c r="Q38" s="68"/>
+      <c r="R38" s="69"/>
+      <c r="S38" s="69"/>
+      <c r="T38" s="69"/>
+      <c r="U38" s="69"/>
+      <c r="V38" s="70"/>
+    </row>
+    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A39" s="63">
+        <v>37</v>
+      </c>
+      <c r="B39" s="79"/>
+      <c r="C39" s="69"/>
+      <c r="D39" s="69"/>
+      <c r="E39" s="69"/>
+      <c r="F39" s="69"/>
+      <c r="G39" s="69"/>
+      <c r="H39" s="69"/>
+      <c r="I39" s="69"/>
+      <c r="J39" s="84"/>
+      <c r="K39" s="79"/>
+      <c r="L39" s="69"/>
+      <c r="M39" s="69"/>
+      <c r="N39" s="69"/>
+      <c r="O39" s="69"/>
+      <c r="P39" s="70"/>
+      <c r="Q39" s="68"/>
+      <c r="R39" s="69"/>
+      <c r="S39" s="69"/>
+      <c r="T39" s="69"/>
+      <c r="U39" s="69"/>
+      <c r="V39" s="70"/>
+    </row>
+    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A40" s="63">
+        <v>38</v>
+      </c>
+      <c r="B40" s="79"/>
+      <c r="C40" s="69"/>
+      <c r="D40" s="69"/>
+      <c r="E40" s="69"/>
+      <c r="F40" s="69"/>
+      <c r="G40" s="69"/>
+      <c r="H40" s="69"/>
+      <c r="I40" s="69"/>
+      <c r="J40" s="84"/>
+      <c r="K40" s="79"/>
+      <c r="L40" s="69"/>
+      <c r="M40" s="69"/>
+      <c r="N40" s="69"/>
+      <c r="O40" s="69"/>
+      <c r="P40" s="70"/>
+      <c r="Q40" s="68"/>
+      <c r="R40" s="69"/>
+      <c r="S40" s="69"/>
+      <c r="T40" s="69"/>
+      <c r="U40" s="69"/>
+      <c r="V40" s="70"/>
+    </row>
+    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A41" s="63">
+        <v>39</v>
+      </c>
+      <c r="B41" s="79"/>
+      <c r="C41" s="69"/>
+      <c r="D41" s="69"/>
+      <c r="E41" s="69"/>
+      <c r="F41" s="69"/>
+      <c r="G41" s="69"/>
+      <c r="H41" s="69"/>
+      <c r="I41" s="69"/>
+      <c r="J41" s="84"/>
+      <c r="K41" s="79"/>
+      <c r="L41" s="69"/>
+      <c r="M41" s="69"/>
+      <c r="N41" s="69"/>
+      <c r="O41" s="69"/>
+      <c r="P41" s="70"/>
+      <c r="Q41" s="68"/>
+      <c r="R41" s="69"/>
+      <c r="S41" s="69"/>
+      <c r="T41" s="69"/>
+      <c r="U41" s="69"/>
+      <c r="V41" s="70"/>
+    </row>
+    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A42" s="63">
+        <v>40</v>
+      </c>
+      <c r="B42" s="79"/>
+      <c r="C42" s="69"/>
+      <c r="D42" s="69"/>
+      <c r="E42" s="69"/>
+      <c r="F42" s="69"/>
+      <c r="G42" s="69"/>
+      <c r="H42" s="69"/>
+      <c r="I42" s="69"/>
+      <c r="J42" s="84"/>
+      <c r="K42" s="79"/>
+      <c r="L42" s="69"/>
+      <c r="M42" s="69"/>
+      <c r="N42" s="69"/>
+      <c r="O42" s="69"/>
+      <c r="P42" s="70"/>
+      <c r="Q42" s="68"/>
+      <c r="R42" s="69"/>
+      <c r="S42" s="69"/>
+      <c r="T42" s="69"/>
+      <c r="U42" s="69"/>
+      <c r="V42" s="70"/>
+    </row>
+    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A43" s="63">
+        <v>41</v>
+      </c>
+      <c r="B43" s="79"/>
+      <c r="C43" s="69"/>
+      <c r="D43" s="69"/>
+      <c r="E43" s="69"/>
+      <c r="F43" s="69"/>
+      <c r="G43" s="69"/>
+      <c r="H43" s="69"/>
+      <c r="I43" s="69"/>
+      <c r="J43" s="84"/>
+      <c r="K43" s="79"/>
+      <c r="L43" s="69"/>
+      <c r="M43" s="69"/>
+      <c r="N43" s="69"/>
+      <c r="O43" s="69"/>
+      <c r="P43" s="70"/>
+      <c r="Q43" s="68"/>
+      <c r="R43" s="69"/>
+      <c r="S43" s="69"/>
+      <c r="T43" s="69"/>
+      <c r="U43" s="69"/>
+      <c r="V43" s="70"/>
+    </row>
+    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A44" s="63">
+        <v>42</v>
+      </c>
+      <c r="B44" s="79"/>
+      <c r="C44" s="69"/>
+      <c r="D44" s="69"/>
+      <c r="E44" s="69"/>
+      <c r="F44" s="69"/>
+      <c r="G44" s="69"/>
+      <c r="H44" s="69"/>
+      <c r="I44" s="69"/>
+      <c r="J44" s="84"/>
+      <c r="K44" s="79"/>
+      <c r="L44" s="69"/>
+      <c r="M44" s="69"/>
+      <c r="N44" s="69"/>
+      <c r="O44" s="69"/>
+      <c r="P44" s="70"/>
+      <c r="Q44" s="68"/>
+      <c r="R44" s="69"/>
+      <c r="S44" s="69"/>
+      <c r="T44" s="69"/>
+      <c r="U44" s="69"/>
+      <c r="V44" s="70"/>
+    </row>
+    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A45" s="63">
+        <v>43</v>
+      </c>
+      <c r="B45" s="79"/>
+      <c r="C45" s="69"/>
+      <c r="D45" s="69"/>
+      <c r="E45" s="69"/>
+      <c r="F45" s="69"/>
+      <c r="G45" s="69"/>
+      <c r="H45" s="69"/>
+      <c r="I45" s="69"/>
+      <c r="J45" s="84"/>
+      <c r="K45" s="79"/>
+      <c r="L45" s="69"/>
+      <c r="M45" s="69"/>
+      <c r="N45" s="69"/>
+      <c r="O45" s="69"/>
+      <c r="P45" s="70"/>
+      <c r="Q45" s="68"/>
+      <c r="R45" s="69"/>
+      <c r="S45" s="69"/>
+      <c r="T45" s="69"/>
+      <c r="U45" s="69"/>
+      <c r="V45" s="70"/>
+    </row>
+    <row r="46" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A46" s="63">
+        <v>44</v>
+      </c>
+      <c r="B46" s="79"/>
+      <c r="C46" s="69"/>
+      <c r="D46" s="69"/>
+      <c r="E46" s="69"/>
+      <c r="F46" s="69"/>
+      <c r="G46" s="69"/>
+      <c r="H46" s="69"/>
+      <c r="I46" s="69"/>
+      <c r="J46" s="84"/>
+      <c r="K46" s="79"/>
+      <c r="L46" s="69"/>
+      <c r="M46" s="69"/>
+      <c r="N46" s="69"/>
+      <c r="O46" s="69"/>
+      <c r="P46" s="70"/>
+      <c r="Q46" s="68"/>
+      <c r="R46" s="69"/>
+      <c r="S46" s="69"/>
+      <c r="T46" s="69"/>
+      <c r="U46" s="69"/>
+      <c r="V46" s="70"/>
+    </row>
+    <row r="47" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A47" s="63">
+        <v>45</v>
+      </c>
+      <c r="B47" s="79"/>
+      <c r="C47" s="69"/>
+      <c r="D47" s="69"/>
+      <c r="E47" s="69"/>
+      <c r="F47" s="69"/>
+      <c r="G47" s="69"/>
+      <c r="H47" s="69"/>
+      <c r="I47" s="69"/>
+      <c r="J47" s="84"/>
+      <c r="K47" s="79"/>
+      <c r="L47" s="69"/>
+      <c r="M47" s="69"/>
+      <c r="N47" s="69"/>
+      <c r="O47" s="69"/>
+      <c r="P47" s="70"/>
+      <c r="Q47" s="68"/>
+      <c r="R47" s="69"/>
+      <c r="S47" s="69"/>
+      <c r="T47" s="69"/>
+      <c r="U47" s="69"/>
+      <c r="V47" s="70"/>
+    </row>
+    <row r="48" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A48" s="63">
+        <v>46</v>
+      </c>
+      <c r="B48" s="79"/>
+      <c r="C48" s="69"/>
+      <c r="D48" s="69"/>
+      <c r="E48" s="69"/>
+      <c r="F48" s="69"/>
+      <c r="G48" s="69"/>
+      <c r="H48" s="69"/>
+      <c r="I48" s="69"/>
+      <c r="J48" s="84"/>
+      <c r="K48" s="79"/>
+      <c r="L48" s="69"/>
+      <c r="M48" s="69"/>
+      <c r="N48" s="69"/>
+      <c r="O48" s="69"/>
+      <c r="P48" s="70"/>
+      <c r="Q48" s="68"/>
+      <c r="R48" s="69"/>
+      <c r="S48" s="69"/>
+      <c r="T48" s="69"/>
+      <c r="U48" s="69"/>
+      <c r="V48" s="70"/>
+    </row>
+    <row r="49" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A49" s="63">
+        <v>47</v>
+      </c>
+      <c r="B49" s="79"/>
+      <c r="C49" s="69"/>
+      <c r="D49" s="69"/>
+      <c r="E49" s="69"/>
+      <c r="F49" s="69"/>
+      <c r="G49" s="69"/>
+      <c r="H49" s="69"/>
+      <c r="I49" s="69"/>
+      <c r="J49" s="84"/>
+      <c r="K49" s="79"/>
+      <c r="L49" s="69"/>
+      <c r="M49" s="69"/>
+      <c r="N49" s="69"/>
+      <c r="O49" s="69"/>
+      <c r="P49" s="70"/>
+      <c r="Q49" s="68"/>
+      <c r="R49" s="69"/>
+      <c r="S49" s="69"/>
+      <c r="T49" s="69"/>
+      <c r="U49" s="69"/>
+      <c r="V49" s="70"/>
+    </row>
+    <row r="50" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A50" s="63">
+        <v>48</v>
+      </c>
+      <c r="B50" s="79"/>
+      <c r="C50" s="69"/>
+      <c r="D50" s="69"/>
+      <c r="E50" s="69"/>
+      <c r="F50" s="69"/>
+      <c r="G50" s="69"/>
+      <c r="H50" s="69"/>
+      <c r="I50" s="69"/>
+      <c r="J50" s="84"/>
+      <c r="K50" s="79"/>
+      <c r="L50" s="69"/>
+      <c r="M50" s="69"/>
+      <c r="N50" s="69"/>
+      <c r="O50" s="69"/>
+      <c r="P50" s="70"/>
+      <c r="Q50" s="68"/>
+      <c r="R50" s="69"/>
+      <c r="S50" s="69"/>
+      <c r="T50" s="69"/>
+      <c r="U50" s="69"/>
+      <c r="V50" s="70"/>
+    </row>
+    <row r="51" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A51" s="63">
+        <v>49</v>
+      </c>
+      <c r="B51" s="79"/>
+      <c r="C51" s="69"/>
+      <c r="D51" s="69"/>
+      <c r="E51" s="69"/>
+      <c r="F51" s="69"/>
+      <c r="G51" s="69"/>
+      <c r="H51" s="69"/>
+      <c r="I51" s="69"/>
+      <c r="J51" s="84"/>
+      <c r="K51" s="79"/>
+      <c r="L51" s="69"/>
+      <c r="M51" s="69"/>
+      <c r="N51" s="69"/>
+      <c r="O51" s="69"/>
+      <c r="P51" s="70"/>
+      <c r="Q51" s="68"/>
+      <c r="R51" s="69"/>
+      <c r="S51" s="69"/>
+      <c r="T51" s="69"/>
+      <c r="U51" s="69"/>
+      <c r="V51" s="70"/>
+    </row>
+    <row r="52" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="64">
+        <v>50</v>
+      </c>
+      <c r="B52" s="80"/>
+      <c r="C52" s="72"/>
+      <c r="D52" s="72"/>
+      <c r="E52" s="72"/>
+      <c r="F52" s="72"/>
+      <c r="G52" s="72"/>
+      <c r="H52" s="72"/>
+      <c r="I52" s="72"/>
+      <c r="J52" s="85"/>
+      <c r="K52" s="80"/>
+      <c r="L52" s="72"/>
+      <c r="M52" s="72"/>
+      <c r="N52" s="72"/>
+      <c r="O52" s="72"/>
+      <c r="P52" s="73"/>
+      <c r="Q52" s="71"/>
+      <c r="R52" s="72"/>
+      <c r="S52" s="72"/>
+      <c r="T52" s="72"/>
+      <c r="U52" s="72"/>
+      <c r="V52" s="73"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFD97391-339B-4313-8D6D-883D8A38F360}">
+  <dimension ref="A1:I16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G13" sqref="G13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>37</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>69</v>
+        <v>42</v>
       </c>
       <c r="C1" s="16" t="s">
         <v>39</v>
@@ -1632,19 +3462,19 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="10">
+      <c r="A2" s="29">
         <v>1</v>
       </c>
-      <c r="B2" s="26" t="s">
-        <v>70</v>
-      </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="12"/>
-      <c r="G2" s="56" t="s">
+      <c r="B2" s="51" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="31"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="22"/>
+      <c r="G2" s="147" t="s">
         <v>52</v>
       </c>
-      <c r="H2" s="57"/>
+      <c r="H2" s="148"/>
       <c r="I2" s="22"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1652,15 +3482,15 @@
         <v>2</v>
       </c>
       <c r="B3" s="27" t="s">
-        <v>71</v>
+        <v>44</v>
       </c>
       <c r="C3" s="18"/>
-      <c r="D3" s="4"/>
+      <c r="D3" s="25"/>
       <c r="E3" s="6"/>
-      <c r="G3" s="58" t="s">
+      <c r="G3" s="149" t="s">
         <v>54</v>
       </c>
-      <c r="H3" s="59"/>
+      <c r="H3" s="150"/>
       <c r="I3" s="23"/>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1668,15 +3498,15 @@
         <v>3</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>72</v>
+        <v>45</v>
       </c>
       <c r="C4" s="18"/>
-      <c r="D4" s="4"/>
+      <c r="D4" s="25"/>
       <c r="E4" s="6"/>
-      <c r="G4" s="60" t="s">
+      <c r="G4" s="151" t="s">
         <v>53</v>
       </c>
-      <c r="H4" s="61"/>
+      <c r="H4" s="152"/>
       <c r="I4" s="24"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -1684,11 +3514,132 @@
         <v>4</v>
       </c>
       <c r="B5" s="27" t="s">
-        <v>73</v>
+        <v>46</v>
       </c>
       <c r="C5" s="18"/>
-      <c r="D5" s="4"/>
+      <c r="D5" s="25"/>
       <c r="E5" s="6"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
+        <v>5</v>
+      </c>
+      <c r="B6" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="18"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="6"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
+        <v>6</v>
+      </c>
+      <c r="B7" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="18"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="6"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
+        <v>7</v>
+      </c>
+      <c r="B8" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" s="18"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="6"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <v>8</v>
+      </c>
+      <c r="B9" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" s="18"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="6"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
+        <v>9</v>
+      </c>
+      <c r="B10" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="C10" s="18"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="6"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
+        <v>10</v>
+      </c>
+      <c r="B11" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" s="18"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="6"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
+        <v>11</v>
+      </c>
+      <c r="B12" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="18"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="6"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="5">
+        <v>12</v>
+      </c>
+      <c r="B13" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" s="18"/>
+      <c r="D13" s="53"/>
+      <c r="E13" s="6"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="5">
+        <v>13</v>
+      </c>
+      <c r="B14" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="C14" s="18"/>
+      <c r="D14" s="53"/>
+      <c r="E14" s="6"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="5">
+        <v>14</v>
+      </c>
+      <c r="B15" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="C15" s="18"/>
+      <c r="D15" s="53"/>
+      <c r="E15" s="6"/>
+    </row>
+    <row r="16" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="7">
+        <v>15</v>
+      </c>
+      <c r="B16" s="52" t="s">
+        <v>90</v>
+      </c>
+      <c r="C16" s="19"/>
+      <c r="D16" s="54"/>
+      <c r="E16" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1701,6 +3652,372 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0761546C-2124-4D87-9532-0ECA1AEF2C0F}">
+  <dimension ref="A1:I5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H35" sqref="H35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="10">
+        <v>1</v>
+      </c>
+      <c r="B2" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="17"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="12"/>
+      <c r="G2" s="147" t="s">
+        <v>52</v>
+      </c>
+      <c r="H2" s="148"/>
+      <c r="I2" s="22"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>2</v>
+      </c>
+      <c r="B3" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" s="18"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="6"/>
+      <c r="G3" s="149" t="s">
+        <v>54</v>
+      </c>
+      <c r="H3" s="150"/>
+      <c r="I3" s="23"/>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="5">
+        <v>3</v>
+      </c>
+      <c r="B4" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4" s="18"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="6"/>
+      <c r="G4" s="151" t="s">
+        <v>53</v>
+      </c>
+      <c r="H4" s="152"/>
+      <c r="I4" s="24"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="C5" s="18"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="6"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="G4:H4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC5846F4-5620-4E75-AD36-23EC709DF9B6}">
+  <dimension ref="A1:I10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J21" sqref="J21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="31.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2" s="18"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="6"/>
+      <c r="G2" s="147" t="s">
+        <v>52</v>
+      </c>
+      <c r="H2" s="148"/>
+      <c r="I2" s="22"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>2</v>
+      </c>
+      <c r="B3" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="C3" s="18"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="6"/>
+      <c r="G3" s="149" t="s">
+        <v>54</v>
+      </c>
+      <c r="H3" s="150"/>
+      <c r="I3" s="23"/>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="5">
+        <v>3</v>
+      </c>
+      <c r="B4" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="C4" s="18"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="6"/>
+      <c r="G4" s="151" t="s">
+        <v>53</v>
+      </c>
+      <c r="H4" s="152"/>
+      <c r="I4" s="24"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="27" t="s">
+        <v>114</v>
+      </c>
+      <c r="C5" s="18"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="6"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
+        <v>5</v>
+      </c>
+      <c r="B6" s="27" t="s">
+        <v>113</v>
+      </c>
+      <c r="C6" s="18"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="6"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
+        <v>6</v>
+      </c>
+      <c r="B7" s="27" t="s">
+        <v>115</v>
+      </c>
+      <c r="C7" s="18"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="6"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
+        <v>7</v>
+      </c>
+      <c r="B8" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="C8" s="18"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="6"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <v>8</v>
+      </c>
+      <c r="B9" s="27" t="s">
+        <v>117</v>
+      </c>
+      <c r="C9" s="18"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="6"/>
+    </row>
+    <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="7">
+        <v>9</v>
+      </c>
+      <c r="B10" s="28" t="s">
+        <v>118</v>
+      </c>
+      <c r="C10" s="19"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="9"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="G4:H4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4BC8A56-D40A-4F65-87E5-EA0E881CA0D3}">
+  <dimension ref="A1:I6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G34" sqref="G34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="10">
+        <v>1</v>
+      </c>
+      <c r="B2" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2" s="17"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="12"/>
+      <c r="G2" s="147" t="s">
+        <v>52</v>
+      </c>
+      <c r="H2" s="148"/>
+      <c r="I2" s="22"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>2</v>
+      </c>
+      <c r="B3" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="C3" s="18"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="6"/>
+      <c r="G3" s="149" t="s">
+        <v>54</v>
+      </c>
+      <c r="H3" s="150"/>
+      <c r="I3" s="23"/>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="5">
+        <v>3</v>
+      </c>
+      <c r="B4" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="C4" s="18"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="6"/>
+      <c r="G4" s="151" t="s">
+        <v>53</v>
+      </c>
+      <c r="H4" s="152"/>
+      <c r="I4" s="24"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="27" t="s">
+        <v>86</v>
+      </c>
+      <c r="C5" s="18"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="6"/>
+    </row>
+    <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="7">
+        <v>5</v>
+      </c>
+      <c r="B6" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="C6" s="19"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="9"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="G4:H4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D049C773-2D95-45A8-A9FA-3F365D74E40B}">
   <dimension ref="A1:J11"/>
   <sheetViews>
@@ -1739,7 +4056,7 @@
       <c r="A2" s="49">
         <v>1</v>
       </c>
-      <c r="B2" s="62" t="s">
+      <c r="B2" s="153" t="s">
         <v>65</v>
       </c>
       <c r="C2" s="50" t="s">
@@ -1748,51 +4065,51 @@
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
       <c r="F2" s="12"/>
-      <c r="H2" s="56" t="s">
+      <c r="H2" s="147" t="s">
         <v>52</v>
       </c>
-      <c r="I2" s="57"/>
+      <c r="I2" s="148"/>
       <c r="J2" s="22"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="42">
         <v>2</v>
       </c>
-      <c r="B3" s="63"/>
+      <c r="B3" s="154"/>
       <c r="C3" s="44" t="s">
         <v>59</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="F3" s="6"/>
-      <c r="H3" s="58" t="s">
+      <c r="H3" s="149" t="s">
         <v>54</v>
       </c>
-      <c r="I3" s="59"/>
+      <c r="I3" s="150"/>
       <c r="J3" s="23"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="42">
         <v>3</v>
       </c>
-      <c r="B4" s="63"/>
+      <c r="B4" s="154"/>
       <c r="C4" s="44" t="s">
         <v>60</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="6"/>
-      <c r="H4" s="60" t="s">
+      <c r="H4" s="151" t="s">
         <v>53</v>
       </c>
-      <c r="I4" s="61"/>
+      <c r="I4" s="152"/>
       <c r="J4" s="24"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="42">
         <v>4</v>
       </c>
-      <c r="B5" s="63"/>
+      <c r="B5" s="154"/>
       <c r="C5" s="44" t="s">
         <v>61</v>
       </c>
@@ -1804,7 +4121,7 @@
       <c r="A6" s="42">
         <v>5</v>
       </c>
-      <c r="B6" s="63"/>
+      <c r="B6" s="154"/>
       <c r="C6" s="44" t="s">
         <v>62</v>
       </c>
@@ -1816,7 +4133,7 @@
       <c r="A7" s="42">
         <v>6</v>
       </c>
-      <c r="B7" s="63"/>
+      <c r="B7" s="154"/>
       <c r="C7" s="44" t="s">
         <v>63</v>
       </c>
@@ -1828,7 +4145,7 @@
       <c r="A8" s="42">
         <v>7</v>
       </c>
-      <c r="B8" s="63"/>
+      <c r="B8" s="154"/>
       <c r="C8" s="44" t="s">
         <v>81</v>
       </c>
@@ -1883,290 +4200,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC5846F4-5620-4E75-AD36-23EC709DF9B6}">
-  <dimension ref="A1:I11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G2" sqref="G2:I4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="31.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="B1" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="C1" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="D1" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="E1" s="15" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="29">
-        <v>1</v>
-      </c>
-      <c r="B2" s="51" t="s">
-        <v>119</v>
-      </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="22"/>
-      <c r="G2" s="56" t="s">
-        <v>52</v>
-      </c>
-      <c r="H2" s="57"/>
-      <c r="I2" s="22"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
-        <v>2</v>
-      </c>
-      <c r="B3" s="27" t="s">
-        <v>110</v>
-      </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="6"/>
-      <c r="G3" s="58" t="s">
-        <v>54</v>
-      </c>
-      <c r="H3" s="59"/>
-      <c r="I3" s="23"/>
-    </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="5">
-        <v>3</v>
-      </c>
-      <c r="B4" s="27" t="s">
-        <v>111</v>
-      </c>
-      <c r="C4" s="18"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="6"/>
-      <c r="G4" s="60" t="s">
-        <v>53</v>
-      </c>
-      <c r="H4" s="61"/>
-      <c r="I4" s="24"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
-        <v>4</v>
-      </c>
-      <c r="B5" s="27" t="s">
-        <v>112</v>
-      </c>
-      <c r="C5" s="18"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="6"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
-        <v>5</v>
-      </c>
-      <c r="B6" s="27" t="s">
-        <v>114</v>
-      </c>
-      <c r="C6" s="18"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="6"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
-        <v>6</v>
-      </c>
-      <c r="B7" s="27" t="s">
-        <v>113</v>
-      </c>
-      <c r="C7" s="18"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="6"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
-        <v>7</v>
-      </c>
-      <c r="B8" s="27" t="s">
-        <v>115</v>
-      </c>
-      <c r="C8" s="18"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="6"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
-        <v>8</v>
-      </c>
-      <c r="B9" s="27" t="s">
-        <v>116</v>
-      </c>
-      <c r="C9" s="18"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="6"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
-        <v>9</v>
-      </c>
-      <c r="B10" s="27" t="s">
-        <v>117</v>
-      </c>
-      <c r="C10" s="18"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="6"/>
-    </row>
-    <row r="11" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="7">
-        <v>10</v>
-      </c>
-      <c r="B11" s="28" t="s">
-        <v>118</v>
-      </c>
-      <c r="C11" s="19"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="9"/>
-    </row>
-  </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="G4:H4"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4BC8A56-D40A-4F65-87E5-EA0E881CA0D3}">
-  <dimension ref="A1:I6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G2" sqref="G2:I4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="B1" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="C1" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="D1" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="E1" s="15" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="10">
-        <v>1</v>
-      </c>
-      <c r="B2" s="26" t="s">
-        <v>84</v>
-      </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="12"/>
-      <c r="G2" s="56" t="s">
-        <v>52</v>
-      </c>
-      <c r="H2" s="57"/>
-      <c r="I2" s="22"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
-        <v>2</v>
-      </c>
-      <c r="B3" s="27" t="s">
-        <v>83</v>
-      </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="6"/>
-      <c r="G3" s="58" t="s">
-        <v>54</v>
-      </c>
-      <c r="H3" s="59"/>
-      <c r="I3" s="23"/>
-    </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="5">
-        <v>3</v>
-      </c>
-      <c r="B4" s="27" t="s">
-        <v>85</v>
-      </c>
-      <c r="C4" s="18"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="6"/>
-      <c r="G4" s="60" t="s">
-        <v>53</v>
-      </c>
-      <c r="H4" s="61"/>
-      <c r="I4" s="24"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
-        <v>4</v>
-      </c>
-      <c r="B5" s="27" t="s">
-        <v>86</v>
-      </c>
-      <c r="C5" s="18"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="6"/>
-    </row>
-    <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="7">
-        <v>5</v>
-      </c>
-      <c r="B6" s="28" t="s">
-        <v>87</v>
-      </c>
-      <c r="C6" s="19"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="9"/>
-    </row>
-  </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="G4:H4"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9A2992A-FC23-4018-88DA-5C212CD73515}">
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M16" sqref="M16"/>
+      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2201,10 +4241,10 @@
       <c r="C2" s="17"/>
       <c r="D2" s="55"/>
       <c r="E2" s="12"/>
-      <c r="G2" s="56" t="s">
+      <c r="G2" s="147" t="s">
         <v>52</v>
       </c>
-      <c r="H2" s="57"/>
+      <c r="H2" s="148"/>
       <c r="I2" s="22"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -2217,10 +4257,10 @@
       <c r="C3" s="18"/>
       <c r="D3" s="25"/>
       <c r="E3" s="6"/>
-      <c r="G3" s="58" t="s">
+      <c r="G3" s="149" t="s">
         <v>54</v>
       </c>
-      <c r="H3" s="59"/>
+      <c r="H3" s="150"/>
       <c r="I3" s="23"/>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2233,10 +4273,10 @@
       <c r="C4" s="18"/>
       <c r="D4" s="4"/>
       <c r="E4" s="6"/>
-      <c r="G4" s="60" t="s">
+      <c r="G4" s="151" t="s">
         <v>53</v>
       </c>
-      <c r="H4" s="61"/>
+      <c r="H4" s="152"/>
       <c r="I4" s="24"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -2271,161 +4311,6 @@
       <c r="C7" s="19"/>
       <c r="D7" s="8"/>
       <c r="E7" s="9"/>
-    </row>
-  </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="G4:H4"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1683BD35-68D1-40C8-810D-7B22B62F74CE}">
-  <dimension ref="A1:I10"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F33" sqref="F33"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="B1" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="C1" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="D1" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="E1" s="15" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="29">
-        <v>1</v>
-      </c>
-      <c r="B2" s="51" t="s">
-        <v>92</v>
-      </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="22"/>
-      <c r="G2" s="56" t="s">
-        <v>52</v>
-      </c>
-      <c r="H2" s="57"/>
-      <c r="I2" s="22"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
-        <v>2</v>
-      </c>
-      <c r="B3" s="27" t="s">
-        <v>93</v>
-      </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="6"/>
-      <c r="G3" s="58" t="s">
-        <v>54</v>
-      </c>
-      <c r="H3" s="59"/>
-      <c r="I3" s="23"/>
-    </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="5">
-        <v>3</v>
-      </c>
-      <c r="B4" s="27" t="s">
-        <v>94</v>
-      </c>
-      <c r="C4" s="18"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="6"/>
-      <c r="G4" s="60" t="s">
-        <v>53</v>
-      </c>
-      <c r="H4" s="61"/>
-      <c r="I4" s="24"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
-        <v>4</v>
-      </c>
-      <c r="B5" s="27" t="s">
-        <v>96</v>
-      </c>
-      <c r="C5" s="18"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="6"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
-        <v>5</v>
-      </c>
-      <c r="B6" s="27" t="s">
-        <v>95</v>
-      </c>
-      <c r="C6" s="18"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="6"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
-        <v>6</v>
-      </c>
-      <c r="B7" s="27" t="s">
-        <v>97</v>
-      </c>
-      <c r="C7" s="18"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="6"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
-        <v>7</v>
-      </c>
-      <c r="B8" s="27" t="s">
-        <v>98</v>
-      </c>
-      <c r="C8" s="18"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="6"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
-        <v>8</v>
-      </c>
-      <c r="B9" s="27" t="s">
-        <v>99</v>
-      </c>
-      <c r="C9" s="18"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="6"/>
-    </row>
-    <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="7">
-        <v>9</v>
-      </c>
-      <c r="B10" s="28" t="s">
-        <v>100</v>
-      </c>
-      <c r="C10" s="19"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2438,22 +4323,25 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFD97391-339B-4313-8D6D-883D8A38F360}">
-  <dimension ref="A1:I16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1683BD35-68D1-40C8-810D-7B22B62F74CE}">
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H30" sqref="H30"/>
+      <selection pane="bottomLeft" activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>37</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>42</v>
+        <v>91</v>
       </c>
       <c r="C1" s="16" t="s">
         <v>39</v>
@@ -2470,15 +4358,15 @@
         <v>1</v>
       </c>
       <c r="B2" s="51" t="s">
-        <v>43</v>
+        <v>92</v>
       </c>
       <c r="C2" s="31"/>
       <c r="D2" s="35"/>
       <c r="E2" s="22"/>
-      <c r="G2" s="56" t="s">
+      <c r="G2" s="147" t="s">
         <v>52</v>
       </c>
-      <c r="H2" s="57"/>
+      <c r="H2" s="148"/>
       <c r="I2" s="22"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -2486,15 +4374,15 @@
         <v>2</v>
       </c>
       <c r="B3" s="27" t="s">
-        <v>44</v>
+        <v>93</v>
       </c>
       <c r="C3" s="18"/>
-      <c r="D3" s="25"/>
+      <c r="D3" s="4"/>
       <c r="E3" s="6"/>
-      <c r="G3" s="58" t="s">
+      <c r="G3" s="149" t="s">
         <v>54</v>
       </c>
-      <c r="H3" s="59"/>
+      <c r="H3" s="150"/>
       <c r="I3" s="23"/>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2502,15 +4390,15 @@
         <v>3</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>45</v>
+        <v>94</v>
       </c>
       <c r="C4" s="18"/>
       <c r="D4" s="25"/>
       <c r="E4" s="6"/>
-      <c r="G4" s="60" t="s">
+      <c r="G4" s="151" t="s">
         <v>53</v>
       </c>
-      <c r="H4" s="61"/>
+      <c r="H4" s="152"/>
       <c r="I4" s="24"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -2518,10 +4406,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="27" t="s">
-        <v>46</v>
+        <v>96</v>
       </c>
       <c r="C5" s="18"/>
-      <c r="D5" s="25"/>
+      <c r="D5" s="4"/>
       <c r="E5" s="6"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -2529,10 +4417,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="27" t="s">
-        <v>48</v>
+        <v>95</v>
       </c>
       <c r="C6" s="18"/>
-      <c r="D6" s="25"/>
+      <c r="D6" s="4"/>
       <c r="E6" s="6"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -2540,10 +4428,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="27" t="s">
-        <v>47</v>
+        <v>97</v>
       </c>
       <c r="C7" s="18"/>
-      <c r="D7" s="25"/>
+      <c r="D7" s="4"/>
       <c r="E7" s="6"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -2551,10 +4439,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="27" t="s">
-        <v>55</v>
+        <v>98</v>
       </c>
       <c r="C8" s="18"/>
-      <c r="D8" s="25"/>
+      <c r="D8" s="4"/>
       <c r="E8" s="6"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -2562,88 +4450,22 @@
         <v>8</v>
       </c>
       <c r="B9" s="27" t="s">
-        <v>56</v>
+        <v>99</v>
       </c>
       <c r="C9" s="18"/>
       <c r="D9" s="4"/>
       <c r="E9" s="6"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
+    <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="7">
         <v>9</v>
       </c>
-      <c r="B10" s="27" t="s">
-        <v>101</v>
-      </c>
-      <c r="C10" s="18"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="6"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
-        <v>10</v>
-      </c>
-      <c r="B11" s="27" t="s">
-        <v>50</v>
-      </c>
-      <c r="C11" s="18"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="6"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="5">
-        <v>11</v>
-      </c>
-      <c r="B12" s="27" t="s">
-        <v>51</v>
-      </c>
-      <c r="C12" s="18"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="6"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="5">
-        <v>12</v>
-      </c>
-      <c r="B13" s="27" t="s">
-        <v>49</v>
-      </c>
-      <c r="C13" s="18"/>
-      <c r="D13" s="53"/>
-      <c r="E13" s="6"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="5">
-        <v>13</v>
-      </c>
-      <c r="B14" s="27" t="s">
-        <v>88</v>
-      </c>
-      <c r="C14" s="18"/>
-      <c r="D14" s="53"/>
-      <c r="E14" s="6"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="5">
-        <v>14</v>
-      </c>
-      <c r="B15" s="27" t="s">
-        <v>89</v>
-      </c>
-      <c r="C15" s="18"/>
-      <c r="D15" s="53"/>
-      <c r="E15" s="6"/>
-    </row>
-    <row r="16" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="7">
-        <v>15</v>
-      </c>
-      <c r="B16" s="52" t="s">
-        <v>90</v>
-      </c>
-      <c r="C16" s="19"/>
-      <c r="D16" s="54"/>
-      <c r="E16" s="9"/>
+      <c r="B10" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="C10" s="19"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2660,7 +4482,7 @@
   <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2670,7 +4492,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="64" t="s">
+      <c r="A1" s="155" t="s">
         <v>33</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -2679,15 +4501,15 @@
       <c r="C1" s="1"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="64"/>
+      <c r="A2" s="155"/>
       <c r="B2" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C2" s="1"/>
-      <c r="D2" s="56" t="s">
+      <c r="D2" s="147" t="s">
         <v>52</v>
       </c>
-      <c r="E2" s="57"/>
+      <c r="E2" s="148"/>
       <c r="F2" s="22"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -2696,10 +4518,10 @@
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="58" t="s">
+      <c r="D3" s="149" t="s">
         <v>54</v>
       </c>
-      <c r="E3" s="59"/>
+      <c r="E3" s="150"/>
       <c r="F3" s="23"/>
     </row>
     <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2708,10 +4530,10 @@
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="1"/>
-      <c r="D4" s="60" t="s">
+      <c r="D4" s="151" t="s">
         <v>53</v>
       </c>
-      <c r="E4" s="61"/>
+      <c r="E4" s="152"/>
       <c r="F4" s="24"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -2722,113 +4544,113 @@
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="64" t="s">
+      <c r="A6" s="155" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C6" s="1"/>
-      <c r="K6" s="65" t="s">
+      <c r="K6" s="156" t="s">
         <v>32</v>
       </c>
-      <c r="L6" s="65"/>
+      <c r="L6" s="156"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="64"/>
+      <c r="A7" s="155"/>
       <c r="B7" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C7" s="1"/>
-      <c r="K7" s="65"/>
-      <c r="L7" s="65"/>
+      <c r="K7" s="156"/>
+      <c r="L7" s="156"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="64"/>
+      <c r="A8" s="155"/>
       <c r="B8" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C8" s="1"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="64"/>
+      <c r="A9" s="155"/>
       <c r="B9" s="2" t="s">
         <v>20</v>
       </c>
       <c r="C9" s="1"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="64"/>
+      <c r="A10" s="155"/>
       <c r="B10" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C10" s="1"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="64"/>
+      <c r="A11" s="155"/>
       <c r="B11" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C11" s="1"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="64"/>
+      <c r="A12" s="155"/>
       <c r="B12" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C12" s="1"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="64"/>
+      <c r="A13" s="155"/>
       <c r="B13" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C13" s="1"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="64"/>
+      <c r="A14" s="155"/>
       <c r="B14" s="2" t="s">
         <v>24</v>
       </c>
       <c r="C14" s="1"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="64"/>
+      <c r="A15" s="155"/>
       <c r="B15" s="2" t="s">
         <v>25</v>
       </c>
       <c r="C15" s="1"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="64"/>
+      <c r="A16" s="155"/>
       <c r="B16" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C16" s="1"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="64"/>
+      <c r="A17" s="155"/>
       <c r="B17" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C17" s="1"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="64"/>
+      <c r="A18" s="155"/>
       <c r="B18" s="2" t="s">
         <v>28</v>
       </c>
       <c r="C18" s="1"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="64"/>
+      <c r="A19" s="155"/>
       <c r="B19" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C19" s="1"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="64"/>
+      <c r="A20" s="155"/>
       <c r="B20" s="2" t="s">
         <v>30</v>
       </c>
@@ -2842,7 +4664,7 @@
       <c r="C21" s="1"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="64" t="s">
+      <c r="A22" s="155" t="s">
         <v>9</v>
       </c>
       <c r="B22" s="2" t="s">
@@ -2853,7 +4675,7 @@
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="64"/>
+      <c r="A23" s="155"/>
       <c r="B23" s="2" t="s">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
added flight control system hardware architecture
</commit_message>
<xml_diff>
--- a/Library_architecture.xlsx
+++ b/Library_architecture.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ssipvtltd-my.sharepoint.com/personal/abhinay_singh_ssinnovations_org/Documents/Abhinay's Workspace/main x/GitHub Repo/Repository_architecture/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ssipvtltd-my.sharepoint.com/personal/abhinay_singh_ssinnovations_org/Documents/Abhinay's Workspace/GitHub Repo/Repository_architecture/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1596" documentId="13_ncr:1_{D84D0752-E4BB-48DB-83F5-1B8FFA54D692}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{000EC04E-880C-40F9-8A8D-0211F1E3B859}"/>
+  <xr:revisionPtr revIDLastSave="1624" documentId="13_ncr:1_{D84D0752-E4BB-48DB-83F5-1B8FFA54D692}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{44518E92-B031-4EDE-99B4-E1CC2A7A436D}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="11" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="4" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Control system" sheetId="5" r:id="rId1"/>
@@ -23,14 +23,12 @@
     <sheet name="Constants" sheetId="4" r:id="rId8"/>
     <sheet name="Math" sheetId="2" r:id="rId9"/>
     <sheet name="Aerial vehicle" sheetId="11" r:id="rId10"/>
-    <sheet name="Aerial vehicle-2" sheetId="12" r:id="rId11"/>
-    <sheet name="System architecture" sheetId="13" r:id="rId12"/>
-    <sheet name="Flight stack" sheetId="14" r:id="rId13"/>
-    <sheet name="Estimation layer" sheetId="15" r:id="rId14"/>
-    <sheet name="Control layer" sheetId="16" r:id="rId15"/>
-    <sheet name="Vehicle FCS" sheetId="17" r:id="rId16"/>
-    <sheet name="Vehicle FMS" sheetId="18" r:id="rId17"/>
-    <sheet name="Health monitoring and safety" sheetId="19" r:id="rId18"/>
+    <sheet name="Sheet1" sheetId="20" r:id="rId11"/>
+    <sheet name="Aerial vehicle-2" sheetId="12" r:id="rId12"/>
+    <sheet name="System architecture" sheetId="13" r:id="rId13"/>
+    <sheet name="Vehicle FCS" sheetId="17" r:id="rId14"/>
+    <sheet name="Vehicle FMS" sheetId="18" r:id="rId15"/>
+    <sheet name="Health monitoring and safety" sheetId="19" r:id="rId16"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -53,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="287">
   <si>
     <t>Sr. No.</t>
   </si>
@@ -736,9 +734,6 @@
     <t>Buck converter</t>
   </si>
   <si>
-    <t>Complex umber</t>
-  </si>
-  <si>
     <t>Algebra</t>
   </si>
   <si>
@@ -914,6 +909,9 @@
   </si>
   <si>
     <t>TTL</t>
+  </si>
+  <si>
+    <t>SONAR</t>
   </si>
 </sst>
 </file>
@@ -979,7 +977,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1037,6 +1035,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="52">
     <border>
@@ -1720,7 +1724,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="181">
+  <cellXfs count="182">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2038,6 +2042,9 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2095,25 +2102,25 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="50" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="50" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2409,7 +2416,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O9" sqref="O9:P21"/>
+      <selection pane="bottomLeft" activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2452,10 +2459,10 @@
       <c r="F2" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="155" t="s">
+      <c r="H2" s="156" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="156"/>
+      <c r="I2" s="157"/>
       <c r="J2" s="22"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -2471,10 +2478,10 @@
       <c r="F3" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="157" t="s">
+      <c r="H3" s="158" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="158"/>
+      <c r="I3" s="159"/>
       <c r="J3" s="23"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2490,10 +2497,10 @@
       <c r="F4" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="159" t="s">
+      <c r="H4" s="160" t="s">
         <v>12</v>
       </c>
-      <c r="I4" s="160"/>
+      <c r="I4" s="161"/>
       <c r="J4" s="24"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -2653,7 +2660,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P32" sqref="P32"/>
+      <selection pane="bottomLeft" activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2668,19 +2675,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="169" t="s">
+      <c r="A1" s="170" t="s">
         <v>119</v>
       </c>
-      <c r="B1" s="171" t="s">
+      <c r="B1" s="172" t="s">
         <v>120</v>
       </c>
-      <c r="C1" s="171"/>
-      <c r="D1" s="172"/>
-      <c r="E1" s="171" t="s">
+      <c r="C1" s="172"/>
+      <c r="D1" s="173"/>
+      <c r="E1" s="172" t="s">
         <v>121</v>
       </c>
-      <c r="F1" s="171"/>
-      <c r="G1" s="171"/>
+      <c r="F1" s="172"/>
+      <c r="G1" s="172"/>
       <c r="H1" s="56" t="s">
         <v>122</v>
       </c>
@@ -2693,27 +2700,27 @@
       <c r="K1" s="56" t="s">
         <v>125</v>
       </c>
-      <c r="L1" s="171" t="s">
+      <c r="L1" s="172" t="s">
         <v>126</v>
       </c>
-      <c r="M1" s="171"/>
-      <c r="N1" s="171"/>
-      <c r="O1" s="171"/>
-      <c r="P1" s="171"/>
-      <c r="Q1" s="171"/>
-      <c r="R1" s="169" t="s">
+      <c r="M1" s="172"/>
+      <c r="N1" s="172"/>
+      <c r="O1" s="172"/>
+      <c r="P1" s="172"/>
+      <c r="Q1" s="172"/>
+      <c r="R1" s="170" t="s">
         <v>127</v>
       </c>
-      <c r="S1" s="169" t="s">
+      <c r="S1" s="170" t="s">
         <v>128</v>
       </c>
-      <c r="T1" s="165" t="s">
+      <c r="T1" s="166" t="s">
         <v>129</v>
       </c>
-      <c r="U1" s="166"/>
+      <c r="U1" s="167"/>
     </row>
     <row r="2" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="170"/>
+      <c r="A2" s="171"/>
       <c r="B2" s="109" t="s">
         <v>130</v>
       </c>
@@ -2762,10 +2769,10 @@
       <c r="Q2" s="109" t="s">
         <v>145</v>
       </c>
-      <c r="R2" s="170"/>
-      <c r="S2" s="170"/>
-      <c r="T2" s="167"/>
-      <c r="U2" s="168"/>
+      <c r="R2" s="171"/>
+      <c r="S2" s="171"/>
+      <c r="T2" s="168"/>
+      <c r="U2" s="169"/>
     </row>
     <row r="3" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="84">
@@ -3264,12 +3271,92 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73C30089-60C5-452F-9A94-BDE05D9F4ADC}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>168</v>
+      </c>
+      <c r="B2" t="s">
+        <v>260</v>
+      </c>
+      <c r="C2" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B3" t="s">
+        <v>260</v>
+      </c>
+      <c r="C3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>178</v>
+      </c>
+      <c r="B4" t="s">
+        <v>260</v>
+      </c>
+      <c r="C4" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>183</v>
+      </c>
+      <c r="B5" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>286</v>
+      </c>
+      <c r="B6" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>185</v>
+      </c>
+      <c r="B7" t="s">
+        <v>257</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D86F05D0-180B-43C4-AE12-37977CC3422F}">
   <dimension ref="A1:AC19"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q33" sqref="Q33"/>
+      <selection pane="bottomLeft" activeCell="AI25" sqref="AI25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3285,19 +3372,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="169" t="s">
+      <c r="A1" s="170" t="s">
         <v>119</v>
       </c>
-      <c r="C1" s="173" t="s">
+      <c r="C1" s="174" t="s">
         <v>120</v>
       </c>
-      <c r="D1" s="171"/>
-      <c r="E1" s="172"/>
-      <c r="G1" s="173" t="s">
+      <c r="D1" s="172"/>
+      <c r="E1" s="173"/>
+      <c r="G1" s="174" t="s">
         <v>121</v>
       </c>
-      <c r="H1" s="171"/>
-      <c r="I1" s="172"/>
+      <c r="H1" s="172"/>
+      <c r="I1" s="173"/>
       <c r="K1" s="56" t="s">
         <v>122</v>
       </c>
@@ -3310,27 +3397,27 @@
       <c r="Q1" s="56" t="s">
         <v>125</v>
       </c>
-      <c r="S1" s="173" t="s">
+      <c r="S1" s="174" t="s">
         <v>126</v>
       </c>
-      <c r="T1" s="171"/>
-      <c r="U1" s="171"/>
-      <c r="V1" s="171"/>
-      <c r="W1" s="171"/>
-      <c r="X1" s="172"/>
-      <c r="Z1" s="169" t="s">
+      <c r="T1" s="172"/>
+      <c r="U1" s="172"/>
+      <c r="V1" s="172"/>
+      <c r="W1" s="172"/>
+      <c r="X1" s="173"/>
+      <c r="Z1" s="170" t="s">
         <v>127</v>
       </c>
-      <c r="AA1" s="169" t="s">
+      <c r="AA1" s="170" t="s">
         <v>128</v>
       </c>
-      <c r="AB1" s="165" t="s">
+      <c r="AB1" s="166" t="s">
         <v>129</v>
       </c>
-      <c r="AC1" s="166"/>
+      <c r="AC1" s="167"/>
     </row>
     <row r="2" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="170"/>
+      <c r="A2" s="171"/>
       <c r="C2" s="93" t="s">
         <v>130</v>
       </c>
@@ -3379,10 +3466,10 @@
       <c r="X2" s="94" t="s">
         <v>145</v>
       </c>
-      <c r="Z2" s="170"/>
-      <c r="AA2" s="170"/>
-      <c r="AB2" s="167"/>
-      <c r="AC2" s="168"/>
+      <c r="Z2" s="171"/>
+      <c r="AA2" s="171"/>
+      <c r="AB2" s="168"/>
+      <c r="AC2" s="169"/>
     </row>
     <row r="3" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="84">
@@ -3880,12 +3967,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FF7264C-E7A0-49C5-B2A0-72B8B547DC0E}">
   <dimension ref="A2:O93"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="I32" sqref="I32:I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3911,19 +3998,19 @@
         <v>165</v>
       </c>
       <c r="B2" s="1"/>
-      <c r="C2" s="179" t="s">
+      <c r="C2" s="178" t="s">
         <v>166</v>
       </c>
       <c r="D2" s="175" t="s">
         <v>167</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="155" t="s">
         <v>168</v>
       </c>
-      <c r="G2" s="178" t="s">
+      <c r="G2" s="179" t="s">
         <v>169</v>
       </c>
-      <c r="H2" s="178" t="s">
+      <c r="H2" s="179" t="s">
         <v>170</v>
       </c>
       <c r="I2" s="150" t="s">
@@ -3942,13 +4029,13 @@
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
-      <c r="C3" s="179"/>
-      <c r="D3" s="177"/>
-      <c r="E3" s="2" t="s">
+      <c r="C3" s="178"/>
+      <c r="D3" s="176"/>
+      <c r="E3" s="155" t="s">
         <v>175</v>
       </c>
-      <c r="G3" s="178"/>
-      <c r="H3" s="178"/>
+      <c r="G3" s="179"/>
+      <c r="H3" s="179"/>
       <c r="I3" s="150" t="s">
         <v>176</v>
       </c>
@@ -3958,13 +4045,13 @@
         <v>177</v>
       </c>
       <c r="B4" s="1"/>
-      <c r="C4" s="179"/>
-      <c r="D4" s="177"/>
-      <c r="E4" s="2" t="s">
+      <c r="C4" s="178"/>
+      <c r="D4" s="176"/>
+      <c r="E4" s="155" t="s">
         <v>178</v>
       </c>
-      <c r="G4" s="178"/>
-      <c r="H4" s="178"/>
+      <c r="G4" s="179"/>
+      <c r="H4" s="179"/>
       <c r="I4" s="150" t="s">
         <v>179</v>
       </c>
@@ -3973,12 +4060,12 @@
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
-      <c r="C5" s="179"/>
-      <c r="D5" s="177"/>
-      <c r="E5" s="2" t="s">
+      <c r="C5" s="178"/>
+      <c r="D5" s="176"/>
+      <c r="E5" s="155" t="s">
         <v>180</v>
       </c>
-      <c r="G5" s="178"/>
+      <c r="G5" s="179"/>
       <c r="H5" s="180" t="s">
         <v>181</v>
       </c>
@@ -3990,12 +4077,12 @@
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
-      <c r="C6" s="179"/>
-      <c r="D6" s="177"/>
-      <c r="E6" s="2" t="s">
+      <c r="C6" s="178"/>
+      <c r="D6" s="176"/>
+      <c r="E6" s="155" t="s">
         <v>182</v>
       </c>
-      <c r="G6" s="178"/>
+      <c r="G6" s="179"/>
       <c r="H6" s="180"/>
       <c r="I6" s="154" t="s">
         <v>9</v>
@@ -4005,12 +4092,12 @@
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
-      <c r="C7" s="179"/>
-      <c r="D7" s="177"/>
-      <c r="E7" s="2" t="s">
+      <c r="C7" s="178"/>
+      <c r="D7" s="176"/>
+      <c r="E7" s="155" t="s">
         <v>183</v>
       </c>
-      <c r="G7" s="178"/>
+      <c r="G7" s="179"/>
       <c r="H7" s="180"/>
       <c r="I7" s="154" t="s">
         <v>11</v>
@@ -4020,12 +4107,12 @@
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
-      <c r="C8" s="179"/>
-      <c r="D8" s="177"/>
-      <c r="E8" s="2" t="s">
+      <c r="C8" s="178"/>
+      <c r="D8" s="176"/>
+      <c r="E8" s="155" t="s">
         <v>184</v>
       </c>
-      <c r="G8" s="178"/>
+      <c r="G8" s="179"/>
       <c r="H8" s="180"/>
       <c r="I8" s="154" t="s">
         <v>13</v>
@@ -4035,12 +4122,12 @@
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
-      <c r="C9" s="179"/>
-      <c r="D9" s="177"/>
-      <c r="E9" s="2" t="s">
+      <c r="C9" s="178"/>
+      <c r="D9" s="176"/>
+      <c r="E9" s="155" t="s">
         <v>185</v>
       </c>
-      <c r="G9" s="178"/>
+      <c r="G9" s="179"/>
       <c r="H9" s="180"/>
       <c r="I9" s="154" t="s">
         <v>14</v>
@@ -4050,12 +4137,12 @@
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
-      <c r="C10" s="179"/>
-      <c r="D10" s="177"/>
-      <c r="E10" s="2" t="s">
+      <c r="C10" s="178"/>
+      <c r="D10" s="176"/>
+      <c r="E10" s="155" t="s">
         <v>186</v>
       </c>
-      <c r="G10" s="178"/>
+      <c r="G10" s="179"/>
       <c r="H10" s="180"/>
       <c r="I10" s="154" t="s">
         <v>15</v>
@@ -4065,12 +4152,12 @@
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
-      <c r="C11" s="179"/>
-      <c r="D11" s="177"/>
-      <c r="E11" s="2" t="s">
+      <c r="C11" s="178"/>
+      <c r="D11" s="176"/>
+      <c r="E11" s="155" t="s">
         <v>187</v>
       </c>
-      <c r="G11" s="178"/>
+      <c r="G11" s="179"/>
       <c r="H11" s="180"/>
       <c r="I11" s="154" t="s">
         <v>16</v>
@@ -4080,12 +4167,12 @@
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
-      <c r="C12" s="179"/>
-      <c r="D12" s="177"/>
-      <c r="E12" s="2" t="s">
+      <c r="C12" s="178"/>
+      <c r="D12" s="176"/>
+      <c r="E12" s="155" t="s">
         <v>188</v>
       </c>
-      <c r="G12" s="178"/>
+      <c r="G12" s="179"/>
       <c r="H12" s="180"/>
       <c r="I12" s="154" t="s">
         <v>17</v>
@@ -4095,12 +4182,12 @@
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
-      <c r="C13" s="179"/>
-      <c r="D13" s="177"/>
-      <c r="E13" s="2" t="s">
+      <c r="C13" s="178"/>
+      <c r="D13" s="176"/>
+      <c r="E13" s="155" t="s">
         <v>189</v>
       </c>
-      <c r="G13" s="178"/>
+      <c r="G13" s="179"/>
       <c r="H13" s="180"/>
       <c r="I13" s="154" t="s">
         <v>18</v>
@@ -4110,12 +4197,12 @@
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
-      <c r="C14" s="179"/>
-      <c r="D14" s="177"/>
-      <c r="E14" s="2" t="s">
+      <c r="C14" s="178"/>
+      <c r="D14" s="176"/>
+      <c r="E14" s="155" t="s">
         <v>190</v>
       </c>
-      <c r="G14" s="178"/>
+      <c r="G14" s="179"/>
       <c r="H14" s="180"/>
       <c r="I14" s="154" t="s">
         <v>19</v>
@@ -4125,12 +4212,12 @@
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
-      <c r="C15" s="179"/>
-      <c r="D15" s="176"/>
-      <c r="E15" s="2" t="s">
+      <c r="C15" s="178"/>
+      <c r="D15" s="177"/>
+      <c r="E15" s="155" t="s">
         <v>191</v>
       </c>
-      <c r="G15" s="178"/>
+      <c r="G15" s="179"/>
       <c r="H15" s="180"/>
       <c r="I15" s="154" t="s">
         <v>20</v>
@@ -4140,14 +4227,14 @@
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
-      <c r="C16" s="179"/>
+      <c r="C16" s="178"/>
       <c r="D16" s="175" t="s">
         <v>192</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="G16" s="178"/>
+      <c r="G16" s="179"/>
       <c r="H16" s="180"/>
       <c r="I16" s="154" t="s">
         <v>22</v>
@@ -4157,12 +4244,12 @@
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
-      <c r="C17" s="179"/>
-      <c r="D17" s="177"/>
+      <c r="C17" s="178"/>
+      <c r="D17" s="176"/>
       <c r="E17" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="G17" s="178"/>
+      <c r="G17" s="179"/>
       <c r="H17" s="180"/>
       <c r="I17" s="154" t="s">
         <v>23</v>
@@ -4172,13 +4259,13 @@
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
-      <c r="C18" s="179"/>
-      <c r="D18" s="176"/>
+      <c r="C18" s="178"/>
+      <c r="D18" s="177"/>
       <c r="E18" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="G18" s="178"/>
-      <c r="H18" s="178" t="s">
+      <c r="G18" s="179"/>
+      <c r="H18" s="179" t="s">
         <v>196</v>
       </c>
       <c r="I18" s="150" t="s">
@@ -4188,15 +4275,15 @@
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
-      <c r="C19" s="179"/>
+      <c r="C19" s="178"/>
       <c r="D19" s="175" t="s">
         <v>198</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="G19" s="178"/>
-      <c r="H19" s="178"/>
+      <c r="G19" s="179"/>
+      <c r="H19" s="179"/>
       <c r="I19" s="150" t="s">
         <v>200</v>
       </c>
@@ -4204,13 +4291,13 @@
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
-      <c r="C20" s="179"/>
-      <c r="D20" s="176"/>
+      <c r="C20" s="178"/>
+      <c r="D20" s="177"/>
       <c r="E20" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="G20" s="178"/>
-      <c r="H20" s="178"/>
+      <c r="G20" s="179"/>
+      <c r="H20" s="179"/>
       <c r="I20" s="150" t="s">
         <v>202</v>
       </c>
@@ -4218,15 +4305,15 @@
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
-      <c r="C21" s="179"/>
+      <c r="C21" s="178"/>
       <c r="D21" s="175" t="s">
         <v>203</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="G21" s="178"/>
-      <c r="H21" s="178" t="s">
+      <c r="G21" s="179"/>
+      <c r="H21" s="179" t="s">
         <v>205</v>
       </c>
       <c r="I21" s="150" t="s">
@@ -4236,13 +4323,13 @@
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
-      <c r="C22" s="179"/>
-      <c r="D22" s="176"/>
+      <c r="C22" s="178"/>
+      <c r="D22" s="177"/>
       <c r="E22" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="G22" s="178"/>
-      <c r="H22" s="178"/>
+      <c r="G22" s="179"/>
+      <c r="H22" s="179"/>
       <c r="I22" s="150" t="s">
         <v>208</v>
       </c>
@@ -4250,15 +4337,15 @@
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
-      <c r="C23" s="179"/>
+      <c r="C23" s="178"/>
       <c r="D23" s="175" t="s">
         <v>209</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="G23" s="178"/>
-      <c r="H23" s="178"/>
+      <c r="G23" s="179"/>
+      <c r="H23" s="179"/>
       <c r="I23" s="150" t="s">
         <v>211</v>
       </c>
@@ -4266,12 +4353,12 @@
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
-      <c r="C24" s="179"/>
-      <c r="D24" s="177"/>
+      <c r="C24" s="178"/>
+      <c r="D24" s="176"/>
       <c r="E24" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="G24" s="178"/>
+      <c r="G24" s="179"/>
       <c r="H24" s="149" t="s">
         <v>213</v>
       </c>
@@ -4279,12 +4366,12 @@
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
-      <c r="C25" s="179"/>
-      <c r="D25" s="176"/>
+      <c r="C25" s="178"/>
+      <c r="D25" s="177"/>
       <c r="E25" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="G25" s="178"/>
+      <c r="G25" s="179"/>
       <c r="H25" s="149" t="s">
         <v>215</v>
       </c>
@@ -4292,15 +4379,15 @@
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
-      <c r="C26" s="179"/>
+      <c r="C26" s="178"/>
       <c r="D26" s="175" t="s">
         <v>216</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="G26" s="178"/>
-      <c r="H26" s="178" t="s">
+      <c r="G26" s="179"/>
+      <c r="H26" s="179" t="s">
         <v>218</v>
       </c>
       <c r="I26" s="150" t="s">
@@ -4313,14 +4400,14 @@
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
-      <c r="C27" s="179"/>
-      <c r="D27" s="177"/>
+      <c r="C27" s="178"/>
+      <c r="D27" s="176"/>
       <c r="E27" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="G27" s="178"/>
-      <c r="H27" s="178"/>
-      <c r="I27" s="174" t="s">
+      <c r="G27" s="179"/>
+      <c r="H27" s="179"/>
+      <c r="I27" s="181" t="s">
         <v>91</v>
       </c>
       <c r="J27" s="150" t="s">
@@ -4330,14 +4417,14 @@
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
-      <c r="C28" s="179"/>
-      <c r="D28" s="176"/>
+      <c r="C28" s="178"/>
+      <c r="D28" s="177"/>
       <c r="E28" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="G28" s="178"/>
-      <c r="H28" s="178"/>
-      <c r="I28" s="174"/>
+      <c r="G28" s="179"/>
+      <c r="H28" s="179"/>
+      <c r="I28" s="181"/>
       <c r="J28" s="150" t="s">
         <v>224</v>
       </c>
@@ -4345,530 +4432,521 @@
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
-      <c r="C29" s="179"/>
-      <c r="D29" s="163" t="s">
+      <c r="C29" s="178"/>
+      <c r="D29" s="164" t="s">
         <v>225</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="G29" s="178"/>
-      <c r="H29" s="178"/>
-      <c r="I29" s="174" t="s">
+      <c r="G29" s="179"/>
+      <c r="H29" s="179"/>
+      <c r="I29" s="181" t="s">
+        <v>94</v>
+      </c>
+      <c r="J29" s="150" t="s">
         <v>227</v>
-      </c>
-      <c r="J29" s="150" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
-      <c r="C30" s="179"/>
-      <c r="D30" s="163"/>
+      <c r="C30" s="178"/>
+      <c r="D30" s="164"/>
       <c r="E30" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="G30" s="179"/>
+      <c r="H30" s="179"/>
+      <c r="I30" s="181"/>
+      <c r="J30" s="150" t="s">
         <v>229</v>
       </c>
-      <c r="G30" s="178"/>
-      <c r="H30" s="178"/>
-      <c r="I30" s="174"/>
-      <c r="J30" s="150" t="s">
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C31" s="178"/>
+      <c r="D31" s="164"/>
+      <c r="E31" s="2" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C31" s="179"/>
-      <c r="D31" s="163"/>
-      <c r="E31" s="2" t="s">
+      <c r="G31" s="179"/>
+      <c r="H31" s="179"/>
+      <c r="I31" s="181"/>
+      <c r="J31" s="150" t="s">
         <v>231</v>
       </c>
-      <c r="G31" s="178"/>
-      <c r="H31" s="178"/>
-      <c r="I31" s="174"/>
-      <c r="J31" s="150" t="s">
-        <v>232</v>
-      </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G32" s="178"/>
-      <c r="H32" s="178"/>
-      <c r="I32" s="174" t="s">
+      <c r="G32" s="179"/>
+      <c r="H32" s="179"/>
+      <c r="I32" s="181" t="s">
         <v>95</v>
       </c>
       <c r="J32" s="150" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="33" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="G33" s="178"/>
-      <c r="H33" s="178"/>
-      <c r="I33" s="174"/>
+      <c r="G33" s="179"/>
+      <c r="H33" s="179"/>
+      <c r="I33" s="181"/>
       <c r="J33" s="150" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="34" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="G34" s="178"/>
-      <c r="H34" s="178"/>
-      <c r="I34" s="174"/>
+      <c r="G34" s="179"/>
+      <c r="H34" s="179"/>
+      <c r="I34" s="181"/>
       <c r="J34" s="150" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="35" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="G35" s="178"/>
-      <c r="H35" s="178"/>
-      <c r="I35" s="174" t="s">
+      <c r="G35" s="179"/>
+      <c r="H35" s="179"/>
+      <c r="I35" s="181" t="s">
         <v>97</v>
       </c>
       <c r="J35" s="150" t="s">
         <v>98</v>
       </c>
       <c r="K35" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="L35" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="L35" s="2" t="s">
-        <v>234</v>
-      </c>
     </row>
     <row r="36" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="G36" s="178"/>
-      <c r="H36" s="178"/>
-      <c r="I36" s="174"/>
+      <c r="G36" s="179"/>
+      <c r="H36" s="179"/>
+      <c r="I36" s="181"/>
       <c r="J36" s="150" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="37" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="G37" s="178"/>
-      <c r="H37" s="178"/>
-      <c r="I37" s="174"/>
+      <c r="G37" s="179"/>
+      <c r="H37" s="179"/>
+      <c r="I37" s="181"/>
       <c r="J37" s="150" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="38" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="G38" s="178"/>
-      <c r="H38" s="178"/>
-      <c r="I38" s="174"/>
+      <c r="G38" s="179"/>
+      <c r="H38" s="179"/>
+      <c r="I38" s="181"/>
       <c r="J38" s="150" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="39" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="G39" s="178"/>
-      <c r="H39" s="178"/>
-      <c r="I39" s="174"/>
+      <c r="G39" s="179"/>
+      <c r="H39" s="179"/>
+      <c r="I39" s="181"/>
       <c r="J39" s="150" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="40" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="G40" s="178"/>
-      <c r="H40" s="178"/>
-      <c r="I40" s="174"/>
+      <c r="G40" s="179"/>
+      <c r="H40" s="179"/>
+      <c r="I40" s="181"/>
       <c r="J40" s="150" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="41" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G41" s="179"/>
+      <c r="H41" s="179"/>
+      <c r="I41" s="181"/>
+      <c r="J41" s="150" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="41" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="G41" s="178"/>
-      <c r="H41" s="178"/>
-      <c r="I41" s="174"/>
-      <c r="J41" s="150" t="s">
+    <row r="42" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G42" s="179"/>
+      <c r="H42" s="179"/>
+      <c r="I42" s="181"/>
+      <c r="J42" s="181" t="s">
         <v>237</v>
-      </c>
-    </row>
-    <row r="42" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="G42" s="178"/>
-      <c r="H42" s="178"/>
-      <c r="I42" s="174"/>
-      <c r="J42" s="174" t="s">
-        <v>238</v>
       </c>
       <c r="K42" s="151" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="43" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="G43" s="178"/>
-      <c r="H43" s="178"/>
-      <c r="I43" s="174"/>
-      <c r="J43" s="174"/>
+      <c r="G43" s="179"/>
+      <c r="H43" s="179"/>
+      <c r="I43" s="181"/>
+      <c r="J43" s="181"/>
       <c r="K43" s="151" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="44" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="G44" s="178"/>
-      <c r="H44" s="178"/>
-      <c r="I44" s="174"/>
-      <c r="J44" s="174"/>
+      <c r="G44" s="179"/>
+      <c r="H44" s="179"/>
+      <c r="I44" s="181"/>
+      <c r="J44" s="181"/>
       <c r="K44" s="151" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="45" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="G45" s="178"/>
-      <c r="H45" s="178"/>
-      <c r="I45" s="174"/>
-      <c r="J45" s="174"/>
+      <c r="G45" s="179"/>
+      <c r="H45" s="179"/>
+      <c r="I45" s="181"/>
+      <c r="J45" s="181"/>
       <c r="K45" s="151" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="46" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="G46" s="178"/>
-      <c r="H46" s="178"/>
-      <c r="I46" s="174"/>
+      <c r="G46" s="179"/>
+      <c r="H46" s="179"/>
+      <c r="I46" s="181"/>
       <c r="J46" s="150" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="47" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G47" s="179"/>
+      <c r="H47" s="179"/>
+      <c r="I47" s="150" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="47" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="G47" s="178"/>
-      <c r="H47" s="178"/>
-      <c r="I47" s="150" t="s">
+    <row r="48" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G48" s="179"/>
+      <c r="H48" s="179"/>
+      <c r="I48" s="150" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="48" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="G48" s="178"/>
-      <c r="H48" s="178"/>
-      <c r="I48" s="150" t="s">
+    <row r="49" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G49" s="179"/>
+      <c r="H49" s="179" t="s">
+        <v>24</v>
+      </c>
+      <c r="I49" s="154" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="49" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G49" s="178"/>
-      <c r="H49" s="178" t="s">
-        <v>24</v>
-      </c>
-      <c r="I49" s="154" t="s">
+    <row r="50" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G50" s="179"/>
+      <c r="H50" s="179"/>
+      <c r="I50" s="154" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="50" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G50" s="178"/>
-      <c r="H50" s="178"/>
-      <c r="I50" s="154" t="s">
+    <row r="51" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G51" s="179"/>
+      <c r="H51" s="179"/>
+      <c r="I51" s="154" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="51" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G51" s="178"/>
-      <c r="H51" s="178"/>
-      <c r="I51" s="154" t="s">
+    <row r="52" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G52" s="179"/>
+      <c r="H52" s="179"/>
+      <c r="I52" s="154" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="52" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G52" s="178"/>
-      <c r="H52" s="178"/>
-      <c r="I52" s="154" t="s">
+    <row r="53" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G53" s="179"/>
+      <c r="H53" s="179"/>
+      <c r="I53" s="154" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="53" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G53" s="178"/>
-      <c r="H53" s="178"/>
-      <c r="I53" s="154" t="s">
+    <row r="54" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G54" s="179"/>
+      <c r="H54" s="179"/>
+      <c r="I54" s="154" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="54" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G54" s="178"/>
-      <c r="H54" s="178"/>
-      <c r="I54" s="154" t="s">
+    <row r="55" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G55" s="179"/>
+      <c r="H55" s="179"/>
+      <c r="I55" s="154" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="55" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G55" s="178"/>
-      <c r="H55" s="178"/>
-      <c r="I55" s="154" t="s">
+    <row r="56" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G56" s="179"/>
+      <c r="H56" s="179"/>
+      <c r="I56" s="150" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="56" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G56" s="178"/>
-      <c r="H56" s="178"/>
-      <c r="I56" s="150" t="s">
+    <row r="57" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G57" s="179"/>
+      <c r="H57" s="179"/>
+      <c r="I57" s="150" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="57" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G57" s="178"/>
-      <c r="H57" s="178"/>
-      <c r="I57" s="150" t="s">
+    <row r="58" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G58" s="179"/>
+      <c r="H58" s="179"/>
+      <c r="I58" s="150" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="58" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G58" s="178"/>
-      <c r="H58" s="178"/>
-      <c r="I58" s="150" t="s">
+    <row r="59" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G59" s="179"/>
+      <c r="H59" s="179"/>
+      <c r="I59" s="152" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="59" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G59" s="178"/>
-      <c r="H59" s="178"/>
-      <c r="I59" s="152" t="s">
+    <row r="60" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G60" s="179"/>
+      <c r="H60" s="179" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="60" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G60" s="178"/>
-      <c r="H60" s="178" t="s">
+      <c r="I60" s="153" t="s">
         <v>253</v>
       </c>
-      <c r="I60" s="153" t="s">
+    </row>
+    <row r="61" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G61" s="179"/>
+      <c r="H61" s="179"/>
+      <c r="I61" s="153" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="61" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G61" s="178"/>
-      <c r="H61" s="178"/>
-      <c r="I61" s="153" t="s">
+    <row r="62" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G62" s="179"/>
+      <c r="H62" s="179"/>
+      <c r="I62" s="153" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="62" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G62" s="178"/>
-      <c r="H62" s="178"/>
-      <c r="I62" s="153" t="s">
+    <row r="63" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G63" s="179"/>
+      <c r="H63" s="179"/>
+      <c r="I63" s="153" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="63" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G63" s="178"/>
-      <c r="H63" s="178"/>
-      <c r="I63" s="153" t="s">
+    <row r="64" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G64" s="179"/>
+      <c r="H64" s="179"/>
+      <c r="I64" s="153" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="64" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G64" s="178"/>
-      <c r="H64" s="178"/>
-      <c r="I64" s="153" t="s">
+    <row r="65" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G65" s="179"/>
+      <c r="H65" s="179"/>
+      <c r="I65" s="153" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="65" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G65" s="178"/>
-      <c r="H65" s="178"/>
-      <c r="I65" s="153" t="s">
+    <row r="66" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G66" s="179"/>
+      <c r="H66" s="179"/>
+      <c r="I66" s="153" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="66" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G66" s="178"/>
-      <c r="H66" s="178"/>
-      <c r="I66" s="153" t="s">
+    <row r="67" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G67" s="179"/>
+      <c r="H67" s="179"/>
+      <c r="I67" s="153" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="67" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G67" s="178"/>
-      <c r="H67" s="178"/>
-      <c r="I67" s="153" t="s">
+    <row r="68" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G68" s="179"/>
+      <c r="H68" s="179"/>
+      <c r="I68" s="153" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="68" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G68" s="178"/>
-      <c r="H68" s="178"/>
-      <c r="I68" s="153" t="s">
+    <row r="69" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G69" s="179"/>
+      <c r="H69" s="179"/>
+      <c r="I69" s="153" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="69" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G69" s="178"/>
-      <c r="H69" s="178"/>
-      <c r="I69" s="153" t="s">
+    <row r="70" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G70" s="179"/>
+      <c r="H70" s="179"/>
+      <c r="I70" s="153" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="70" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G70" s="178"/>
-      <c r="H70" s="178"/>
-      <c r="I70" s="153" t="s">
+    <row r="71" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G71" s="179"/>
+      <c r="H71" s="179"/>
+      <c r="I71" s="153" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="71" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G71" s="178"/>
-      <c r="H71" s="178"/>
-      <c r="I71" s="153" t="s">
+    <row r="72" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G72" s="179"/>
+      <c r="H72" s="179"/>
+      <c r="I72" s="153" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="72" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G72" s="178"/>
-      <c r="H72" s="178"/>
-      <c r="I72" s="153" t="s">
+    <row r="73" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G73" s="179"/>
+      <c r="H73" s="179"/>
+      <c r="I73" s="153" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="73" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G73" s="178"/>
-      <c r="H73" s="178"/>
-      <c r="I73" s="153" t="s">
+    <row r="74" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G74" s="179"/>
+      <c r="H74" s="179"/>
+      <c r="I74" s="153" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="74" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G74" s="178"/>
-      <c r="H74" s="178"/>
-      <c r="I74" s="153" t="s">
+    <row r="75" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G75" s="179"/>
+      <c r="H75" s="179"/>
+      <c r="I75" s="153" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="75" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G75" s="178"/>
-      <c r="H75" s="178"/>
-      <c r="I75" s="153" t="s">
+    <row r="76" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G76" s="179"/>
+      <c r="H76" s="179"/>
+      <c r="I76" s="153" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="76" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G76" s="178"/>
-      <c r="H76" s="178"/>
-      <c r="I76" s="153" t="s">
+    <row r="77" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G77" s="179"/>
+      <c r="H77" s="179"/>
+      <c r="I77" s="153" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="77" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G77" s="178"/>
-      <c r="H77" s="178"/>
-      <c r="I77" s="153" t="s">
+    <row r="78" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G78" s="179"/>
+      <c r="H78" s="179"/>
+      <c r="I78" s="153" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="78" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G78" s="178"/>
-      <c r="H78" s="178"/>
-      <c r="I78" s="153" t="s">
+    <row r="79" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G79" s="179"/>
+      <c r="H79" s="179"/>
+      <c r="I79" s="153" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="79" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G79" s="178"/>
-      <c r="H79" s="178"/>
-      <c r="I79" s="153" t="s">
+    <row r="80" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G80" s="179"/>
+      <c r="H80" s="179"/>
+      <c r="I80" s="153" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="80" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G80" s="178"/>
-      <c r="H80" s="178"/>
-      <c r="I80" s="153" t="s">
+    <row r="81" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G81" s="179"/>
+      <c r="H81" s="179"/>
+      <c r="I81" s="153" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="81" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G81" s="178"/>
-      <c r="H81" s="178"/>
-      <c r="I81" s="153" t="s">
+    <row r="82" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G82" s="179"/>
+      <c r="H82" s="179"/>
+      <c r="I82" s="153" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="82" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G82" s="178"/>
-      <c r="H82" s="178"/>
-      <c r="I82" s="153" t="s">
+    <row r="83" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G83" s="179"/>
+      <c r="H83" s="179"/>
+      <c r="I83" s="153" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="83" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G83" s="178"/>
-      <c r="H83" s="178"/>
-      <c r="I83" s="153" t="s">
+    <row r="84" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G84" s="179"/>
+      <c r="H84" s="179"/>
+      <c r="I84" s="153" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="84" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G84" s="178"/>
-      <c r="H84" s="178"/>
-      <c r="I84" s="153" t="s">
+    <row r="85" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G85" s="179"/>
+      <c r="H85" s="179"/>
+      <c r="I85" s="153" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="85" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G85" s="178"/>
-      <c r="H85" s="178"/>
-      <c r="I85" s="153" t="s">
+    <row r="86" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G86" s="179"/>
+      <c r="H86" s="179"/>
+      <c r="I86" s="153" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="86" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G86" s="178"/>
-      <c r="H86" s="178"/>
-      <c r="I86" s="153" t="s">
-        <v>280</v>
-      </c>
-    </row>
     <row r="87" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G87" s="178"/>
-      <c r="H87" s="178"/>
+      <c r="G87" s="179"/>
+      <c r="H87" s="179"/>
       <c r="I87" s="153" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="88" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G88" s="178"/>
-      <c r="H88" s="178"/>
+      <c r="G88" s="179"/>
+      <c r="H88" s="179"/>
       <c r="I88" s="153" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="89" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G89" s="179"/>
+      <c r="H89" s="179"/>
+      <c r="I89" s="153" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="89" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G89" s="178"/>
-      <c r="H89" s="178"/>
-      <c r="I89" s="153" t="s">
+    <row r="90" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G90" s="179"/>
+      <c r="H90" s="179"/>
+      <c r="I90" s="153" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="90" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G90" s="178"/>
-      <c r="H90" s="178"/>
-      <c r="I90" s="153" t="s">
+    <row r="91" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G91" s="179"/>
+      <c r="H91" s="179"/>
+      <c r="I91" s="153" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="91" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G91" s="178"/>
-      <c r="H91" s="178"/>
-      <c r="I91" s="153" t="s">
+    <row r="92" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G92" s="179"/>
+      <c r="H92" s="179"/>
+      <c r="I92" s="153" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="92" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G92" s="178"/>
-      <c r="H92" s="178"/>
-      <c r="I92" s="153" t="s">
+    <row r="93" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G93" s="179"/>
+      <c r="H93" s="179"/>
+      <c r="I93" s="153" t="s">
         <v>285</v>
-      </c>
-    </row>
-    <row r="93" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G93" s="178"/>
-      <c r="H93" s="178"/>
-      <c r="I93" s="153" t="s">
-        <v>286</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="D2:D15"/>
-    <mergeCell ref="D16:D18"/>
-    <mergeCell ref="D29:D31"/>
-    <mergeCell ref="C2:C31"/>
-    <mergeCell ref="H2:H4"/>
-    <mergeCell ref="H5:H17"/>
-    <mergeCell ref="G2:G93"/>
-    <mergeCell ref="H60:H93"/>
-    <mergeCell ref="H49:H59"/>
     <mergeCell ref="J42:J45"/>
     <mergeCell ref="I27:I28"/>
     <mergeCell ref="I29:I31"/>
@@ -4881,29 +4959,26 @@
     <mergeCell ref="I32:I34"/>
     <mergeCell ref="I35:I46"/>
     <mergeCell ref="H26:H48"/>
+    <mergeCell ref="D2:D15"/>
+    <mergeCell ref="D16:D18"/>
+    <mergeCell ref="D29:D31"/>
+    <mergeCell ref="C2:C31"/>
+    <mergeCell ref="H2:H4"/>
+    <mergeCell ref="H5:H17"/>
+    <mergeCell ref="G2:G93"/>
+    <mergeCell ref="H60:H93"/>
+    <mergeCell ref="H49:H59"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC7747E6-62D3-4152-BD4D-7F49D1734AF5}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D00BE0B-CDDF-425B-AD29-406227FC3C1E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A497FCDD-7AFC-448F-BBBB-19B8588E5BE4}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M30" sqref="M30"/>
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4913,32 +4988,6 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9774AD9-F210-408D-8DE0-DC5FA13F3AA3}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N22" sqref="N22"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A497FCDD-7AFC-448F-BBBB-19B8588E5BE4}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93ABF146-28AE-46B6-9D9F-239E5A87C7F8}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -4950,7 +4999,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4946E28-29BC-43B7-9786-7F012DB60FDA}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -4970,7 +5019,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G13" sqref="G13"/>
+      <selection pane="bottomLeft" activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5002,10 +5051,10 @@
       <c r="C2" s="31"/>
       <c r="D2" s="35"/>
       <c r="E2" s="22"/>
-      <c r="G2" s="155" t="s">
+      <c r="G2" s="156" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="156"/>
+      <c r="H2" s="157"/>
       <c r="I2" s="22"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -5018,10 +5067,10 @@
       <c r="C3" s="18"/>
       <c r="D3" s="25"/>
       <c r="E3" s="6"/>
-      <c r="G3" s="157" t="s">
+      <c r="G3" s="158" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="158"/>
+      <c r="H3" s="159"/>
       <c r="I3" s="23"/>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5034,10 +5083,10 @@
       <c r="C4" s="18"/>
       <c r="D4" s="25"/>
       <c r="E4" s="6"/>
-      <c r="G4" s="159" t="s">
+      <c r="G4" s="160" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="160"/>
+      <c r="H4" s="161"/>
       <c r="I4" s="24"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -5223,10 +5272,10 @@
       <c r="C2" s="17"/>
       <c r="D2" s="11"/>
       <c r="E2" s="12"/>
-      <c r="G2" s="155" t="s">
+      <c r="G2" s="156" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="156"/>
+      <c r="H2" s="157"/>
       <c r="I2" s="22"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -5239,10 +5288,10 @@
       <c r="C3" s="18"/>
       <c r="D3" s="4"/>
       <c r="E3" s="6"/>
-      <c r="G3" s="157" t="s">
+      <c r="G3" s="158" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="158"/>
+      <c r="H3" s="159"/>
       <c r="I3" s="23"/>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5255,10 +5304,10 @@
       <c r="C4" s="18"/>
       <c r="D4" s="4"/>
       <c r="E4" s="6"/>
-      <c r="G4" s="159" t="s">
+      <c r="G4" s="160" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="160"/>
+      <c r="H4" s="161"/>
       <c r="I4" s="24"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -5323,10 +5372,10 @@
       <c r="C2" s="18"/>
       <c r="D2" s="4"/>
       <c r="E2" s="6"/>
-      <c r="G2" s="155" t="s">
+      <c r="G2" s="156" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="156"/>
+      <c r="H2" s="157"/>
       <c r="I2" s="22"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -5339,10 +5388,10 @@
       <c r="C3" s="18"/>
       <c r="D3" s="4"/>
       <c r="E3" s="6"/>
-      <c r="G3" s="157" t="s">
+      <c r="G3" s="158" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="158"/>
+      <c r="H3" s="159"/>
       <c r="I3" s="23"/>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5355,10 +5404,10 @@
       <c r="C4" s="18"/>
       <c r="D4" s="4"/>
       <c r="E4" s="6"/>
-      <c r="G4" s="159" t="s">
+      <c r="G4" s="160" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="160"/>
+      <c r="H4" s="161"/>
       <c r="I4" s="24"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -5478,10 +5527,10 @@
       <c r="C2" s="17"/>
       <c r="D2" s="11"/>
       <c r="E2" s="12"/>
-      <c r="G2" s="155" t="s">
+      <c r="G2" s="156" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="156"/>
+      <c r="H2" s="157"/>
       <c r="I2" s="22"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -5494,10 +5543,10 @@
       <c r="C3" s="18"/>
       <c r="D3" s="4"/>
       <c r="E3" s="6"/>
-      <c r="G3" s="157" t="s">
+      <c r="G3" s="158" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="158"/>
+      <c r="H3" s="159"/>
       <c r="I3" s="23"/>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5510,10 +5559,10 @@
       <c r="C4" s="18"/>
       <c r="D4" s="4"/>
       <c r="E4" s="6"/>
-      <c r="G4" s="159" t="s">
+      <c r="G4" s="160" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="160"/>
+      <c r="H4" s="161"/>
       <c r="I4" s="24"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -5587,7 +5636,7 @@
       <c r="A2" s="49">
         <v>1</v>
       </c>
-      <c r="B2" s="161" t="s">
+      <c r="B2" s="162" t="s">
         <v>63</v>
       </c>
       <c r="C2" s="50" t="s">
@@ -5596,51 +5645,51 @@
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
       <c r="F2" s="12"/>
-      <c r="H2" s="155" t="s">
+      <c r="H2" s="156" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="156"/>
+      <c r="I2" s="157"/>
       <c r="J2" s="22"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="42">
         <v>2</v>
       </c>
-      <c r="B3" s="162"/>
+      <c r="B3" s="163"/>
       <c r="C3" s="44" t="s">
         <v>65</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="F3" s="6"/>
-      <c r="H3" s="157" t="s">
+      <c r="H3" s="158" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="158"/>
+      <c r="I3" s="159"/>
       <c r="J3" s="23"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="42">
         <v>3</v>
       </c>
-      <c r="B4" s="162"/>
+      <c r="B4" s="163"/>
       <c r="C4" s="44" t="s">
         <v>66</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="6"/>
-      <c r="H4" s="159" t="s">
+      <c r="H4" s="160" t="s">
         <v>12</v>
       </c>
-      <c r="I4" s="160"/>
+      <c r="I4" s="161"/>
       <c r="J4" s="24"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="42">
         <v>4</v>
       </c>
-      <c r="B5" s="162"/>
+      <c r="B5" s="163"/>
       <c r="C5" s="44" t="s">
         <v>67</v>
       </c>
@@ -5652,7 +5701,7 @@
       <c r="A6" s="42">
         <v>5</v>
       </c>
-      <c r="B6" s="162"/>
+      <c r="B6" s="163"/>
       <c r="C6" s="44" t="s">
         <v>68</v>
       </c>
@@ -5664,7 +5713,7 @@
       <c r="A7" s="42">
         <v>6</v>
       </c>
-      <c r="B7" s="162"/>
+      <c r="B7" s="163"/>
       <c r="C7" s="44" t="s">
         <v>69</v>
       </c>
@@ -5676,7 +5725,7 @@
       <c r="A8" s="42">
         <v>7</v>
       </c>
-      <c r="B8" s="162"/>
+      <c r="B8" s="163"/>
       <c r="C8" s="44" t="s">
         <v>70</v>
       </c>
@@ -5772,10 +5821,10 @@
       <c r="C2" s="17"/>
       <c r="D2" s="55"/>
       <c r="E2" s="12"/>
-      <c r="G2" s="155" t="s">
+      <c r="G2" s="156" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="156"/>
+      <c r="H2" s="157"/>
       <c r="I2" s="22"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -5788,10 +5837,10 @@
       <c r="C3" s="18"/>
       <c r="D3" s="25"/>
       <c r="E3" s="6"/>
-      <c r="G3" s="157" t="s">
+      <c r="G3" s="158" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="158"/>
+      <c r="H3" s="159"/>
       <c r="I3" s="23"/>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5804,10 +5853,10 @@
       <c r="C4" s="18"/>
       <c r="D4" s="4"/>
       <c r="E4" s="6"/>
-      <c r="G4" s="159" t="s">
+      <c r="G4" s="160" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="160"/>
+      <c r="H4" s="161"/>
       <c r="I4" s="24"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -5894,10 +5943,10 @@
       <c r="C2" s="31"/>
       <c r="D2" s="35"/>
       <c r="E2" s="22"/>
-      <c r="G2" s="155" t="s">
+      <c r="G2" s="156" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="156"/>
+      <c r="H2" s="157"/>
       <c r="I2" s="22"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -5910,10 +5959,10 @@
       <c r="C3" s="18"/>
       <c r="D3" s="4"/>
       <c r="E3" s="6"/>
-      <c r="G3" s="157" t="s">
+      <c r="G3" s="158" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="158"/>
+      <c r="H3" s="159"/>
       <c r="I3" s="23"/>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5926,10 +5975,10 @@
       <c r="C4" s="18"/>
       <c r="D4" s="25"/>
       <c r="E4" s="6"/>
-      <c r="G4" s="159" t="s">
+      <c r="G4" s="160" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="160"/>
+      <c r="H4" s="161"/>
       <c r="I4" s="24"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -6013,7 +6062,7 @@
   <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6023,7 +6072,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="163" t="s">
+      <c r="A1" s="164" t="s">
         <v>91</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -6032,15 +6081,15 @@
       <c r="C1" s="1"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="163"/>
+      <c r="A2" s="164"/>
       <c r="B2" s="2" t="s">
         <v>93</v>
       </c>
       <c r="C2" s="1"/>
-      <c r="D2" s="155" t="s">
+      <c r="D2" s="156" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="156"/>
+      <c r="E2" s="157"/>
       <c r="F2" s="22"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -6049,10 +6098,10 @@
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="157" t="s">
+      <c r="D3" s="158" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="158"/>
+      <c r="E3" s="159"/>
       <c r="F3" s="23"/>
     </row>
     <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6061,10 +6110,10 @@
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="1"/>
-      <c r="D4" s="159" t="s">
+      <c r="D4" s="160" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="160"/>
+      <c r="E4" s="161"/>
       <c r="F4" s="24"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -6075,113 +6124,113 @@
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="163" t="s">
+      <c r="A6" s="164" t="s">
         <v>97</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>98</v>
       </c>
       <c r="C6" s="1"/>
-      <c r="K6" s="164" t="s">
+      <c r="K6" s="165" t="s">
         <v>99</v>
       </c>
-      <c r="L6" s="164"/>
+      <c r="L6" s="165"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="163"/>
+      <c r="A7" s="164"/>
       <c r="B7" s="2" t="s">
         <v>100</v>
       </c>
       <c r="C7" s="1"/>
-      <c r="K7" s="164"/>
-      <c r="L7" s="164"/>
+      <c r="K7" s="165"/>
+      <c r="L7" s="165"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="163"/>
+      <c r="A8" s="164"/>
       <c r="B8" s="2" t="s">
         <v>101</v>
       </c>
       <c r="C8" s="1"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="163"/>
+      <c r="A9" s="164"/>
       <c r="B9" s="2" t="s">
         <v>102</v>
       </c>
       <c r="C9" s="1"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="163"/>
+      <c r="A10" s="164"/>
       <c r="B10" s="2" t="s">
         <v>103</v>
       </c>
       <c r="C10" s="1"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="163"/>
+      <c r="A11" s="164"/>
       <c r="B11" s="2" t="s">
         <v>104</v>
       </c>
       <c r="C11" s="1"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="163"/>
+      <c r="A12" s="164"/>
       <c r="B12" s="2" t="s">
         <v>105</v>
       </c>
       <c r="C12" s="1"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="163"/>
+      <c r="A13" s="164"/>
       <c r="B13" s="2" t="s">
         <v>106</v>
       </c>
       <c r="C13" s="1"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="163"/>
+      <c r="A14" s="164"/>
       <c r="B14" s="2" t="s">
         <v>107</v>
       </c>
       <c r="C14" s="1"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="163"/>
+      <c r="A15" s="164"/>
       <c r="B15" s="2" t="s">
         <v>108</v>
       </c>
       <c r="C15" s="1"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="163"/>
+      <c r="A16" s="164"/>
       <c r="B16" s="2" t="s">
         <v>109</v>
       </c>
       <c r="C16" s="1"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="163"/>
+      <c r="A17" s="164"/>
       <c r="B17" s="2" t="s">
         <v>110</v>
       </c>
       <c r="C17" s="1"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="163"/>
+      <c r="A18" s="164"/>
       <c r="B18" s="2" t="s">
         <v>111</v>
       </c>
       <c r="C18" s="1"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="163"/>
+      <c r="A19" s="164"/>
       <c r="B19" s="2" t="s">
         <v>112</v>
       </c>
       <c r="C19" s="1"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="163"/>
+      <c r="A20" s="164"/>
       <c r="B20" s="2" t="s">
         <v>113</v>
       </c>
@@ -6195,7 +6244,7 @@
       <c r="C21" s="1"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="163" t="s">
+      <c r="A22" s="164" t="s">
         <v>115</v>
       </c>
       <c r="B22" s="2" t="s">
@@ -6206,7 +6255,7 @@
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="163"/>
+      <c r="A23" s="164"/>
       <c r="B23" s="2" t="s">
         <v>118</v>
       </c>

</xml_diff>